<commit_message>
inicio de enrutamiento rip edificio 1
</commit_message>
<xml_diff>
--- a/taller-2/Taller#2.xlsx
+++ b/taller-2/Taller#2.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan JS\Documents\ucc\Interconexion\taller-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF91EE8-2129-4020-A7A8-90FEC14B99CA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8BDE2F92-B9E1-4CCE-9694-33723D7E9A18}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -144,7 +143,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -519,11 +518,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F469E335-6B4A-4489-9E5A-B9805EBAEB60}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AA127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="V5" sqref="V5"/>
+    <sheetView tabSelected="1" topLeftCell="K74" workbookViewId="0">
+      <selection activeCell="Y86" sqref="Y86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -867,7 +866,7 @@
         <v>172.1.0.1</v>
       </c>
       <c r="K6" s="2">
-        <f t="shared" ref="K6:K35" si="11">K5</f>
+        <f t="shared" ref="K6:K31" si="11">K5</f>
         <v>2</v>
       </c>
       <c r="L6" s="2">
@@ -1152,7 +1151,7 @@
         <v>2</v>
       </c>
       <c r="L9" s="2">
-        <f t="shared" ref="L9:L35" si="19">L5+1</f>
+        <f t="shared" ref="L9:L31" si="19">L5+1</f>
         <v>1</v>
       </c>
       <c r="M9" s="2" t="str">
@@ -1160,7 +1159,7 @@
         <v>PC-29</v>
       </c>
       <c r="N9" s="2">
-        <f t="shared" ref="N9:N35" si="20">N5</f>
+        <f t="shared" ref="N9:N31" si="20">N5</f>
         <v>2</v>
       </c>
       <c r="O9" s="2" t="str">
@@ -2968,7 +2967,7 @@
         <v>6</v>
       </c>
       <c r="M28" s="2" t="str">
-        <f t="shared" ref="M28:M35" si="23">_xlfn.CONCAT("PC-",MID(M27,FIND("-",M27)+ 1, LEN(M27))+1)</f>
+        <f t="shared" ref="M28:M31" si="23">_xlfn.CONCAT("PC-",MID(M27,FIND("-",M27)+ 1, LEN(M27))+1)</f>
         <v>PC-48</v>
       </c>
       <c r="N28" s="2">
@@ -2976,19 +2975,19 @@
         <v>1</v>
       </c>
       <c r="O28" s="2" t="str">
-        <f t="shared" ref="O28:O35" si="24">_xlfn.CONCAT("172.",K28,".",L28,".0/24")</f>
+        <f t="shared" ref="O28:O31" si="24">_xlfn.CONCAT("172.",K28,".",L28,".0/24")</f>
         <v>172.2.6.0/24</v>
       </c>
       <c r="P28" s="2" t="str">
-        <f t="shared" ref="P28:P35" si="25">_xlfn.CONCAT("172.",K28,".",L28,".",N28 + 1)</f>
+        <f t="shared" ref="P28:P31" si="25">_xlfn.CONCAT("172.",K28,".",L28,".",N28 + 1)</f>
         <v>172.2.6.2</v>
       </c>
       <c r="Q28" s="2" t="str">
-        <f t="shared" ref="Q28:Q35" si="26">Q27</f>
+        <f t="shared" ref="Q28:Q31" si="26">Q27</f>
         <v>255.255.255.0</v>
       </c>
       <c r="R28" s="2" t="str">
-        <f t="shared" ref="R28:R35" si="27">_xlfn.CONCAT("172.",K28,".",L28,".1")</f>
+        <f t="shared" ref="R28:R31" si="27">_xlfn.CONCAT("172.",K28,".",L28,".1")</f>
         <v>172.2.6.1</v>
       </c>
       <c r="T28" s="2">

</xml_diff>

<commit_message>
Se acaba hasta el PC-100
</commit_message>
<xml_diff>
--- a/taller-2/Taller#2.xlsx
+++ b/taller-2/Taller#2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivanbotero/Projects/interconexion/taller-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5847CA-4929-9346-863B-C6E0481CBDE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3CE08B3-93FD-B442-86BF-C2E71CC4758A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -176,7 +176,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -186,6 +186,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -202,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -210,10 +216,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -566,36 +575,36 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:27" ht="18" x14ac:dyDescent="0.2">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="K2" s="3" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="K2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="T2" s="3" t="s">
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="T2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="4"/>
+      <c r="AA2" s="4"/>
     </row>
     <row r="3" spans="2:27" ht="16" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
@@ -5305,8 +5314,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B2:AA127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="P40" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="S51" sqref="S51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5338,36 +5347,36 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:27" ht="18" x14ac:dyDescent="0.2">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="K2" s="3" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="K2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="T2" s="3" t="s">
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="T2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="4"/>
+      <c r="AA2" s="4"/>
     </row>
     <row r="3" spans="2:27" ht="16" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
@@ -5444,382 +5453,382 @@
       </c>
     </row>
     <row r="4" spans="2:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="B4" s="4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4">
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3">
         <v>0</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="4" t="str">
+      <c r="D4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3" t="str">
         <f>_xlfn.CONCAT("2001:",B4,":",C4 + 1,"::/112")</f>
         <v>2001:1:1::/112</v>
       </c>
-      <c r="G4" s="4" t="str">
+      <c r="G4" s="3" t="str">
         <f>_xlfn.CONCAT("2001:",B4,":",C4+1,"::",E4 + 1)</f>
         <v>2001:1:1::2</v>
       </c>
-      <c r="H4" s="4">
-        <v>112</v>
-      </c>
-      <c r="I4" s="4" t="str">
+      <c r="H4" s="3">
+        <v>112</v>
+      </c>
+      <c r="I4" s="3" t="str">
         <f>_xlfn.CONCAT("2001:",B4,":",C4+1,"::1")</f>
         <v>2001:1:1::1</v>
       </c>
-      <c r="K4" s="2">
-        <v>2</v>
-      </c>
-      <c r="L4" s="2">
+      <c r="K4" s="5">
+        <v>2</v>
+      </c>
+      <c r="L4" s="5">
         <v>0</v>
       </c>
-      <c r="M4" s="2" t="str">
+      <c r="M4" s="5" t="str">
         <f>_xlfn.CONCAT("PC-",MID(D27,FIND("-",D27)+ 1, LEN(D27))+1)</f>
         <v>PC-24</v>
       </c>
-      <c r="N4" s="2">
-        <v>1</v>
-      </c>
-      <c r="O4" s="2" t="str">
+      <c r="N4" s="5">
+        <v>1</v>
+      </c>
+      <c r="O4" s="5" t="str">
         <f>_xlfn.CONCAT("2001:",K4,":",L4 + 1,"::/112")</f>
         <v>2001:2:1::/112</v>
       </c>
-      <c r="P4" s="2" t="str">
+      <c r="P4" s="5" t="str">
         <f>_xlfn.CONCAT("2001:",K4,":",L4+1,"::",N4 + 1)</f>
         <v>2001:2:1::2</v>
       </c>
-      <c r="Q4" s="2">
-        <v>112</v>
-      </c>
-      <c r="R4" s="2" t="str">
+      <c r="Q4" s="5">
+        <v>112</v>
+      </c>
+      <c r="R4" s="5" t="str">
         <f>_xlfn.CONCAT("2001:",K4,":",L4+1,"::1")</f>
         <v>2001:2:1::1</v>
       </c>
-      <c r="T4" s="2">
-        <v>3</v>
-      </c>
-      <c r="U4" s="2">
+      <c r="T4" s="5">
+        <v>3</v>
+      </c>
+      <c r="U4" s="5">
         <v>0</v>
       </c>
-      <c r="V4" s="2" t="str">
+      <c r="V4" s="5" t="str">
         <f>_xlfn.CONCAT("PC-",MID(M31,FIND("-",M31)+ 1, LEN(M31))+1)</f>
         <v>PC-52</v>
       </c>
-      <c r="W4" s="2">
-        <v>1</v>
-      </c>
-      <c r="X4" s="2" t="str">
+      <c r="W4" s="5">
+        <v>1</v>
+      </c>
+      <c r="X4" s="5" t="str">
         <f>_xlfn.CONCAT("2001:",T4,":",U4 + 1,"::/112")</f>
         <v>2001:3:1::/112</v>
       </c>
-      <c r="Y4" s="2" t="str">
+      <c r="Y4" s="5" t="str">
         <f>_xlfn.CONCAT("2001:",T4,":",U4+1,"::",W4 + 1)</f>
         <v>2001:3:1::2</v>
       </c>
-      <c r="Z4" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA4" s="2" t="str">
+      <c r="Z4" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA4" s="5" t="str">
         <f>_xlfn.CONCAT("2001:",T4,":",U4+1,"::1")</f>
         <v>2001:3:1::1</v>
       </c>
     </row>
     <row r="5" spans="2:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <f>B4</f>
         <v>1</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>0</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="4">
-        <v>2</v>
-      </c>
-      <c r="F5" s="4" t="str">
+      <c r="D5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="3">
+        <v>2</v>
+      </c>
+      <c r="F5" s="3" t="str">
         <f t="shared" ref="F5:F27" si="0">_xlfn.CONCAT("2001:",B5,":",C5 + 1,"::/112")</f>
         <v>2001:1:1::/112</v>
       </c>
-      <c r="G5" s="4" t="str">
+      <c r="G5" s="3" t="str">
         <f t="shared" ref="G5:G27" si="1">_xlfn.CONCAT("2001:",B5,":",C5+1,"::",E5 + 1)</f>
         <v>2001:1:1::3</v>
       </c>
-      <c r="H5" s="4">
-        <v>112</v>
-      </c>
-      <c r="I5" s="4" t="str">
+      <c r="H5" s="3">
+        <v>112</v>
+      </c>
+      <c r="I5" s="3" t="str">
         <f t="shared" ref="I5:I27" si="2">_xlfn.CONCAT("2001:",B5,":",C5+1,"::1")</f>
         <v>2001:1:1::1</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="5">
         <f>K4</f>
         <v>2</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5" s="5">
         <v>0</v>
       </c>
-      <c r="M5" s="2" t="str">
+      <c r="M5" s="5" t="str">
         <f>_xlfn.CONCAT("PC-",MID(M4,FIND("-",M4)+ 1, LEN(M4))+1)</f>
         <v>PC-25</v>
       </c>
-      <c r="N5" s="2">
-        <v>2</v>
-      </c>
-      <c r="O5" s="2" t="str">
+      <c r="N5" s="5">
+        <v>2</v>
+      </c>
+      <c r="O5" s="5" t="str">
         <f t="shared" ref="O5:O31" si="3">_xlfn.CONCAT("2001:",K5,":",L5 + 1,"::/112")</f>
         <v>2001:2:1::/112</v>
       </c>
-      <c r="P5" s="2" t="str">
+      <c r="P5" s="5" t="str">
         <f t="shared" ref="P5:P31" si="4">_xlfn.CONCAT("2001:",K5,":",L5+1,"::",N5 + 1)</f>
         <v>2001:2:1::3</v>
       </c>
-      <c r="Q5" s="2">
-        <v>112</v>
-      </c>
-      <c r="R5" s="2" t="str">
+      <c r="Q5" s="5">
+        <v>112</v>
+      </c>
+      <c r="R5" s="5" t="str">
         <f t="shared" ref="R5:R31" si="5">_xlfn.CONCAT("2001:",K5,":",L5+1,"::1")</f>
         <v>2001:2:1::1</v>
       </c>
-      <c r="T5" s="2">
+      <c r="T5" s="5">
         <f>T4</f>
         <v>3</v>
       </c>
-      <c r="U5" s="2">
+      <c r="U5" s="5">
         <v>0</v>
       </c>
-      <c r="V5" s="2" t="str">
+      <c r="V5" s="5" t="str">
         <f>_xlfn.CONCAT("PC-",MID(V4,FIND("-",V4)+ 1, LEN(V4))+1)</f>
         <v>PC-53</v>
       </c>
-      <c r="W5" s="2">
-        <v>2</v>
-      </c>
-      <c r="X5" s="2" t="str">
+      <c r="W5" s="5">
+        <v>2</v>
+      </c>
+      <c r="X5" s="5" t="str">
         <f t="shared" ref="X5:X68" si="6">_xlfn.CONCAT("2001:",T5,":",U5 + 1,"::/112")</f>
         <v>2001:3:1::/112</v>
       </c>
-      <c r="Y5" s="2" t="str">
+      <c r="Y5" s="5" t="str">
         <f t="shared" ref="Y5:Y68" si="7">_xlfn.CONCAT("2001:",T5,":",U5+1,"::",W5 + 1)</f>
         <v>2001:3:1::3</v>
       </c>
-      <c r="Z5" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA5" s="2" t="str">
+      <c r="Z5" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA5" s="5" t="str">
         <f t="shared" ref="AA5:AA68" si="8">_xlfn.CONCAT("2001:",T5,":",U5+1,"::1")</f>
         <v>2001:3:1::1</v>
       </c>
     </row>
     <row r="6" spans="2:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <f t="shared" ref="B6:B27" si="9">B5</f>
         <v>1</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>0</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="4">
-        <v>3</v>
-      </c>
-      <c r="F6" s="4" t="str">
+      <c r="E6" s="3">
+        <v>3</v>
+      </c>
+      <c r="F6" s="3" t="str">
         <f t="shared" si="0"/>
         <v>2001:1:1::/112</v>
       </c>
-      <c r="G6" s="4" t="str">
+      <c r="G6" s="3" t="str">
         <f t="shared" si="1"/>
         <v>2001:1:1::4</v>
       </c>
-      <c r="H6" s="4">
-        <v>112</v>
-      </c>
-      <c r="I6" s="4" t="str">
+      <c r="H6" s="3">
+        <v>112</v>
+      </c>
+      <c r="I6" s="3" t="str">
         <f t="shared" si="2"/>
         <v>2001:1:1::1</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="5">
         <f t="shared" ref="K6:K31" si="10">K5</f>
         <v>2</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L6" s="5">
         <v>0</v>
       </c>
-      <c r="M6" s="2" t="str">
+      <c r="M6" s="5" t="str">
         <f t="shared" ref="M6:M31" si="11">_xlfn.CONCAT("PC-",MID(M5,FIND("-",M5)+ 1, LEN(M5))+1)</f>
         <v>PC-26</v>
       </c>
-      <c r="N6" s="2">
-        <v>3</v>
-      </c>
-      <c r="O6" s="2" t="str">
+      <c r="N6" s="5">
+        <v>3</v>
+      </c>
+      <c r="O6" s="5" t="str">
         <f t="shared" si="3"/>
         <v>2001:2:1::/112</v>
       </c>
-      <c r="P6" s="2" t="str">
+      <c r="P6" s="5" t="str">
         <f t="shared" si="4"/>
         <v>2001:2:1::4</v>
       </c>
-      <c r="Q6" s="2">
-        <v>112</v>
-      </c>
-      <c r="R6" s="2" t="str">
+      <c r="Q6" s="5">
+        <v>112</v>
+      </c>
+      <c r="R6" s="5" t="str">
         <f t="shared" si="5"/>
         <v>2001:2:1::1</v>
       </c>
-      <c r="T6" s="2">
+      <c r="T6" s="5">
         <f t="shared" ref="T6:T69" si="12">T5</f>
         <v>3</v>
       </c>
-      <c r="U6" s="2">
+      <c r="U6" s="5">
         <v>0</v>
       </c>
-      <c r="V6" s="2" t="str">
+      <c r="V6" s="5" t="str">
         <f t="shared" ref="V6:V69" si="13">_xlfn.CONCAT("PC-",MID(V5,FIND("-",V5)+ 1, LEN(V5))+1)</f>
         <v>PC-54</v>
       </c>
-      <c r="W6" s="2">
-        <v>3</v>
-      </c>
-      <c r="X6" s="2" t="str">
+      <c r="W6" s="5">
+        <v>3</v>
+      </c>
+      <c r="X6" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:1::/112</v>
       </c>
-      <c r="Y6" s="2" t="str">
+      <c r="Y6" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:1::4</v>
       </c>
-      <c r="Z6" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA6" s="2" t="str">
+      <c r="Z6" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA6" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:1::1</v>
       </c>
     </row>
     <row r="7" spans="2:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>0</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>4</v>
       </c>
-      <c r="F7" s="4" t="str">
+      <c r="F7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>2001:1:1::/112</v>
       </c>
-      <c r="G7" s="4" t="str">
+      <c r="G7" s="3" t="str">
         <f t="shared" si="1"/>
         <v>2001:1:1::5</v>
       </c>
-      <c r="H7" s="4">
-        <v>112</v>
-      </c>
-      <c r="I7" s="4" t="str">
+      <c r="H7" s="3">
+        <v>112</v>
+      </c>
+      <c r="I7" s="3" t="str">
         <f t="shared" si="2"/>
         <v>2001:1:1::1</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="5">
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7" s="5">
         <v>0</v>
       </c>
-      <c r="M7" s="2" t="str">
+      <c r="M7" s="5" t="str">
         <f t="shared" si="11"/>
         <v>PC-27</v>
       </c>
-      <c r="N7" s="2">
+      <c r="N7" s="5">
         <v>4</v>
       </c>
-      <c r="O7" s="2" t="str">
+      <c r="O7" s="5" t="str">
         <f t="shared" si="3"/>
         <v>2001:2:1::/112</v>
       </c>
-      <c r="P7" s="2" t="str">
+      <c r="P7" s="5" t="str">
         <f t="shared" si="4"/>
         <v>2001:2:1::5</v>
       </c>
-      <c r="Q7" s="2">
-        <v>112</v>
-      </c>
-      <c r="R7" s="2" t="str">
+      <c r="Q7" s="5">
+        <v>112</v>
+      </c>
+      <c r="R7" s="5" t="str">
         <f t="shared" si="5"/>
         <v>2001:2:1::1</v>
       </c>
-      <c r="T7" s="2">
+      <c r="T7" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U7" s="2">
+      <c r="U7" s="5">
         <v>0</v>
       </c>
-      <c r="V7" s="2" t="str">
+      <c r="V7" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-55</v>
       </c>
-      <c r="W7" s="2">
+      <c r="W7" s="5">
         <v>4</v>
       </c>
-      <c r="X7" s="2" t="str">
+      <c r="X7" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:1::/112</v>
       </c>
-      <c r="Y7" s="2" t="str">
+      <c r="Y7" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:1::5</v>
       </c>
-      <c r="Z7" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA7" s="2" t="str">
+      <c r="Z7" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA7" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:1::1</v>
       </c>
     </row>
     <row r="8" spans="2:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <f>C4+1</f>
         <v>1</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <f>E4</f>
         <v>1</v>
       </c>
-      <c r="F8" s="4" t="str">
+      <c r="F8" s="3" t="str">
         <f t="shared" si="0"/>
         <v>2001:1:2::/112</v>
       </c>
-      <c r="G8" s="4" t="str">
+      <c r="G8" s="3" t="str">
         <f t="shared" si="1"/>
         <v>2001:1:2::2</v>
       </c>
-      <c r="H8" s="4">
-        <v>112</v>
-      </c>
-      <c r="I8" s="4" t="str">
+      <c r="H8" s="3">
+        <v>112</v>
+      </c>
+      <c r="I8" s="3" t="str">
         <f t="shared" si="2"/>
         <v>2001:1:2::1</v>
       </c>
@@ -5854,66 +5863,66 @@
         <f t="shared" si="5"/>
         <v>2001:2:2::1</v>
       </c>
-      <c r="T8" s="2">
+      <c r="T8" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U8" s="2">
+      <c r="U8" s="5">
         <f>U4+1</f>
         <v>1</v>
       </c>
-      <c r="V8" s="2" t="str">
+      <c r="V8" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-56</v>
       </c>
-      <c r="W8" s="2">
+      <c r="W8" s="5">
         <f>W4</f>
         <v>1</v>
       </c>
-      <c r="X8" s="2" t="str">
+      <c r="X8" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:2::/112</v>
       </c>
-      <c r="Y8" s="2" t="str">
+      <c r="Y8" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:2::2</v>
       </c>
-      <c r="Z8" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA8" s="2" t="str">
+      <c r="Z8" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA8" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:2::1</v>
       </c>
     </row>
     <row r="9" spans="2:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <f t="shared" ref="C9:C27" si="14">C5+1</f>
         <v>1</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <f t="shared" ref="E9:E27" si="15">E5</f>
         <v>2</v>
       </c>
-      <c r="F9" s="4" t="str">
+      <c r="F9" s="3" t="str">
         <f t="shared" si="0"/>
         <v>2001:1:2::/112</v>
       </c>
-      <c r="G9" s="4" t="str">
+      <c r="G9" s="3" t="str">
         <f t="shared" si="1"/>
         <v>2001:1:2::3</v>
       </c>
-      <c r="H9" s="4">
-        <v>112</v>
-      </c>
-      <c r="I9" s="4" t="str">
+      <c r="H9" s="3">
+        <v>112</v>
+      </c>
+      <c r="I9" s="3" t="str">
         <f t="shared" si="2"/>
         <v>2001:1:2::1</v>
       </c>
@@ -5948,66 +5957,66 @@
         <f t="shared" si="5"/>
         <v>2001:2:2::1</v>
       </c>
-      <c r="T9" s="2">
+      <c r="T9" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U9" s="2">
+      <c r="U9" s="5">
         <f t="shared" ref="U9:U72" si="18">U5+1</f>
         <v>1</v>
       </c>
-      <c r="V9" s="2" t="str">
+      <c r="V9" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-57</v>
       </c>
-      <c r="W9" s="2">
+      <c r="W9" s="5">
         <f t="shared" ref="W9:W72" si="19">W5</f>
         <v>2</v>
       </c>
-      <c r="X9" s="2" t="str">
+      <c r="X9" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:2::/112</v>
       </c>
-      <c r="Y9" s="2" t="str">
+      <c r="Y9" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:2::3</v>
       </c>
-      <c r="Z9" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA9" s="2" t="str">
+      <c r="Z9" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA9" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:2::1</v>
       </c>
     </row>
     <row r="10" spans="2:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <f t="shared" si="15"/>
         <v>3</v>
       </c>
-      <c r="F10" s="4" t="str">
+      <c r="F10" s="3" t="str">
         <f t="shared" si="0"/>
         <v>2001:1:2::/112</v>
       </c>
-      <c r="G10" s="4" t="str">
+      <c r="G10" s="3" t="str">
         <f t="shared" si="1"/>
         <v>2001:1:2::4</v>
       </c>
-      <c r="H10" s="4">
-        <v>112</v>
-      </c>
-      <c r="I10" s="4" t="str">
+      <c r="H10" s="3">
+        <v>112</v>
+      </c>
+      <c r="I10" s="3" t="str">
         <f t="shared" si="2"/>
         <v>2001:1:2::1</v>
       </c>
@@ -6042,66 +6051,66 @@
         <f t="shared" si="5"/>
         <v>2001:2:2::1</v>
       </c>
-      <c r="T10" s="2">
+      <c r="T10" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U10" s="2">
+      <c r="U10" s="5">
         <f t="shared" si="18"/>
         <v>1</v>
       </c>
-      <c r="V10" s="2" t="str">
+      <c r="V10" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-58</v>
       </c>
-      <c r="W10" s="2">
+      <c r="W10" s="5">
         <f t="shared" si="19"/>
         <v>3</v>
       </c>
-      <c r="X10" s="2" t="str">
+      <c r="X10" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:2::/112</v>
       </c>
-      <c r="Y10" s="2" t="str">
+      <c r="Y10" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:2::4</v>
       </c>
-      <c r="Z10" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA10" s="2" t="str">
+      <c r="Z10" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA10" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:2::1</v>
       </c>
     </row>
     <row r="11" spans="2:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="B11" s="4">
+      <c r="B11" s="3">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <f t="shared" si="15"/>
         <v>4</v>
       </c>
-      <c r="F11" s="4" t="str">
+      <c r="F11" s="3" t="str">
         <f t="shared" si="0"/>
         <v>2001:1:2::/112</v>
       </c>
-      <c r="G11" s="4" t="str">
+      <c r="G11" s="3" t="str">
         <f t="shared" si="1"/>
         <v>2001:1:2::5</v>
       </c>
-      <c r="H11" s="4">
-        <v>112</v>
-      </c>
-      <c r="I11" s="4" t="str">
+      <c r="H11" s="3">
+        <v>112</v>
+      </c>
+      <c r="I11" s="3" t="str">
         <f t="shared" si="2"/>
         <v>2001:1:2::1</v>
       </c>
@@ -6136,66 +6145,66 @@
         <f t="shared" si="5"/>
         <v>2001:2:2::1</v>
       </c>
-      <c r="T11" s="2">
+      <c r="T11" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U11" s="2">
+      <c r="U11" s="5">
         <f t="shared" si="18"/>
         <v>1</v>
       </c>
-      <c r="V11" s="2" t="str">
+      <c r="V11" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-59</v>
       </c>
-      <c r="W11" s="2">
+      <c r="W11" s="5">
         <f t="shared" si="19"/>
         <v>4</v>
       </c>
-      <c r="X11" s="2" t="str">
+      <c r="X11" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:2::/112</v>
       </c>
-      <c r="Y11" s="2" t="str">
+      <c r="Y11" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:2::5</v>
       </c>
-      <c r="Z11" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA11" s="2" t="str">
+      <c r="Z11" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA11" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:2::1</v>
       </c>
     </row>
     <row r="12" spans="2:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <f>C8+1</f>
         <v>2</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <f t="shared" si="15"/>
         <v>1</v>
       </c>
-      <c r="F12" s="4" t="str">
+      <c r="F12" s="3" t="str">
         <f t="shared" si="0"/>
         <v>2001:1:3::/112</v>
       </c>
-      <c r="G12" s="4" t="str">
+      <c r="G12" s="3" t="str">
         <f t="shared" si="1"/>
         <v>2001:1:3::2</v>
       </c>
-      <c r="H12" s="4">
-        <v>112</v>
-      </c>
-      <c r="I12" s="4" t="str">
+      <c r="H12" s="3">
+        <v>112</v>
+      </c>
+      <c r="I12" s="3" t="str">
         <f t="shared" si="2"/>
         <v>2001:1:3::1</v>
       </c>
@@ -6230,66 +6239,66 @@
         <f t="shared" si="5"/>
         <v>2001:2:3::1</v>
       </c>
-      <c r="T12" s="2">
+      <c r="T12" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U12" s="2">
+      <c r="U12" s="5">
         <f>U8+1</f>
         <v>2</v>
       </c>
-      <c r="V12" s="2" t="str">
+      <c r="V12" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-60</v>
       </c>
-      <c r="W12" s="2">
+      <c r="W12" s="5">
         <f t="shared" si="19"/>
         <v>1</v>
       </c>
-      <c r="X12" s="2" t="str">
+      <c r="X12" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:3::/112</v>
       </c>
-      <c r="Y12" s="2" t="str">
+      <c r="Y12" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:3::2</v>
       </c>
-      <c r="Z12" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA12" s="2" t="str">
+      <c r="Z12" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA12" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:3::1</v>
       </c>
     </row>
     <row r="13" spans="2:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="B13" s="4">
+      <c r="B13" s="3">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="3">
         <f t="shared" si="15"/>
         <v>2</v>
       </c>
-      <c r="F13" s="4" t="str">
+      <c r="F13" s="3" t="str">
         <f t="shared" si="0"/>
         <v>2001:1:3::/112</v>
       </c>
-      <c r="G13" s="4" t="str">
+      <c r="G13" s="3" t="str">
         <f t="shared" si="1"/>
         <v>2001:1:3::3</v>
       </c>
-      <c r="H13" s="4">
-        <v>112</v>
-      </c>
-      <c r="I13" s="4" t="str">
+      <c r="H13" s="3">
+        <v>112</v>
+      </c>
+      <c r="I13" s="3" t="str">
         <f t="shared" si="2"/>
         <v>2001:1:3::1</v>
       </c>
@@ -6324,66 +6333,66 @@
         <f t="shared" si="5"/>
         <v>2001:2:3::1</v>
       </c>
-      <c r="T13" s="2">
+      <c r="T13" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U13" s="2">
+      <c r="U13" s="5">
         <f t="shared" si="18"/>
         <v>2</v>
       </c>
-      <c r="V13" s="2" t="str">
+      <c r="V13" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-61</v>
       </c>
-      <c r="W13" s="2">
+      <c r="W13" s="5">
         <f t="shared" si="19"/>
         <v>2</v>
       </c>
-      <c r="X13" s="2" t="str">
+      <c r="X13" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:3::/112</v>
       </c>
-      <c r="Y13" s="2" t="str">
+      <c r="Y13" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:3::3</v>
       </c>
-      <c r="Z13" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA13" s="2" t="str">
+      <c r="Z13" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA13" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:3::1</v>
       </c>
     </row>
     <row r="14" spans="2:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="B14" s="4">
+      <c r="B14" s="3">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="3">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="3">
         <f t="shared" si="15"/>
         <v>3</v>
       </c>
-      <c r="F14" s="4" t="str">
+      <c r="F14" s="3" t="str">
         <f t="shared" si="0"/>
         <v>2001:1:3::/112</v>
       </c>
-      <c r="G14" s="4" t="str">
+      <c r="G14" s="3" t="str">
         <f t="shared" si="1"/>
         <v>2001:1:3::4</v>
       </c>
-      <c r="H14" s="4">
-        <v>112</v>
-      </c>
-      <c r="I14" s="4" t="str">
+      <c r="H14" s="3">
+        <v>112</v>
+      </c>
+      <c r="I14" s="3" t="str">
         <f t="shared" si="2"/>
         <v>2001:1:3::1</v>
       </c>
@@ -6418,66 +6427,66 @@
         <f t="shared" si="5"/>
         <v>2001:2:3::1</v>
       </c>
-      <c r="T14" s="2">
+      <c r="T14" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U14" s="2">
+      <c r="U14" s="5">
         <f t="shared" si="18"/>
         <v>2</v>
       </c>
-      <c r="V14" s="2" t="str">
+      <c r="V14" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-62</v>
       </c>
-      <c r="W14" s="2">
+      <c r="W14" s="5">
         <f t="shared" si="19"/>
         <v>3</v>
       </c>
-      <c r="X14" s="2" t="str">
+      <c r="X14" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:3::/112</v>
       </c>
-      <c r="Y14" s="2" t="str">
+      <c r="Y14" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:3::4</v>
       </c>
-      <c r="Z14" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA14" s="2" t="str">
+      <c r="Z14" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA14" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:3::1</v>
       </c>
     </row>
     <row r="15" spans="2:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="B15" s="4">
+      <c r="B15" s="3">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <f t="shared" si="15"/>
         <v>4</v>
       </c>
-      <c r="F15" s="4" t="str">
+      <c r="F15" s="3" t="str">
         <f t="shared" si="0"/>
         <v>2001:1:3::/112</v>
       </c>
-      <c r="G15" s="4" t="str">
+      <c r="G15" s="3" t="str">
         <f t="shared" si="1"/>
         <v>2001:1:3::5</v>
       </c>
-      <c r="H15" s="4">
-        <v>112</v>
-      </c>
-      <c r="I15" s="4" t="str">
+      <c r="H15" s="3">
+        <v>112</v>
+      </c>
+      <c r="I15" s="3" t="str">
         <f t="shared" si="2"/>
         <v>2001:1:3::1</v>
       </c>
@@ -6512,66 +6521,66 @@
         <f t="shared" si="5"/>
         <v>2001:2:3::1</v>
       </c>
-      <c r="T15" s="2">
+      <c r="T15" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U15" s="2">
+      <c r="U15" s="5">
         <f t="shared" si="18"/>
         <v>2</v>
       </c>
-      <c r="V15" s="2" t="str">
+      <c r="V15" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-63</v>
       </c>
-      <c r="W15" s="2">
+      <c r="W15" s="5">
         <f t="shared" si="19"/>
         <v>4</v>
       </c>
-      <c r="X15" s="2" t="str">
+      <c r="X15" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:3::/112</v>
       </c>
-      <c r="Y15" s="2" t="str">
+      <c r="Y15" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:3::5</v>
       </c>
-      <c r="Z15" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA15" s="2" t="str">
+      <c r="Z15" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA15" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:3::1</v>
       </c>
     </row>
     <row r="16" spans="2:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="B16" s="4">
+      <c r="B16" s="3">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="3">
         <f>C12+1</f>
         <v>3</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="3">
         <f t="shared" si="15"/>
         <v>1</v>
       </c>
-      <c r="F16" s="4" t="str">
+      <c r="F16" s="3" t="str">
         <f t="shared" si="0"/>
         <v>2001:1:4::/112</v>
       </c>
-      <c r="G16" s="4" t="str">
+      <c r="G16" s="3" t="str">
         <f t="shared" si="1"/>
         <v>2001:1:4::2</v>
       </c>
-      <c r="H16" s="4">
-        <v>112</v>
-      </c>
-      <c r="I16" s="4" t="str">
+      <c r="H16" s="3">
+        <v>112</v>
+      </c>
+      <c r="I16" s="3" t="str">
         <f t="shared" si="2"/>
         <v>2001:1:4::1</v>
       </c>
@@ -6606,66 +6615,66 @@
         <f t="shared" si="5"/>
         <v>2001:2:4::1</v>
       </c>
-      <c r="T16" s="2">
+      <c r="T16" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U16" s="2">
+      <c r="U16" s="5">
         <f>U12+1</f>
         <v>3</v>
       </c>
-      <c r="V16" s="2" t="str">
+      <c r="V16" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-64</v>
       </c>
-      <c r="W16" s="2">
+      <c r="W16" s="5">
         <f t="shared" si="19"/>
         <v>1</v>
       </c>
-      <c r="X16" s="2" t="str">
+      <c r="X16" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:4::/112</v>
       </c>
-      <c r="Y16" s="2" t="str">
+      <c r="Y16" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:4::2</v>
       </c>
-      <c r="Z16" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA16" s="2" t="str">
+      <c r="Z16" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA16" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:4::1</v>
       </c>
     </row>
     <row r="17" spans="2:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="B17" s="4">
+      <c r="B17" s="3">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="3">
         <f t="shared" si="14"/>
         <v>3</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="3">
         <f t="shared" si="15"/>
         <v>2</v>
       </c>
-      <c r="F17" s="4" t="str">
+      <c r="F17" s="3" t="str">
         <f t="shared" si="0"/>
         <v>2001:1:4::/112</v>
       </c>
-      <c r="G17" s="4" t="str">
+      <c r="G17" s="3" t="str">
         <f t="shared" si="1"/>
         <v>2001:1:4::3</v>
       </c>
-      <c r="H17" s="4">
-        <v>112</v>
-      </c>
-      <c r="I17" s="4" t="str">
+      <c r="H17" s="3">
+        <v>112</v>
+      </c>
+      <c r="I17" s="3" t="str">
         <f t="shared" si="2"/>
         <v>2001:1:4::1</v>
       </c>
@@ -6700,66 +6709,66 @@
         <f t="shared" si="5"/>
         <v>2001:2:4::1</v>
       </c>
-      <c r="T17" s="2">
+      <c r="T17" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U17" s="2">
+      <c r="U17" s="5">
         <f t="shared" si="18"/>
         <v>3</v>
       </c>
-      <c r="V17" s="2" t="str">
+      <c r="V17" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-65</v>
       </c>
-      <c r="W17" s="2">
+      <c r="W17" s="5">
         <f t="shared" si="19"/>
         <v>2</v>
       </c>
-      <c r="X17" s="2" t="str">
+      <c r="X17" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:4::/112</v>
       </c>
-      <c r="Y17" s="2" t="str">
+      <c r="Y17" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:4::3</v>
       </c>
-      <c r="Z17" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA17" s="2" t="str">
+      <c r="Z17" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA17" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:4::1</v>
       </c>
     </row>
     <row r="18" spans="2:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="B18" s="4">
+      <c r="B18" s="3">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="3">
         <f t="shared" si="14"/>
         <v>3</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="3">
         <f t="shared" si="15"/>
         <v>3</v>
       </c>
-      <c r="F18" s="4" t="str">
+      <c r="F18" s="3" t="str">
         <f t="shared" si="0"/>
         <v>2001:1:4::/112</v>
       </c>
-      <c r="G18" s="4" t="str">
+      <c r="G18" s="3" t="str">
         <f t="shared" si="1"/>
         <v>2001:1:4::4</v>
       </c>
-      <c r="H18" s="4">
-        <v>112</v>
-      </c>
-      <c r="I18" s="4" t="str">
+      <c r="H18" s="3">
+        <v>112</v>
+      </c>
+      <c r="I18" s="3" t="str">
         <f t="shared" si="2"/>
         <v>2001:1:4::1</v>
       </c>
@@ -6794,66 +6803,66 @@
         <f t="shared" si="5"/>
         <v>2001:2:4::1</v>
       </c>
-      <c r="T18" s="2">
+      <c r="T18" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U18" s="2">
+      <c r="U18" s="5">
         <f t="shared" si="18"/>
         <v>3</v>
       </c>
-      <c r="V18" s="2" t="str">
+      <c r="V18" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-66</v>
       </c>
-      <c r="W18" s="2">
+      <c r="W18" s="5">
         <f t="shared" si="19"/>
         <v>3</v>
       </c>
-      <c r="X18" s="2" t="str">
+      <c r="X18" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:4::/112</v>
       </c>
-      <c r="Y18" s="2" t="str">
+      <c r="Y18" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:4::4</v>
       </c>
-      <c r="Z18" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA18" s="2" t="str">
+      <c r="Z18" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA18" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:4::1</v>
       </c>
     </row>
     <row r="19" spans="2:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="B19" s="4">
+      <c r="B19" s="3">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="3">
         <f t="shared" si="14"/>
         <v>3</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="3">
         <f t="shared" si="15"/>
         <v>4</v>
       </c>
-      <c r="F19" s="4" t="str">
+      <c r="F19" s="3" t="str">
         <f t="shared" si="0"/>
         <v>2001:1:4::/112</v>
       </c>
-      <c r="G19" s="4" t="str">
+      <c r="G19" s="3" t="str">
         <f t="shared" si="1"/>
         <v>2001:1:4::5</v>
       </c>
-      <c r="H19" s="4">
-        <v>112</v>
-      </c>
-      <c r="I19" s="4" t="str">
+      <c r="H19" s="3">
+        <v>112</v>
+      </c>
+      <c r="I19" s="3" t="str">
         <f t="shared" si="2"/>
         <v>2001:1:4::1</v>
       </c>
@@ -6888,66 +6897,66 @@
         <f t="shared" si="5"/>
         <v>2001:2:4::1</v>
       </c>
-      <c r="T19" s="2">
+      <c r="T19" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U19" s="2">
+      <c r="U19" s="5">
         <f t="shared" si="18"/>
         <v>3</v>
       </c>
-      <c r="V19" s="2" t="str">
+      <c r="V19" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-67</v>
       </c>
-      <c r="W19" s="2">
+      <c r="W19" s="5">
         <f t="shared" si="19"/>
         <v>4</v>
       </c>
-      <c r="X19" s="2" t="str">
+      <c r="X19" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:4::/112</v>
       </c>
-      <c r="Y19" s="2" t="str">
+      <c r="Y19" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:4::5</v>
       </c>
-      <c r="Z19" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA19" s="2" t="str">
+      <c r="Z19" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA19" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:4::1</v>
       </c>
     </row>
     <row r="20" spans="2:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="B20" s="4">
+      <c r="B20" s="3">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="3">
         <f>C16+1</f>
         <v>4</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="3">
         <f t="shared" si="15"/>
         <v>1</v>
       </c>
-      <c r="F20" s="4" t="str">
+      <c r="F20" s="3" t="str">
         <f t="shared" si="0"/>
         <v>2001:1:5::/112</v>
       </c>
-      <c r="G20" s="4" t="str">
+      <c r="G20" s="3" t="str">
         <f t="shared" si="1"/>
         <v>2001:1:5::2</v>
       </c>
-      <c r="H20" s="4">
-        <v>112</v>
-      </c>
-      <c r="I20" s="4" t="str">
+      <c r="H20" s="3">
+        <v>112</v>
+      </c>
+      <c r="I20" s="3" t="str">
         <f t="shared" si="2"/>
         <v>2001:1:5::1</v>
       </c>
@@ -6982,66 +6991,66 @@
         <f t="shared" si="5"/>
         <v>2001:2:5::1</v>
       </c>
-      <c r="T20" s="2">
+      <c r="T20" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U20" s="2">
+      <c r="U20" s="5">
         <f>U16+1</f>
         <v>4</v>
       </c>
-      <c r="V20" s="2" t="str">
+      <c r="V20" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-68</v>
       </c>
-      <c r="W20" s="2">
+      <c r="W20" s="5">
         <f t="shared" si="19"/>
         <v>1</v>
       </c>
-      <c r="X20" s="2" t="str">
+      <c r="X20" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:5::/112</v>
       </c>
-      <c r="Y20" s="2" t="str">
+      <c r="Y20" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:5::2</v>
       </c>
-      <c r="Z20" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA20" s="2" t="str">
+      <c r="Z20" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA20" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:5::1</v>
       </c>
     </row>
     <row r="21" spans="2:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="B21" s="4">
+      <c r="B21" s="3">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="3">
         <f t="shared" si="14"/>
         <v>4</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="3">
         <f t="shared" si="15"/>
         <v>2</v>
       </c>
-      <c r="F21" s="4" t="str">
+      <c r="F21" s="3" t="str">
         <f t="shared" si="0"/>
         <v>2001:1:5::/112</v>
       </c>
-      <c r="G21" s="4" t="str">
+      <c r="G21" s="3" t="str">
         <f t="shared" si="1"/>
         <v>2001:1:5::3</v>
       </c>
-      <c r="H21" s="4">
-        <v>112</v>
-      </c>
-      <c r="I21" s="4" t="str">
+      <c r="H21" s="3">
+        <v>112</v>
+      </c>
+      <c r="I21" s="3" t="str">
         <f t="shared" si="2"/>
         <v>2001:1:5::1</v>
       </c>
@@ -7076,66 +7085,66 @@
         <f t="shared" si="5"/>
         <v>2001:2:5::1</v>
       </c>
-      <c r="T21" s="2">
+      <c r="T21" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U21" s="2">
+      <c r="U21" s="5">
         <f t="shared" si="18"/>
         <v>4</v>
       </c>
-      <c r="V21" s="2" t="str">
+      <c r="V21" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-69</v>
       </c>
-      <c r="W21" s="2">
+      <c r="W21" s="5">
         <f t="shared" si="19"/>
         <v>2</v>
       </c>
-      <c r="X21" s="2" t="str">
+      <c r="X21" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:5::/112</v>
       </c>
-      <c r="Y21" s="2" t="str">
+      <c r="Y21" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:5::3</v>
       </c>
-      <c r="Z21" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA21" s="2" t="str">
+      <c r="Z21" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA21" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:5::1</v>
       </c>
     </row>
     <row r="22" spans="2:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="B22" s="4">
+      <c r="B22" s="3">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="3">
         <f t="shared" si="14"/>
         <v>4</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="3">
         <f t="shared" si="15"/>
         <v>3</v>
       </c>
-      <c r="F22" s="4" t="str">
+      <c r="F22" s="3" t="str">
         <f t="shared" si="0"/>
         <v>2001:1:5::/112</v>
       </c>
-      <c r="G22" s="4" t="str">
+      <c r="G22" s="3" t="str">
         <f t="shared" si="1"/>
         <v>2001:1:5::4</v>
       </c>
-      <c r="H22" s="4">
-        <v>112</v>
-      </c>
-      <c r="I22" s="4" t="str">
+      <c r="H22" s="3">
+        <v>112</v>
+      </c>
+      <c r="I22" s="3" t="str">
         <f t="shared" si="2"/>
         <v>2001:1:5::1</v>
       </c>
@@ -7170,66 +7179,66 @@
         <f t="shared" si="5"/>
         <v>2001:2:5::1</v>
       </c>
-      <c r="T22" s="2">
+      <c r="T22" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U22" s="2">
+      <c r="U22" s="5">
         <f t="shared" si="18"/>
         <v>4</v>
       </c>
-      <c r="V22" s="2" t="str">
+      <c r="V22" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-70</v>
       </c>
-      <c r="W22" s="2">
+      <c r="W22" s="5">
         <f t="shared" si="19"/>
         <v>3</v>
       </c>
-      <c r="X22" s="2" t="str">
+      <c r="X22" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:5::/112</v>
       </c>
-      <c r="Y22" s="2" t="str">
+      <c r="Y22" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:5::4</v>
       </c>
-      <c r="Z22" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA22" s="2" t="str">
+      <c r="Z22" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA22" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:5::1</v>
       </c>
     </row>
     <row r="23" spans="2:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="B23" s="4">
+      <c r="B23" s="3">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="3">
         <f>C19+1</f>
         <v>4</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="3">
         <f t="shared" si="15"/>
         <v>4</v>
       </c>
-      <c r="F23" s="4" t="str">
+      <c r="F23" s="3" t="str">
         <f t="shared" si="0"/>
         <v>2001:1:5::/112</v>
       </c>
-      <c r="G23" s="4" t="str">
+      <c r="G23" s="3" t="str">
         <f t="shared" si="1"/>
         <v>2001:1:5::5</v>
       </c>
-      <c r="H23" s="4">
-        <v>112</v>
-      </c>
-      <c r="I23" s="4" t="str">
+      <c r="H23" s="3">
+        <v>112</v>
+      </c>
+      <c r="I23" s="3" t="str">
         <f t="shared" si="2"/>
         <v>2001:1:5::1</v>
       </c>
@@ -7264,66 +7273,66 @@
         <f t="shared" si="5"/>
         <v>2001:2:5::1</v>
       </c>
-      <c r="T23" s="2">
+      <c r="T23" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U23" s="2">
+      <c r="U23" s="5">
         <f>U19+1</f>
         <v>4</v>
       </c>
-      <c r="V23" s="2" t="str">
+      <c r="V23" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-71</v>
       </c>
-      <c r="W23" s="2">
+      <c r="W23" s="5">
         <f t="shared" si="19"/>
         <v>4</v>
       </c>
-      <c r="X23" s="2" t="str">
+      <c r="X23" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:5::/112</v>
       </c>
-      <c r="Y23" s="2" t="str">
+      <c r="Y23" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:5::5</v>
       </c>
-      <c r="Z23" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA23" s="2" t="str">
+      <c r="Z23" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA23" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:5::1</v>
       </c>
     </row>
     <row r="24" spans="2:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="B24" s="2">
+      <c r="B24" s="5">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="5">
         <f t="shared" si="14"/>
         <v>5</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="5">
         <f t="shared" si="15"/>
         <v>1</v>
       </c>
-      <c r="F24" s="2" t="str">
+      <c r="F24" s="5" t="str">
         <f t="shared" si="0"/>
         <v>2001:1:6::/112</v>
       </c>
-      <c r="G24" s="2" t="str">
+      <c r="G24" s="5" t="str">
         <f t="shared" si="1"/>
         <v>2001:1:6::2</v>
       </c>
-      <c r="H24" s="2">
-        <v>112</v>
-      </c>
-      <c r="I24" s="2" t="str">
+      <c r="H24" s="5">
+        <v>112</v>
+      </c>
+      <c r="I24" s="5" t="str">
         <f t="shared" si="2"/>
         <v>2001:1:6::1</v>
       </c>
@@ -7358,66 +7367,66 @@
         <f t="shared" si="5"/>
         <v>2001:2:6::1</v>
       </c>
-      <c r="T24" s="2">
+      <c r="T24" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U24" s="2">
+      <c r="U24" s="5">
         <f t="shared" si="18"/>
         <v>5</v>
       </c>
-      <c r="V24" s="2" t="str">
+      <c r="V24" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-72</v>
       </c>
-      <c r="W24" s="2">
+      <c r="W24" s="5">
         <f t="shared" si="19"/>
         <v>1</v>
       </c>
-      <c r="X24" s="2" t="str">
+      <c r="X24" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:6::/112</v>
       </c>
-      <c r="Y24" s="2" t="str">
+      <c r="Y24" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:6::2</v>
       </c>
-      <c r="Z24" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA24" s="2" t="str">
+      <c r="Z24" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA24" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:6::1</v>
       </c>
     </row>
     <row r="25" spans="2:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="B25" s="2">
+      <c r="B25" s="5">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="5">
         <f t="shared" si="14"/>
         <v>5</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="5">
         <f t="shared" si="15"/>
         <v>2</v>
       </c>
-      <c r="F25" s="2" t="str">
+      <c r="F25" s="5" t="str">
         <f t="shared" si="0"/>
         <v>2001:1:6::/112</v>
       </c>
-      <c r="G25" s="2" t="str">
+      <c r="G25" s="5" t="str">
         <f t="shared" si="1"/>
         <v>2001:1:6::3</v>
       </c>
-      <c r="H25" s="2">
-        <v>112</v>
-      </c>
-      <c r="I25" s="2" t="str">
+      <c r="H25" s="5">
+        <v>112</v>
+      </c>
+      <c r="I25" s="5" t="str">
         <f t="shared" si="2"/>
         <v>2001:1:6::1</v>
       </c>
@@ -7452,66 +7461,66 @@
         <f t="shared" si="5"/>
         <v>2001:2:6::1</v>
       </c>
-      <c r="T25" s="2">
+      <c r="T25" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U25" s="2">
+      <c r="U25" s="5">
         <f t="shared" si="18"/>
         <v>5</v>
       </c>
-      <c r="V25" s="2" t="str">
+      <c r="V25" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-73</v>
       </c>
-      <c r="W25" s="2">
+      <c r="W25" s="5">
         <f t="shared" si="19"/>
         <v>2</v>
       </c>
-      <c r="X25" s="2" t="str">
+      <c r="X25" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:6::/112</v>
       </c>
-      <c r="Y25" s="2" t="str">
+      <c r="Y25" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:6::3</v>
       </c>
-      <c r="Z25" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA25" s="2" t="str">
+      <c r="Z25" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA25" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:6::1</v>
       </c>
     </row>
     <row r="26" spans="2:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="B26" s="2">
+      <c r="B26" s="5">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="5">
         <f>C22+1</f>
         <v>5</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26" s="5">
         <f t="shared" si="15"/>
         <v>3</v>
       </c>
-      <c r="F26" s="2" t="str">
+      <c r="F26" s="5" t="str">
         <f t="shared" si="0"/>
         <v>2001:1:6::/112</v>
       </c>
-      <c r="G26" s="2" t="str">
+      <c r="G26" s="5" t="str">
         <f t="shared" si="1"/>
         <v>2001:1:6::4</v>
       </c>
-      <c r="H26" s="2">
-        <v>112</v>
-      </c>
-      <c r="I26" s="2" t="str">
+      <c r="H26" s="5">
+        <v>112</v>
+      </c>
+      <c r="I26" s="5" t="str">
         <f t="shared" si="2"/>
         <v>2001:1:6::1</v>
       </c>
@@ -7546,66 +7555,66 @@
         <f t="shared" si="5"/>
         <v>2001:2:6::1</v>
       </c>
-      <c r="T26" s="2">
+      <c r="T26" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U26" s="2">
+      <c r="U26" s="5">
         <f>U22+1</f>
         <v>5</v>
       </c>
-      <c r="V26" s="2" t="str">
+      <c r="V26" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-74</v>
       </c>
-      <c r="W26" s="2">
+      <c r="W26" s="5">
         <f t="shared" si="19"/>
         <v>3</v>
       </c>
-      <c r="X26" s="2" t="str">
+      <c r="X26" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:6::/112</v>
       </c>
-      <c r="Y26" s="2" t="str">
+      <c r="Y26" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:6::4</v>
       </c>
-      <c r="Z26" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA26" s="2" t="str">
+      <c r="Z26" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA26" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:6::1</v>
       </c>
     </row>
     <row r="27" spans="2:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="B27" s="2">
+      <c r="B27" s="5">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="5">
         <f t="shared" si="14"/>
         <v>5</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27" s="5">
         <f t="shared" si="15"/>
         <v>4</v>
       </c>
-      <c r="F27" s="2" t="str">
+      <c r="F27" s="5" t="str">
         <f t="shared" si="0"/>
         <v>2001:1:6::/112</v>
       </c>
-      <c r="G27" s="2" t="str">
+      <c r="G27" s="5" t="str">
         <f t="shared" si="1"/>
         <v>2001:1:6::5</v>
       </c>
-      <c r="H27" s="2">
-        <v>112</v>
-      </c>
-      <c r="I27" s="2" t="str">
+      <c r="H27" s="5">
+        <v>112</v>
+      </c>
+      <c r="I27" s="5" t="str">
         <f t="shared" si="2"/>
         <v>2001:1:6::1</v>
       </c>
@@ -7640,34 +7649,34 @@
         <f t="shared" si="5"/>
         <v>2001:2:6::1</v>
       </c>
-      <c r="T27" s="2">
+      <c r="T27" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U27" s="2">
+      <c r="U27" s="5">
         <f t="shared" si="18"/>
         <v>5</v>
       </c>
-      <c r="V27" s="2" t="str">
+      <c r="V27" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-75</v>
       </c>
-      <c r="W27" s="2">
+      <c r="W27" s="5">
         <f t="shared" si="19"/>
         <v>4</v>
       </c>
-      <c r="X27" s="2" t="str">
+      <c r="X27" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:6::/112</v>
       </c>
-      <c r="Y27" s="2" t="str">
+      <c r="Y27" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:6::5</v>
       </c>
-      <c r="Z27" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA27" s="2" t="str">
+      <c r="Z27" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA27" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:6::1</v>
       </c>
@@ -7704,34 +7713,34 @@
         <f t="shared" si="5"/>
         <v>2001:2:7::1</v>
       </c>
-      <c r="T28" s="2">
+      <c r="T28" s="5">
         <f>T27</f>
         <v>3</v>
       </c>
-      <c r="U28" s="2">
+      <c r="U28" s="5">
         <f t="shared" si="18"/>
         <v>6</v>
       </c>
-      <c r="V28" s="2" t="str">
+      <c r="V28" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-76</v>
       </c>
-      <c r="W28" s="2">
+      <c r="W28" s="5">
         <f t="shared" si="19"/>
         <v>1</v>
       </c>
-      <c r="X28" s="2" t="str">
+      <c r="X28" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:7::/112</v>
       </c>
-      <c r="Y28" s="2" t="str">
+      <c r="Y28" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:7::2</v>
       </c>
-      <c r="Z28" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA28" s="2" t="str">
+      <c r="Z28" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA28" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:7::1</v>
       </c>
@@ -7768,34 +7777,34 @@
         <f t="shared" si="5"/>
         <v>2001:2:7::1</v>
       </c>
-      <c r="T29" s="2">
+      <c r="T29" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U29" s="2">
+      <c r="U29" s="5">
         <f t="shared" si="18"/>
         <v>6</v>
       </c>
-      <c r="V29" s="2" t="str">
+      <c r="V29" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-77</v>
       </c>
-      <c r="W29" s="2">
+      <c r="W29" s="5">
         <f t="shared" si="19"/>
         <v>2</v>
       </c>
-      <c r="X29" s="2" t="str">
+      <c r="X29" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:7::/112</v>
       </c>
-      <c r="Y29" s="2" t="str">
+      <c r="Y29" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:7::3</v>
       </c>
-      <c r="Z29" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA29" s="2" t="str">
+      <c r="Z29" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA29" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:7::1</v>
       </c>
@@ -7832,34 +7841,34 @@
         <f t="shared" si="5"/>
         <v>2001:2:7::1</v>
       </c>
-      <c r="T30" s="2">
+      <c r="T30" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U30" s="2">
+      <c r="U30" s="5">
         <f t="shared" si="18"/>
         <v>6</v>
       </c>
-      <c r="V30" s="2" t="str">
+      <c r="V30" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-78</v>
       </c>
-      <c r="W30" s="2">
+      <c r="W30" s="5">
         <f t="shared" si="19"/>
         <v>3</v>
       </c>
-      <c r="X30" s="2" t="str">
+      <c r="X30" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:7::/112</v>
       </c>
-      <c r="Y30" s="2" t="str">
+      <c r="Y30" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:7::4</v>
       </c>
-      <c r="Z30" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA30" s="2" t="str">
+      <c r="Z30" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA30" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:7::1</v>
       </c>
@@ -7896,34 +7905,34 @@
         <f t="shared" si="5"/>
         <v>2001:2:7::1</v>
       </c>
-      <c r="T31" s="2">
+      <c r="T31" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U31" s="2">
+      <c r="U31" s="5">
         <f t="shared" si="18"/>
         <v>6</v>
       </c>
-      <c r="V31" s="2" t="str">
+      <c r="V31" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-79</v>
       </c>
-      <c r="W31" s="2">
+      <c r="W31" s="5">
         <f t="shared" si="19"/>
         <v>4</v>
       </c>
-      <c r="X31" s="2" t="str">
+      <c r="X31" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:7::/112</v>
       </c>
-      <c r="Y31" s="2" t="str">
+      <c r="Y31" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:7::5</v>
       </c>
-      <c r="Z31" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA31" s="2" t="str">
+      <c r="Z31" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA31" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:7::1</v>
       </c>
@@ -7937,34 +7946,34 @@
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
-      <c r="T32" s="2">
+      <c r="T32" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U32" s="2">
+      <c r="U32" s="5">
         <f t="shared" si="18"/>
         <v>7</v>
       </c>
-      <c r="V32" s="2" t="str">
+      <c r="V32" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-80</v>
       </c>
-      <c r="W32" s="2">
+      <c r="W32" s="5">
         <f t="shared" si="19"/>
         <v>1</v>
       </c>
-      <c r="X32" s="2" t="str">
+      <c r="X32" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:8::/112</v>
       </c>
-      <c r="Y32" s="2" t="str">
+      <c r="Y32" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:8::2</v>
       </c>
-      <c r="Z32" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA32" s="2" t="str">
+      <c r="Z32" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA32" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:8::1</v>
       </c>
@@ -7978,34 +7987,34 @@
       <c r="P33" s="2"/>
       <c r="Q33" s="2"/>
       <c r="R33" s="2"/>
-      <c r="T33" s="2">
+      <c r="T33" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U33" s="2">
+      <c r="U33" s="5">
         <f t="shared" si="18"/>
         <v>7</v>
       </c>
-      <c r="V33" s="2" t="str">
+      <c r="V33" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-81</v>
       </c>
-      <c r="W33" s="2">
+      <c r="W33" s="5">
         <f t="shared" si="19"/>
         <v>2</v>
       </c>
-      <c r="X33" s="2" t="str">
+      <c r="X33" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:8::/112</v>
       </c>
-      <c r="Y33" s="2" t="str">
+      <c r="Y33" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:8::3</v>
       </c>
-      <c r="Z33" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA33" s="2" t="str">
+      <c r="Z33" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA33" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:8::1</v>
       </c>
@@ -8019,34 +8028,34 @@
       <c r="P34" s="2"/>
       <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
-      <c r="T34" s="2">
+      <c r="T34" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U34" s="2">
+      <c r="U34" s="5">
         <f t="shared" si="18"/>
         <v>7</v>
       </c>
-      <c r="V34" s="2" t="str">
+      <c r="V34" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-82</v>
       </c>
-      <c r="W34" s="2">
+      <c r="W34" s="5">
         <f t="shared" si="19"/>
         <v>3</v>
       </c>
-      <c r="X34" s="2" t="str">
+      <c r="X34" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:8::/112</v>
       </c>
-      <c r="Y34" s="2" t="str">
+      <c r="Y34" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:8::4</v>
       </c>
-      <c r="Z34" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA34" s="2" t="str">
+      <c r="Z34" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA34" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:8::1</v>
       </c>
@@ -8060,595 +8069,595 @@
       <c r="P35" s="2"/>
       <c r="Q35" s="2"/>
       <c r="R35" s="2"/>
-      <c r="T35" s="2">
+      <c r="T35" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U35" s="2">
+      <c r="U35" s="5">
         <f t="shared" si="18"/>
         <v>7</v>
       </c>
-      <c r="V35" s="2" t="str">
+      <c r="V35" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-83</v>
       </c>
-      <c r="W35" s="2">
+      <c r="W35" s="5">
         <f t="shared" si="19"/>
         <v>4</v>
       </c>
-      <c r="X35" s="2" t="str">
+      <c r="X35" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:8::/112</v>
       </c>
-      <c r="Y35" s="2" t="str">
+      <c r="Y35" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:8::5</v>
       </c>
-      <c r="Z35" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA35" s="2" t="str">
+      <c r="Z35" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA35" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:8::1</v>
       </c>
     </row>
     <row r="36" spans="11:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T36" s="2">
+      <c r="T36" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U36" s="2">
+      <c r="U36" s="5">
         <f t="shared" si="18"/>
         <v>8</v>
       </c>
-      <c r="V36" s="2" t="str">
+      <c r="V36" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-84</v>
       </c>
-      <c r="W36" s="2">
+      <c r="W36" s="5">
         <f t="shared" si="19"/>
         <v>1</v>
       </c>
-      <c r="X36" s="2" t="str">
+      <c r="X36" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:9::/112</v>
       </c>
-      <c r="Y36" s="2" t="str">
+      <c r="Y36" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:9::2</v>
       </c>
-      <c r="Z36" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA36" s="2" t="str">
+      <c r="Z36" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA36" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:9::1</v>
       </c>
     </row>
     <row r="37" spans="11:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T37" s="2">
+      <c r="T37" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U37" s="2">
+      <c r="U37" s="5">
         <f t="shared" si="18"/>
         <v>8</v>
       </c>
-      <c r="V37" s="2" t="str">
+      <c r="V37" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-85</v>
       </c>
-      <c r="W37" s="2">
+      <c r="W37" s="5">
         <f t="shared" si="19"/>
         <v>2</v>
       </c>
-      <c r="X37" s="2" t="str">
+      <c r="X37" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:9::/112</v>
       </c>
-      <c r="Y37" s="2" t="str">
+      <c r="Y37" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:9::3</v>
       </c>
-      <c r="Z37" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA37" s="2" t="str">
+      <c r="Z37" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA37" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:9::1</v>
       </c>
     </row>
     <row r="38" spans="11:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T38" s="2">
+      <c r="T38" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U38" s="2">
+      <c r="U38" s="5">
         <f t="shared" si="18"/>
         <v>8</v>
       </c>
-      <c r="V38" s="2" t="str">
+      <c r="V38" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-86</v>
       </c>
-      <c r="W38" s="2">
+      <c r="W38" s="5">
         <f t="shared" si="19"/>
         <v>3</v>
       </c>
-      <c r="X38" s="2" t="str">
+      <c r="X38" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:9::/112</v>
       </c>
-      <c r="Y38" s="2" t="str">
+      <c r="Y38" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:9::4</v>
       </c>
-      <c r="Z38" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA38" s="2" t="str">
+      <c r="Z38" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA38" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:9::1</v>
       </c>
     </row>
     <row r="39" spans="11:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T39" s="2">
+      <c r="T39" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U39" s="2">
+      <c r="U39" s="5">
         <f t="shared" si="18"/>
         <v>8</v>
       </c>
-      <c r="V39" s="2" t="str">
+      <c r="V39" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-87</v>
       </c>
-      <c r="W39" s="2">
+      <c r="W39" s="5">
         <f t="shared" si="19"/>
         <v>4</v>
       </c>
-      <c r="X39" s="2" t="str">
+      <c r="X39" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:9::/112</v>
       </c>
-      <c r="Y39" s="2" t="str">
+      <c r="Y39" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:9::5</v>
       </c>
-      <c r="Z39" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA39" s="2" t="str">
+      <c r="Z39" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA39" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:9::1</v>
       </c>
     </row>
     <row r="40" spans="11:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T40" s="2">
+      <c r="T40" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U40" s="2">
+      <c r="U40" s="5">
         <f t="shared" si="18"/>
         <v>9</v>
       </c>
-      <c r="V40" s="2" t="str">
+      <c r="V40" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-88</v>
       </c>
-      <c r="W40" s="2">
+      <c r="W40" s="5">
         <f t="shared" si="19"/>
         <v>1</v>
       </c>
-      <c r="X40" s="2" t="str">
+      <c r="X40" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:10::/112</v>
       </c>
-      <c r="Y40" s="2" t="str">
+      <c r="Y40" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:10::2</v>
       </c>
-      <c r="Z40" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA40" s="2" t="str">
+      <c r="Z40" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA40" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:10::1</v>
       </c>
     </row>
     <row r="41" spans="11:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T41" s="2">
+      <c r="T41" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U41" s="2">
+      <c r="U41" s="5">
         <f t="shared" si="18"/>
         <v>9</v>
       </c>
-      <c r="V41" s="2" t="str">
+      <c r="V41" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-89</v>
       </c>
-      <c r="W41" s="2">
+      <c r="W41" s="5">
         <f t="shared" si="19"/>
         <v>2</v>
       </c>
-      <c r="X41" s="2" t="str">
+      <c r="X41" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:10::/112</v>
       </c>
-      <c r="Y41" s="2" t="str">
+      <c r="Y41" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:10::3</v>
       </c>
-      <c r="Z41" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA41" s="2" t="str">
+      <c r="Z41" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA41" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:10::1</v>
       </c>
     </row>
     <row r="42" spans="11:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T42" s="2">
+      <c r="T42" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U42" s="2">
+      <c r="U42" s="5">
         <f t="shared" si="18"/>
         <v>9</v>
       </c>
-      <c r="V42" s="2" t="str">
+      <c r="V42" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-90</v>
       </c>
-      <c r="W42" s="2">
+      <c r="W42" s="5">
         <f t="shared" si="19"/>
         <v>3</v>
       </c>
-      <c r="X42" s="2" t="str">
+      <c r="X42" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:10::/112</v>
       </c>
-      <c r="Y42" s="2" t="str">
+      <c r="Y42" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:10::4</v>
       </c>
-      <c r="Z42" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA42" s="2" t="str">
+      <c r="Z42" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA42" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:10::1</v>
       </c>
     </row>
     <row r="43" spans="11:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T43" s="2">
+      <c r="T43" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U43" s="2">
+      <c r="U43" s="5">
         <f t="shared" si="18"/>
         <v>9</v>
       </c>
-      <c r="V43" s="2" t="str">
+      <c r="V43" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-91</v>
       </c>
-      <c r="W43" s="2">
+      <c r="W43" s="5">
         <f t="shared" si="19"/>
         <v>4</v>
       </c>
-      <c r="X43" s="2" t="str">
+      <c r="X43" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:10::/112</v>
       </c>
-      <c r="Y43" s="2" t="str">
+      <c r="Y43" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:10::5</v>
       </c>
-      <c r="Z43" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA43" s="2" t="str">
+      <c r="Z43" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA43" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:10::1</v>
       </c>
     </row>
     <row r="44" spans="11:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T44" s="2">
+      <c r="T44" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U44" s="2">
+      <c r="U44" s="5">
         <f t="shared" si="18"/>
         <v>10</v>
       </c>
-      <c r="V44" s="2" t="str">
+      <c r="V44" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-92</v>
       </c>
-      <c r="W44" s="2">
+      <c r="W44" s="5">
         <f t="shared" si="19"/>
         <v>1</v>
       </c>
-      <c r="X44" s="2" t="str">
+      <c r="X44" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:11::/112</v>
       </c>
-      <c r="Y44" s="2" t="str">
+      <c r="Y44" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:11::2</v>
       </c>
-      <c r="Z44" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA44" s="2" t="str">
+      <c r="Z44" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA44" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:11::1</v>
       </c>
     </row>
     <row r="45" spans="11:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T45" s="2">
+      <c r="T45" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U45" s="2">
+      <c r="U45" s="5">
         <f t="shared" si="18"/>
         <v>10</v>
       </c>
-      <c r="V45" s="2" t="str">
+      <c r="V45" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-93</v>
       </c>
-      <c r="W45" s="2">
+      <c r="W45" s="5">
         <f t="shared" si="19"/>
         <v>2</v>
       </c>
-      <c r="X45" s="2" t="str">
+      <c r="X45" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:11::/112</v>
       </c>
-      <c r="Y45" s="2" t="str">
+      <c r="Y45" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:11::3</v>
       </c>
-      <c r="Z45" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA45" s="2" t="str">
+      <c r="Z45" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA45" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:11::1</v>
       </c>
     </row>
     <row r="46" spans="11:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T46" s="2">
+      <c r="T46" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U46" s="2">
+      <c r="U46" s="5">
         <f t="shared" si="18"/>
         <v>10</v>
       </c>
-      <c r="V46" s="2" t="str">
+      <c r="V46" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-94</v>
       </c>
-      <c r="W46" s="2">
+      <c r="W46" s="5">
         <f t="shared" si="19"/>
         <v>3</v>
       </c>
-      <c r="X46" s="2" t="str">
+      <c r="X46" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:11::/112</v>
       </c>
-      <c r="Y46" s="2" t="str">
+      <c r="Y46" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:11::4</v>
       </c>
-      <c r="Z46" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA46" s="2" t="str">
+      <c r="Z46" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA46" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:11::1</v>
       </c>
     </row>
     <row r="47" spans="11:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T47" s="2">
+      <c r="T47" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U47" s="2">
+      <c r="U47" s="5">
         <f t="shared" si="18"/>
         <v>10</v>
       </c>
-      <c r="V47" s="2" t="str">
+      <c r="V47" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-95</v>
       </c>
-      <c r="W47" s="2">
+      <c r="W47" s="5">
         <f t="shared" si="19"/>
         <v>4</v>
       </c>
-      <c r="X47" s="2" t="str">
+      <c r="X47" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:11::/112</v>
       </c>
-      <c r="Y47" s="2" t="str">
+      <c r="Y47" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:11::5</v>
       </c>
-      <c r="Z47" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA47" s="2" t="str">
+      <c r="Z47" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA47" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:11::1</v>
       </c>
     </row>
     <row r="48" spans="11:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T48" s="2">
+      <c r="T48" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U48" s="2">
+      <c r="U48" s="5">
         <f t="shared" si="18"/>
         <v>11</v>
       </c>
-      <c r="V48" s="2" t="str">
+      <c r="V48" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-96</v>
       </c>
-      <c r="W48" s="2">
+      <c r="W48" s="5">
         <f t="shared" si="19"/>
         <v>1</v>
       </c>
-      <c r="X48" s="2" t="str">
+      <c r="X48" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:12::/112</v>
       </c>
-      <c r="Y48" s="2" t="str">
+      <c r="Y48" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:12::2</v>
       </c>
-      <c r="Z48" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA48" s="2" t="str">
+      <c r="Z48" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA48" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:12::1</v>
       </c>
     </row>
     <row r="49" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T49" s="2">
+      <c r="T49" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U49" s="2">
+      <c r="U49" s="5">
         <f t="shared" si="18"/>
         <v>11</v>
       </c>
-      <c r="V49" s="2" t="str">
+      <c r="V49" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-97</v>
       </c>
-      <c r="W49" s="2">
+      <c r="W49" s="5">
         <f t="shared" si="19"/>
         <v>2</v>
       </c>
-      <c r="X49" s="2" t="str">
+      <c r="X49" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:12::/112</v>
       </c>
-      <c r="Y49" s="2" t="str">
+      <c r="Y49" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:12::3</v>
       </c>
-      <c r="Z49" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA49" s="2" t="str">
+      <c r="Z49" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA49" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:12::1</v>
       </c>
     </row>
     <row r="50" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T50" s="2">
+      <c r="T50" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U50" s="2">
+      <c r="U50" s="5">
         <f t="shared" si="18"/>
         <v>11</v>
       </c>
-      <c r="V50" s="2" t="str">
+      <c r="V50" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-98</v>
       </c>
-      <c r="W50" s="2">
+      <c r="W50" s="5">
         <f t="shared" si="19"/>
         <v>3</v>
       </c>
-      <c r="X50" s="2" t="str">
+      <c r="X50" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:12::/112</v>
       </c>
-      <c r="Y50" s="2" t="str">
+      <c r="Y50" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:12::4</v>
       </c>
-      <c r="Z50" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA50" s="2" t="str">
+      <c r="Z50" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA50" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:12::1</v>
       </c>
     </row>
     <row r="51" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T51" s="2">
+      <c r="T51" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U51" s="2">
+      <c r="U51" s="5">
         <f t="shared" si="18"/>
         <v>11</v>
       </c>
-      <c r="V51" s="2" t="str">
+      <c r="V51" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-99</v>
       </c>
-      <c r="W51" s="2">
+      <c r="W51" s="5">
         <f t="shared" si="19"/>
         <v>4</v>
       </c>
-      <c r="X51" s="2" t="str">
+      <c r="X51" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:12::/112</v>
       </c>
-      <c r="Y51" s="2" t="str">
+      <c r="Y51" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:12::5</v>
       </c>
-      <c r="Z51" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA51" s="2" t="str">
+      <c r="Z51" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA51" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:12::1</v>
       </c>
     </row>
     <row r="52" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T52" s="2">
+      <c r="T52" s="5">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U52" s="2">
+      <c r="U52" s="5">
         <f t="shared" si="18"/>
         <v>12</v>
       </c>
-      <c r="V52" s="2" t="str">
+      <c r="V52" s="5" t="str">
         <f t="shared" si="13"/>
         <v>PC-100</v>
       </c>
-      <c r="W52" s="2">
+      <c r="W52" s="5">
         <f t="shared" si="19"/>
         <v>1</v>
       </c>
-      <c r="X52" s="2" t="str">
+      <c r="X52" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:13::/112</v>
       </c>
-      <c r="Y52" s="2" t="str">
+      <c r="Y52" s="5" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:13::2</v>
       </c>
-      <c r="Z52" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA52" s="2" t="str">
+      <c r="Z52" s="5">
+        <v>112</v>
+      </c>
+      <c r="AA52" s="5" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:13::1</v>
       </c>

</xml_diff>

<commit_message>
Agregadas ip hasta el ultimo piso SOLO EN PC
</commit_message>
<xml_diff>
--- a/taller-2/Taller#2.xlsx
+++ b/taller-2/Taller#2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivanbotero/Projects/interconexion/taller-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3CE08B3-93FD-B442-86BF-C2E71CC4758A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF75C1F5-4940-F949-ABE4-DF50AB5D474E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -219,11 +219,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -575,36 +575,36 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:27" ht="18" x14ac:dyDescent="0.2">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="K2" s="4" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="K2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="T2" s="4" t="s">
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="T2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="4"/>
-      <c r="Z2" s="4"/>
-      <c r="AA2" s="4"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="5"/>
     </row>
     <row r="3" spans="2:27" ht="16" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
@@ -5314,8 +5314,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B2:AA127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P40" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="S51" sqref="S51"/>
+    <sheetView tabSelected="1" topLeftCell="R70" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="T85" sqref="T85:AA87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5347,36 +5347,36 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:27" ht="18" x14ac:dyDescent="0.2">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="K2" s="4" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="K2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="T2" s="4" t="s">
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="T2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="4"/>
-      <c r="Z2" s="4"/>
-      <c r="AA2" s="4"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="5"/>
     </row>
     <row r="3" spans="2:27" ht="16" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
@@ -5480,59 +5480,59 @@
         <f>_xlfn.CONCAT("2001:",B4,":",C4+1,"::1")</f>
         <v>2001:1:1::1</v>
       </c>
-      <c r="K4" s="5">
-        <v>2</v>
-      </c>
-      <c r="L4" s="5">
+      <c r="K4" s="4">
+        <v>2</v>
+      </c>
+      <c r="L4" s="4">
         <v>0</v>
       </c>
-      <c r="M4" s="5" t="str">
+      <c r="M4" s="4" t="str">
         <f>_xlfn.CONCAT("PC-",MID(D27,FIND("-",D27)+ 1, LEN(D27))+1)</f>
         <v>PC-24</v>
       </c>
-      <c r="N4" s="5">
-        <v>1</v>
-      </c>
-      <c r="O4" s="5" t="str">
+      <c r="N4" s="4">
+        <v>1</v>
+      </c>
+      <c r="O4" s="4" t="str">
         <f>_xlfn.CONCAT("2001:",K4,":",L4 + 1,"::/112")</f>
         <v>2001:2:1::/112</v>
       </c>
-      <c r="P4" s="5" t="str">
+      <c r="P4" s="4" t="str">
         <f>_xlfn.CONCAT("2001:",K4,":",L4+1,"::",N4 + 1)</f>
         <v>2001:2:1::2</v>
       </c>
-      <c r="Q4" s="5">
-        <v>112</v>
-      </c>
-      <c r="R4" s="5" t="str">
+      <c r="Q4" s="4">
+        <v>112</v>
+      </c>
+      <c r="R4" s="4" t="str">
         <f>_xlfn.CONCAT("2001:",K4,":",L4+1,"::1")</f>
         <v>2001:2:1::1</v>
       </c>
-      <c r="T4" s="5">
-        <v>3</v>
-      </c>
-      <c r="U4" s="5">
+      <c r="T4" s="4">
+        <v>3</v>
+      </c>
+      <c r="U4" s="4">
         <v>0</v>
       </c>
-      <c r="V4" s="5" t="str">
+      <c r="V4" s="4" t="str">
         <f>_xlfn.CONCAT("PC-",MID(M31,FIND("-",M31)+ 1, LEN(M31))+1)</f>
         <v>PC-52</v>
       </c>
-      <c r="W4" s="5">
-        <v>1</v>
-      </c>
-      <c r="X4" s="5" t="str">
+      <c r="W4" s="4">
+        <v>1</v>
+      </c>
+      <c r="X4" s="4" t="str">
         <f>_xlfn.CONCAT("2001:",T4,":",U4 + 1,"::/112")</f>
         <v>2001:3:1::/112</v>
       </c>
-      <c r="Y4" s="5" t="str">
+      <c r="Y4" s="4" t="str">
         <f>_xlfn.CONCAT("2001:",T4,":",U4+1,"::",W4 + 1)</f>
         <v>2001:3:1::2</v>
       </c>
-      <c r="Z4" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA4" s="5" t="str">
+      <c r="Z4" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA4" s="4" t="str">
         <f>_xlfn.CONCAT("2001:",T4,":",U4+1,"::1")</f>
         <v>2001:3:1::1</v>
       </c>
@@ -5566,61 +5566,61 @@
         <f t="shared" ref="I5:I27" si="2">_xlfn.CONCAT("2001:",B5,":",C5+1,"::1")</f>
         <v>2001:1:1::1</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="4">
         <f>K4</f>
         <v>2</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="4">
         <v>0</v>
       </c>
-      <c r="M5" s="5" t="str">
+      <c r="M5" s="4" t="str">
         <f>_xlfn.CONCAT("PC-",MID(M4,FIND("-",M4)+ 1, LEN(M4))+1)</f>
         <v>PC-25</v>
       </c>
-      <c r="N5" s="5">
-        <v>2</v>
-      </c>
-      <c r="O5" s="5" t="str">
+      <c r="N5" s="4">
+        <v>2</v>
+      </c>
+      <c r="O5" s="4" t="str">
         <f t="shared" ref="O5:O31" si="3">_xlfn.CONCAT("2001:",K5,":",L5 + 1,"::/112")</f>
         <v>2001:2:1::/112</v>
       </c>
-      <c r="P5" s="5" t="str">
+      <c r="P5" s="4" t="str">
         <f t="shared" ref="P5:P31" si="4">_xlfn.CONCAT("2001:",K5,":",L5+1,"::",N5 + 1)</f>
         <v>2001:2:1::3</v>
       </c>
-      <c r="Q5" s="5">
-        <v>112</v>
-      </c>
-      <c r="R5" s="5" t="str">
+      <c r="Q5" s="4">
+        <v>112</v>
+      </c>
+      <c r="R5" s="4" t="str">
         <f t="shared" ref="R5:R31" si="5">_xlfn.CONCAT("2001:",K5,":",L5+1,"::1")</f>
         <v>2001:2:1::1</v>
       </c>
-      <c r="T5" s="5">
+      <c r="T5" s="4">
         <f>T4</f>
         <v>3</v>
       </c>
-      <c r="U5" s="5">
+      <c r="U5" s="4">
         <v>0</v>
       </c>
-      <c r="V5" s="5" t="str">
+      <c r="V5" s="4" t="str">
         <f>_xlfn.CONCAT("PC-",MID(V4,FIND("-",V4)+ 1, LEN(V4))+1)</f>
         <v>PC-53</v>
       </c>
-      <c r="W5" s="5">
-        <v>2</v>
-      </c>
-      <c r="X5" s="5" t="str">
+      <c r="W5" s="4">
+        <v>2</v>
+      </c>
+      <c r="X5" s="4" t="str">
         <f t="shared" ref="X5:X68" si="6">_xlfn.CONCAT("2001:",T5,":",U5 + 1,"::/112")</f>
         <v>2001:3:1::/112</v>
       </c>
-      <c r="Y5" s="5" t="str">
+      <c r="Y5" s="4" t="str">
         <f t="shared" ref="Y5:Y68" si="7">_xlfn.CONCAT("2001:",T5,":",U5+1,"::",W5 + 1)</f>
         <v>2001:3:1::3</v>
       </c>
-      <c r="Z5" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA5" s="5" t="str">
+      <c r="Z5" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA5" s="4" t="str">
         <f t="shared" ref="AA5:AA68" si="8">_xlfn.CONCAT("2001:",T5,":",U5+1,"::1")</f>
         <v>2001:3:1::1</v>
       </c>
@@ -5654,61 +5654,61 @@
         <f t="shared" si="2"/>
         <v>2001:1:1::1</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="4">
         <f t="shared" ref="K6:K31" si="10">K5</f>
         <v>2</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6" s="4">
         <v>0</v>
       </c>
-      <c r="M6" s="5" t="str">
+      <c r="M6" s="4" t="str">
         <f t="shared" ref="M6:M31" si="11">_xlfn.CONCAT("PC-",MID(M5,FIND("-",M5)+ 1, LEN(M5))+1)</f>
         <v>PC-26</v>
       </c>
-      <c r="N6" s="5">
-        <v>3</v>
-      </c>
-      <c r="O6" s="5" t="str">
+      <c r="N6" s="4">
+        <v>3</v>
+      </c>
+      <c r="O6" s="4" t="str">
         <f t="shared" si="3"/>
         <v>2001:2:1::/112</v>
       </c>
-      <c r="P6" s="5" t="str">
+      <c r="P6" s="4" t="str">
         <f t="shared" si="4"/>
         <v>2001:2:1::4</v>
       </c>
-      <c r="Q6" s="5">
-        <v>112</v>
-      </c>
-      <c r="R6" s="5" t="str">
+      <c r="Q6" s="4">
+        <v>112</v>
+      </c>
+      <c r="R6" s="4" t="str">
         <f t="shared" si="5"/>
         <v>2001:2:1::1</v>
       </c>
-      <c r="T6" s="5">
+      <c r="T6" s="4">
         <f t="shared" ref="T6:T69" si="12">T5</f>
         <v>3</v>
       </c>
-      <c r="U6" s="5">
+      <c r="U6" s="4">
         <v>0</v>
       </c>
-      <c r="V6" s="5" t="str">
+      <c r="V6" s="4" t="str">
         <f t="shared" ref="V6:V69" si="13">_xlfn.CONCAT("PC-",MID(V5,FIND("-",V5)+ 1, LEN(V5))+1)</f>
         <v>PC-54</v>
       </c>
-      <c r="W6" s="5">
-        <v>3</v>
-      </c>
-      <c r="X6" s="5" t="str">
+      <c r="W6" s="4">
+        <v>3</v>
+      </c>
+      <c r="X6" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:1::/112</v>
       </c>
-      <c r="Y6" s="5" t="str">
+      <c r="Y6" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:1::4</v>
       </c>
-      <c r="Z6" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA6" s="5" t="str">
+      <c r="Z6" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA6" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:1::1</v>
       </c>
@@ -5742,61 +5742,61 @@
         <f t="shared" si="2"/>
         <v>2001:1:1::1</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7" s="4">
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="L7" s="5">
+      <c r="L7" s="4">
         <v>0</v>
       </c>
-      <c r="M7" s="5" t="str">
+      <c r="M7" s="4" t="str">
         <f t="shared" si="11"/>
         <v>PC-27</v>
       </c>
-      <c r="N7" s="5">
+      <c r="N7" s="4">
         <v>4</v>
       </c>
-      <c r="O7" s="5" t="str">
+      <c r="O7" s="4" t="str">
         <f t="shared" si="3"/>
         <v>2001:2:1::/112</v>
       </c>
-      <c r="P7" s="5" t="str">
+      <c r="P7" s="4" t="str">
         <f t="shared" si="4"/>
         <v>2001:2:1::5</v>
       </c>
-      <c r="Q7" s="5">
-        <v>112</v>
-      </c>
-      <c r="R7" s="5" t="str">
+      <c r="Q7" s="4">
+        <v>112</v>
+      </c>
+      <c r="R7" s="4" t="str">
         <f t="shared" si="5"/>
         <v>2001:2:1::1</v>
       </c>
-      <c r="T7" s="5">
+      <c r="T7" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U7" s="5">
+      <c r="U7" s="4">
         <v>0</v>
       </c>
-      <c r="V7" s="5" t="str">
+      <c r="V7" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-55</v>
       </c>
-      <c r="W7" s="5">
+      <c r="W7" s="4">
         <v>4</v>
       </c>
-      <c r="X7" s="5" t="str">
+      <c r="X7" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:1::/112</v>
       </c>
-      <c r="Y7" s="5" t="str">
+      <c r="Y7" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:1::5</v>
       </c>
-      <c r="Z7" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA7" s="5" t="str">
+      <c r="Z7" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA7" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:1::1</v>
       </c>
@@ -5863,34 +5863,34 @@
         <f t="shared" si="5"/>
         <v>2001:2:2::1</v>
       </c>
-      <c r="T8" s="5">
+      <c r="T8" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U8" s="5">
+      <c r="U8" s="4">
         <f>U4+1</f>
         <v>1</v>
       </c>
-      <c r="V8" s="5" t="str">
+      <c r="V8" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-56</v>
       </c>
-      <c r="W8" s="5">
+      <c r="W8" s="4">
         <f>W4</f>
         <v>1</v>
       </c>
-      <c r="X8" s="5" t="str">
+      <c r="X8" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:2::/112</v>
       </c>
-      <c r="Y8" s="5" t="str">
+      <c r="Y8" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:2::2</v>
       </c>
-      <c r="Z8" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA8" s="5" t="str">
+      <c r="Z8" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA8" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:2::1</v>
       </c>
@@ -5957,34 +5957,34 @@
         <f t="shared" si="5"/>
         <v>2001:2:2::1</v>
       </c>
-      <c r="T9" s="5">
+      <c r="T9" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U9" s="5">
+      <c r="U9" s="4">
         <f t="shared" ref="U9:U72" si="18">U5+1</f>
         <v>1</v>
       </c>
-      <c r="V9" s="5" t="str">
+      <c r="V9" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-57</v>
       </c>
-      <c r="W9" s="5">
+      <c r="W9" s="4">
         <f t="shared" ref="W9:W72" si="19">W5</f>
         <v>2</v>
       </c>
-      <c r="X9" s="5" t="str">
+      <c r="X9" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:2::/112</v>
       </c>
-      <c r="Y9" s="5" t="str">
+      <c r="Y9" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:2::3</v>
       </c>
-      <c r="Z9" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA9" s="5" t="str">
+      <c r="Z9" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA9" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:2::1</v>
       </c>
@@ -6051,34 +6051,34 @@
         <f t="shared" si="5"/>
         <v>2001:2:2::1</v>
       </c>
-      <c r="T10" s="5">
+      <c r="T10" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U10" s="5">
+      <c r="U10" s="4">
         <f t="shared" si="18"/>
         <v>1</v>
       </c>
-      <c r="V10" s="5" t="str">
+      <c r="V10" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-58</v>
       </c>
-      <c r="W10" s="5">
+      <c r="W10" s="4">
         <f t="shared" si="19"/>
         <v>3</v>
       </c>
-      <c r="X10" s="5" t="str">
+      <c r="X10" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:2::/112</v>
       </c>
-      <c r="Y10" s="5" t="str">
+      <c r="Y10" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:2::4</v>
       </c>
-      <c r="Z10" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA10" s="5" t="str">
+      <c r="Z10" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA10" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:2::1</v>
       </c>
@@ -6145,34 +6145,34 @@
         <f t="shared" si="5"/>
         <v>2001:2:2::1</v>
       </c>
-      <c r="T11" s="5">
+      <c r="T11" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U11" s="5">
+      <c r="U11" s="4">
         <f t="shared" si="18"/>
         <v>1</v>
       </c>
-      <c r="V11" s="5" t="str">
+      <c r="V11" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-59</v>
       </c>
-      <c r="W11" s="5">
+      <c r="W11" s="4">
         <f t="shared" si="19"/>
         <v>4</v>
       </c>
-      <c r="X11" s="5" t="str">
+      <c r="X11" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:2::/112</v>
       </c>
-      <c r="Y11" s="5" t="str">
+      <c r="Y11" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:2::5</v>
       </c>
-      <c r="Z11" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA11" s="5" t="str">
+      <c r="Z11" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA11" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:2::1</v>
       </c>
@@ -6239,34 +6239,34 @@
         <f t="shared" si="5"/>
         <v>2001:2:3::1</v>
       </c>
-      <c r="T12" s="5">
+      <c r="T12" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U12" s="5">
+      <c r="U12" s="4">
         <f>U8+1</f>
         <v>2</v>
       </c>
-      <c r="V12" s="5" t="str">
+      <c r="V12" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-60</v>
       </c>
-      <c r="W12" s="5">
+      <c r="W12" s="4">
         <f t="shared" si="19"/>
         <v>1</v>
       </c>
-      <c r="X12" s="5" t="str">
+      <c r="X12" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:3::/112</v>
       </c>
-      <c r="Y12" s="5" t="str">
+      <c r="Y12" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:3::2</v>
       </c>
-      <c r="Z12" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA12" s="5" t="str">
+      <c r="Z12" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA12" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:3::1</v>
       </c>
@@ -6333,34 +6333,34 @@
         <f t="shared" si="5"/>
         <v>2001:2:3::1</v>
       </c>
-      <c r="T13" s="5">
+      <c r="T13" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U13" s="5">
+      <c r="U13" s="4">
         <f t="shared" si="18"/>
         <v>2</v>
       </c>
-      <c r="V13" s="5" t="str">
+      <c r="V13" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-61</v>
       </c>
-      <c r="W13" s="5">
+      <c r="W13" s="4">
         <f t="shared" si="19"/>
         <v>2</v>
       </c>
-      <c r="X13" s="5" t="str">
+      <c r="X13" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:3::/112</v>
       </c>
-      <c r="Y13" s="5" t="str">
+      <c r="Y13" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:3::3</v>
       </c>
-      <c r="Z13" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA13" s="5" t="str">
+      <c r="Z13" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA13" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:3::1</v>
       </c>
@@ -6427,34 +6427,34 @@
         <f t="shared" si="5"/>
         <v>2001:2:3::1</v>
       </c>
-      <c r="T14" s="5">
+      <c r="T14" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U14" s="5">
+      <c r="U14" s="4">
         <f t="shared" si="18"/>
         <v>2</v>
       </c>
-      <c r="V14" s="5" t="str">
+      <c r="V14" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-62</v>
       </c>
-      <c r="W14" s="5">
+      <c r="W14" s="4">
         <f t="shared" si="19"/>
         <v>3</v>
       </c>
-      <c r="X14" s="5" t="str">
+      <c r="X14" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:3::/112</v>
       </c>
-      <c r="Y14" s="5" t="str">
+      <c r="Y14" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:3::4</v>
       </c>
-      <c r="Z14" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA14" s="5" t="str">
+      <c r="Z14" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA14" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:3::1</v>
       </c>
@@ -6521,34 +6521,34 @@
         <f t="shared" si="5"/>
         <v>2001:2:3::1</v>
       </c>
-      <c r="T15" s="5">
+      <c r="T15" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U15" s="5">
+      <c r="U15" s="4">
         <f t="shared" si="18"/>
         <v>2</v>
       </c>
-      <c r="V15" s="5" t="str">
+      <c r="V15" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-63</v>
       </c>
-      <c r="W15" s="5">
+      <c r="W15" s="4">
         <f t="shared" si="19"/>
         <v>4</v>
       </c>
-      <c r="X15" s="5" t="str">
+      <c r="X15" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:3::/112</v>
       </c>
-      <c r="Y15" s="5" t="str">
+      <c r="Y15" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:3::5</v>
       </c>
-      <c r="Z15" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA15" s="5" t="str">
+      <c r="Z15" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA15" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:3::1</v>
       </c>
@@ -6615,34 +6615,34 @@
         <f t="shared" si="5"/>
         <v>2001:2:4::1</v>
       </c>
-      <c r="T16" s="5">
+      <c r="T16" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U16" s="5">
+      <c r="U16" s="4">
         <f>U12+1</f>
         <v>3</v>
       </c>
-      <c r="V16" s="5" t="str">
+      <c r="V16" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-64</v>
       </c>
-      <c r="W16" s="5">
+      <c r="W16" s="4">
         <f t="shared" si="19"/>
         <v>1</v>
       </c>
-      <c r="X16" s="5" t="str">
+      <c r="X16" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:4::/112</v>
       </c>
-      <c r="Y16" s="5" t="str">
+      <c r="Y16" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:4::2</v>
       </c>
-      <c r="Z16" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA16" s="5" t="str">
+      <c r="Z16" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA16" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:4::1</v>
       </c>
@@ -6709,34 +6709,34 @@
         <f t="shared" si="5"/>
         <v>2001:2:4::1</v>
       </c>
-      <c r="T17" s="5">
+      <c r="T17" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U17" s="5">
+      <c r="U17" s="4">
         <f t="shared" si="18"/>
         <v>3</v>
       </c>
-      <c r="V17" s="5" t="str">
+      <c r="V17" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-65</v>
       </c>
-      <c r="W17" s="5">
+      <c r="W17" s="4">
         <f t="shared" si="19"/>
         <v>2</v>
       </c>
-      <c r="X17" s="5" t="str">
+      <c r="X17" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:4::/112</v>
       </c>
-      <c r="Y17" s="5" t="str">
+      <c r="Y17" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:4::3</v>
       </c>
-      <c r="Z17" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA17" s="5" t="str">
+      <c r="Z17" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA17" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:4::1</v>
       </c>
@@ -6803,34 +6803,34 @@
         <f t="shared" si="5"/>
         <v>2001:2:4::1</v>
       </c>
-      <c r="T18" s="5">
+      <c r="T18" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U18" s="5">
+      <c r="U18" s="4">
         <f t="shared" si="18"/>
         <v>3</v>
       </c>
-      <c r="V18" s="5" t="str">
+      <c r="V18" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-66</v>
       </c>
-      <c r="W18" s="5">
+      <c r="W18" s="4">
         <f t="shared" si="19"/>
         <v>3</v>
       </c>
-      <c r="X18" s="5" t="str">
+      <c r="X18" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:4::/112</v>
       </c>
-      <c r="Y18" s="5" t="str">
+      <c r="Y18" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:4::4</v>
       </c>
-      <c r="Z18" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA18" s="5" t="str">
+      <c r="Z18" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA18" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:4::1</v>
       </c>
@@ -6897,34 +6897,34 @@
         <f t="shared" si="5"/>
         <v>2001:2:4::1</v>
       </c>
-      <c r="T19" s="5">
+      <c r="T19" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U19" s="5">
+      <c r="U19" s="4">
         <f t="shared" si="18"/>
         <v>3</v>
       </c>
-      <c r="V19" s="5" t="str">
+      <c r="V19" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-67</v>
       </c>
-      <c r="W19" s="5">
+      <c r="W19" s="4">
         <f t="shared" si="19"/>
         <v>4</v>
       </c>
-      <c r="X19" s="5" t="str">
+      <c r="X19" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:4::/112</v>
       </c>
-      <c r="Y19" s="5" t="str">
+      <c r="Y19" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:4::5</v>
       </c>
-      <c r="Z19" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA19" s="5" t="str">
+      <c r="Z19" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA19" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:4::1</v>
       </c>
@@ -6991,34 +6991,34 @@
         <f t="shared" si="5"/>
         <v>2001:2:5::1</v>
       </c>
-      <c r="T20" s="5">
+      <c r="T20" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U20" s="5">
+      <c r="U20" s="4">
         <f>U16+1</f>
         <v>4</v>
       </c>
-      <c r="V20" s="5" t="str">
+      <c r="V20" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-68</v>
       </c>
-      <c r="W20" s="5">
+      <c r="W20" s="4">
         <f t="shared" si="19"/>
         <v>1</v>
       </c>
-      <c r="X20" s="5" t="str">
+      <c r="X20" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:5::/112</v>
       </c>
-      <c r="Y20" s="5" t="str">
+      <c r="Y20" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:5::2</v>
       </c>
-      <c r="Z20" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA20" s="5" t="str">
+      <c r="Z20" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA20" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:5::1</v>
       </c>
@@ -7085,34 +7085,34 @@
         <f t="shared" si="5"/>
         <v>2001:2:5::1</v>
       </c>
-      <c r="T21" s="5">
+      <c r="T21" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U21" s="5">
+      <c r="U21" s="4">
         <f t="shared" si="18"/>
         <v>4</v>
       </c>
-      <c r="V21" s="5" t="str">
+      <c r="V21" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-69</v>
       </c>
-      <c r="W21" s="5">
+      <c r="W21" s="4">
         <f t="shared" si="19"/>
         <v>2</v>
       </c>
-      <c r="X21" s="5" t="str">
+      <c r="X21" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:5::/112</v>
       </c>
-      <c r="Y21" s="5" t="str">
+      <c r="Y21" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:5::3</v>
       </c>
-      <c r="Z21" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA21" s="5" t="str">
+      <c r="Z21" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA21" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:5::1</v>
       </c>
@@ -7179,34 +7179,34 @@
         <f t="shared" si="5"/>
         <v>2001:2:5::1</v>
       </c>
-      <c r="T22" s="5">
+      <c r="T22" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U22" s="5">
+      <c r="U22" s="4">
         <f t="shared" si="18"/>
         <v>4</v>
       </c>
-      <c r="V22" s="5" t="str">
+      <c r="V22" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-70</v>
       </c>
-      <c r="W22" s="5">
+      <c r="W22" s="4">
         <f t="shared" si="19"/>
         <v>3</v>
       </c>
-      <c r="X22" s="5" t="str">
+      <c r="X22" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:5::/112</v>
       </c>
-      <c r="Y22" s="5" t="str">
+      <c r="Y22" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:5::4</v>
       </c>
-      <c r="Z22" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA22" s="5" t="str">
+      <c r="Z22" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA22" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:5::1</v>
       </c>
@@ -7273,66 +7273,66 @@
         <f t="shared" si="5"/>
         <v>2001:2:5::1</v>
       </c>
-      <c r="T23" s="5">
+      <c r="T23" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U23" s="5">
+      <c r="U23" s="4">
         <f>U19+1</f>
         <v>4</v>
       </c>
-      <c r="V23" s="5" t="str">
+      <c r="V23" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-71</v>
       </c>
-      <c r="W23" s="5">
+      <c r="W23" s="4">
         <f t="shared" si="19"/>
         <v>4</v>
       </c>
-      <c r="X23" s="5" t="str">
+      <c r="X23" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:5::/112</v>
       </c>
-      <c r="Y23" s="5" t="str">
+      <c r="Y23" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:5::5</v>
       </c>
-      <c r="Z23" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA23" s="5" t="str">
+      <c r="Z23" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA23" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:5::1</v>
       </c>
     </row>
     <row r="24" spans="2:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="B24" s="5">
+      <c r="B24" s="4">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="4">
         <f t="shared" si="14"/>
         <v>5</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="4">
         <f t="shared" si="15"/>
         <v>1</v>
       </c>
-      <c r="F24" s="5" t="str">
+      <c r="F24" s="4" t="str">
         <f t="shared" si="0"/>
         <v>2001:1:6::/112</v>
       </c>
-      <c r="G24" s="5" t="str">
+      <c r="G24" s="4" t="str">
         <f t="shared" si="1"/>
         <v>2001:1:6::2</v>
       </c>
-      <c r="H24" s="5">
-        <v>112</v>
-      </c>
-      <c r="I24" s="5" t="str">
+      <c r="H24" s="4">
+        <v>112</v>
+      </c>
+      <c r="I24" s="4" t="str">
         <f t="shared" si="2"/>
         <v>2001:1:6::1</v>
       </c>
@@ -7367,66 +7367,66 @@
         <f t="shared" si="5"/>
         <v>2001:2:6::1</v>
       </c>
-      <c r="T24" s="5">
+      <c r="T24" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U24" s="5">
+      <c r="U24" s="4">
         <f t="shared" si="18"/>
         <v>5</v>
       </c>
-      <c r="V24" s="5" t="str">
+      <c r="V24" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-72</v>
       </c>
-      <c r="W24" s="5">
+      <c r="W24" s="4">
         <f t="shared" si="19"/>
         <v>1</v>
       </c>
-      <c r="X24" s="5" t="str">
+      <c r="X24" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:6::/112</v>
       </c>
-      <c r="Y24" s="5" t="str">
+      <c r="Y24" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:6::2</v>
       </c>
-      <c r="Z24" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA24" s="5" t="str">
+      <c r="Z24" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA24" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:6::1</v>
       </c>
     </row>
     <row r="25" spans="2:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="B25" s="5">
+      <c r="B25" s="4">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="4">
         <f t="shared" si="14"/>
         <v>5</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25" s="4">
         <f t="shared" si="15"/>
         <v>2</v>
       </c>
-      <c r="F25" s="5" t="str">
+      <c r="F25" s="4" t="str">
         <f t="shared" si="0"/>
         <v>2001:1:6::/112</v>
       </c>
-      <c r="G25" s="5" t="str">
+      <c r="G25" s="4" t="str">
         <f t="shared" si="1"/>
         <v>2001:1:6::3</v>
       </c>
-      <c r="H25" s="5">
-        <v>112</v>
-      </c>
-      <c r="I25" s="5" t="str">
+      <c r="H25" s="4">
+        <v>112</v>
+      </c>
+      <c r="I25" s="4" t="str">
         <f t="shared" si="2"/>
         <v>2001:1:6::1</v>
       </c>
@@ -7461,66 +7461,66 @@
         <f t="shared" si="5"/>
         <v>2001:2:6::1</v>
       </c>
-      <c r="T25" s="5">
+      <c r="T25" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U25" s="5">
+      <c r="U25" s="4">
         <f t="shared" si="18"/>
         <v>5</v>
       </c>
-      <c r="V25" s="5" t="str">
+      <c r="V25" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-73</v>
       </c>
-      <c r="W25" s="5">
+      <c r="W25" s="4">
         <f t="shared" si="19"/>
         <v>2</v>
       </c>
-      <c r="X25" s="5" t="str">
+      <c r="X25" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:6::/112</v>
       </c>
-      <c r="Y25" s="5" t="str">
+      <c r="Y25" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:6::3</v>
       </c>
-      <c r="Z25" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA25" s="5" t="str">
+      <c r="Z25" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA25" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:6::1</v>
       </c>
     </row>
     <row r="26" spans="2:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="B26" s="5">
+      <c r="B26" s="4">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="4">
         <f>C22+1</f>
         <v>5</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E26" s="4">
         <f t="shared" si="15"/>
         <v>3</v>
       </c>
-      <c r="F26" s="5" t="str">
+      <c r="F26" s="4" t="str">
         <f t="shared" si="0"/>
         <v>2001:1:6::/112</v>
       </c>
-      <c r="G26" s="5" t="str">
+      <c r="G26" s="4" t="str">
         <f t="shared" si="1"/>
         <v>2001:1:6::4</v>
       </c>
-      <c r="H26" s="5">
-        <v>112</v>
-      </c>
-      <c r="I26" s="5" t="str">
+      <c r="H26" s="4">
+        <v>112</v>
+      </c>
+      <c r="I26" s="4" t="str">
         <f t="shared" si="2"/>
         <v>2001:1:6::1</v>
       </c>
@@ -7555,66 +7555,66 @@
         <f t="shared" si="5"/>
         <v>2001:2:6::1</v>
       </c>
-      <c r="T26" s="5">
+      <c r="T26" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U26" s="5">
+      <c r="U26" s="4">
         <f>U22+1</f>
         <v>5</v>
       </c>
-      <c r="V26" s="5" t="str">
+      <c r="V26" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-74</v>
       </c>
-      <c r="W26" s="5">
+      <c r="W26" s="4">
         <f t="shared" si="19"/>
         <v>3</v>
       </c>
-      <c r="X26" s="5" t="str">
+      <c r="X26" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:6::/112</v>
       </c>
-      <c r="Y26" s="5" t="str">
+      <c r="Y26" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:6::4</v>
       </c>
-      <c r="Z26" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA26" s="5" t="str">
+      <c r="Z26" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA26" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:6::1</v>
       </c>
     </row>
     <row r="27" spans="2:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="B27" s="5">
+      <c r="B27" s="4">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C27" s="4">
         <f t="shared" si="14"/>
         <v>5</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E27" s="5">
+      <c r="E27" s="4">
         <f t="shared" si="15"/>
         <v>4</v>
       </c>
-      <c r="F27" s="5" t="str">
+      <c r="F27" s="4" t="str">
         <f t="shared" si="0"/>
         <v>2001:1:6::/112</v>
       </c>
-      <c r="G27" s="5" t="str">
+      <c r="G27" s="4" t="str">
         <f t="shared" si="1"/>
         <v>2001:1:6::5</v>
       </c>
-      <c r="H27" s="5">
-        <v>112</v>
-      </c>
-      <c r="I27" s="5" t="str">
+      <c r="H27" s="4">
+        <v>112</v>
+      </c>
+      <c r="I27" s="4" t="str">
         <f t="shared" si="2"/>
         <v>2001:1:6::1</v>
       </c>
@@ -7649,34 +7649,34 @@
         <f t="shared" si="5"/>
         <v>2001:2:6::1</v>
       </c>
-      <c r="T27" s="5">
+      <c r="T27" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U27" s="5">
+      <c r="U27" s="4">
         <f t="shared" si="18"/>
         <v>5</v>
       </c>
-      <c r="V27" s="5" t="str">
+      <c r="V27" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-75</v>
       </c>
-      <c r="W27" s="5">
+      <c r="W27" s="4">
         <f t="shared" si="19"/>
         <v>4</v>
       </c>
-      <c r="X27" s="5" t="str">
+      <c r="X27" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:6::/112</v>
       </c>
-      <c r="Y27" s="5" t="str">
+      <c r="Y27" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:6::5</v>
       </c>
-      <c r="Z27" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA27" s="5" t="str">
+      <c r="Z27" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA27" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:6::1</v>
       </c>
@@ -7713,34 +7713,34 @@
         <f t="shared" si="5"/>
         <v>2001:2:7::1</v>
       </c>
-      <c r="T28" s="5">
+      <c r="T28" s="4">
         <f>T27</f>
         <v>3</v>
       </c>
-      <c r="U28" s="5">
+      <c r="U28" s="4">
         <f t="shared" si="18"/>
         <v>6</v>
       </c>
-      <c r="V28" s="5" t="str">
+      <c r="V28" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-76</v>
       </c>
-      <c r="W28" s="5">
+      <c r="W28" s="4">
         <f t="shared" si="19"/>
         <v>1</v>
       </c>
-      <c r="X28" s="5" t="str">
+      <c r="X28" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:7::/112</v>
       </c>
-      <c r="Y28" s="5" t="str">
+      <c r="Y28" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:7::2</v>
       </c>
-      <c r="Z28" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA28" s="5" t="str">
+      <c r="Z28" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA28" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:7::1</v>
       </c>
@@ -7777,34 +7777,34 @@
         <f t="shared" si="5"/>
         <v>2001:2:7::1</v>
       </c>
-      <c r="T29" s="5">
+      <c r="T29" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U29" s="5">
+      <c r="U29" s="4">
         <f t="shared" si="18"/>
         <v>6</v>
       </c>
-      <c r="V29" s="5" t="str">
+      <c r="V29" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-77</v>
       </c>
-      <c r="W29" s="5">
+      <c r="W29" s="4">
         <f t="shared" si="19"/>
         <v>2</v>
       </c>
-      <c r="X29" s="5" t="str">
+      <c r="X29" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:7::/112</v>
       </c>
-      <c r="Y29" s="5" t="str">
+      <c r="Y29" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:7::3</v>
       </c>
-      <c r="Z29" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA29" s="5" t="str">
+      <c r="Z29" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA29" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:7::1</v>
       </c>
@@ -7841,34 +7841,34 @@
         <f t="shared" si="5"/>
         <v>2001:2:7::1</v>
       </c>
-      <c r="T30" s="5">
+      <c r="T30" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U30" s="5">
+      <c r="U30" s="4">
         <f t="shared" si="18"/>
         <v>6</v>
       </c>
-      <c r="V30" s="5" t="str">
+      <c r="V30" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-78</v>
       </c>
-      <c r="W30" s="5">
+      <c r="W30" s="4">
         <f t="shared" si="19"/>
         <v>3</v>
       </c>
-      <c r="X30" s="5" t="str">
+      <c r="X30" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:7::/112</v>
       </c>
-      <c r="Y30" s="5" t="str">
+      <c r="Y30" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:7::4</v>
       </c>
-      <c r="Z30" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA30" s="5" t="str">
+      <c r="Z30" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA30" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:7::1</v>
       </c>
@@ -7905,34 +7905,34 @@
         <f t="shared" si="5"/>
         <v>2001:2:7::1</v>
       </c>
-      <c r="T31" s="5">
+      <c r="T31" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U31" s="5">
+      <c r="U31" s="4">
         <f t="shared" si="18"/>
         <v>6</v>
       </c>
-      <c r="V31" s="5" t="str">
+      <c r="V31" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-79</v>
       </c>
-      <c r="W31" s="5">
+      <c r="W31" s="4">
         <f t="shared" si="19"/>
         <v>4</v>
       </c>
-      <c r="X31" s="5" t="str">
+      <c r="X31" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:7::/112</v>
       </c>
-      <c r="Y31" s="5" t="str">
+      <c r="Y31" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:7::5</v>
       </c>
-      <c r="Z31" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA31" s="5" t="str">
+      <c r="Z31" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA31" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:7::1</v>
       </c>
@@ -7946,34 +7946,34 @@
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
-      <c r="T32" s="5">
+      <c r="T32" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U32" s="5">
+      <c r="U32" s="4">
         <f t="shared" si="18"/>
         <v>7</v>
       </c>
-      <c r="V32" s="5" t="str">
+      <c r="V32" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-80</v>
       </c>
-      <c r="W32" s="5">
+      <c r="W32" s="4">
         <f t="shared" si="19"/>
         <v>1</v>
       </c>
-      <c r="X32" s="5" t="str">
+      <c r="X32" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:8::/112</v>
       </c>
-      <c r="Y32" s="5" t="str">
+      <c r="Y32" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:8::2</v>
       </c>
-      <c r="Z32" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA32" s="5" t="str">
+      <c r="Z32" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA32" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:8::1</v>
       </c>
@@ -7987,34 +7987,34 @@
       <c r="P33" s="2"/>
       <c r="Q33" s="2"/>
       <c r="R33" s="2"/>
-      <c r="T33" s="5">
+      <c r="T33" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U33" s="5">
+      <c r="U33" s="4">
         <f t="shared" si="18"/>
         <v>7</v>
       </c>
-      <c r="V33" s="5" t="str">
+      <c r="V33" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-81</v>
       </c>
-      <c r="W33" s="5">
+      <c r="W33" s="4">
         <f t="shared" si="19"/>
         <v>2</v>
       </c>
-      <c r="X33" s="5" t="str">
+      <c r="X33" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:8::/112</v>
       </c>
-      <c r="Y33" s="5" t="str">
+      <c r="Y33" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:8::3</v>
       </c>
-      <c r="Z33" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA33" s="5" t="str">
+      <c r="Z33" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA33" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:8::1</v>
       </c>
@@ -8028,34 +8028,34 @@
       <c r="P34" s="2"/>
       <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
-      <c r="T34" s="5">
+      <c r="T34" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U34" s="5">
+      <c r="U34" s="4">
         <f t="shared" si="18"/>
         <v>7</v>
       </c>
-      <c r="V34" s="5" t="str">
+      <c r="V34" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-82</v>
       </c>
-      <c r="W34" s="5">
+      <c r="W34" s="4">
         <f t="shared" si="19"/>
         <v>3</v>
       </c>
-      <c r="X34" s="5" t="str">
+      <c r="X34" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:8::/112</v>
       </c>
-      <c r="Y34" s="5" t="str">
+      <c r="Y34" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:8::4</v>
       </c>
-      <c r="Z34" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA34" s="5" t="str">
+      <c r="Z34" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA34" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:8::1</v>
       </c>
@@ -8069,1750 +8069,1750 @@
       <c r="P35" s="2"/>
       <c r="Q35" s="2"/>
       <c r="R35" s="2"/>
-      <c r="T35" s="5">
+      <c r="T35" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U35" s="5">
+      <c r="U35" s="4">
         <f t="shared" si="18"/>
         <v>7</v>
       </c>
-      <c r="V35" s="5" t="str">
+      <c r="V35" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-83</v>
       </c>
-      <c r="W35" s="5">
+      <c r="W35" s="4">
         <f t="shared" si="19"/>
         <v>4</v>
       </c>
-      <c r="X35" s="5" t="str">
+      <c r="X35" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:8::/112</v>
       </c>
-      <c r="Y35" s="5" t="str">
+      <c r="Y35" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:8::5</v>
       </c>
-      <c r="Z35" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA35" s="5" t="str">
+      <c r="Z35" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA35" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:8::1</v>
       </c>
     </row>
     <row r="36" spans="11:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T36" s="5">
+      <c r="T36" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U36" s="5">
+      <c r="U36" s="4">
         <f t="shared" si="18"/>
         <v>8</v>
       </c>
-      <c r="V36" s="5" t="str">
+      <c r="V36" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-84</v>
       </c>
-      <c r="W36" s="5">
+      <c r="W36" s="4">
         <f t="shared" si="19"/>
         <v>1</v>
       </c>
-      <c r="X36" s="5" t="str">
+      <c r="X36" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:9::/112</v>
       </c>
-      <c r="Y36" s="5" t="str">
+      <c r="Y36" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:9::2</v>
       </c>
-      <c r="Z36" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA36" s="5" t="str">
+      <c r="Z36" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA36" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:9::1</v>
       </c>
     </row>
     <row r="37" spans="11:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T37" s="5">
+      <c r="T37" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U37" s="5">
+      <c r="U37" s="4">
         <f t="shared" si="18"/>
         <v>8</v>
       </c>
-      <c r="V37" s="5" t="str">
+      <c r="V37" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-85</v>
       </c>
-      <c r="W37" s="5">
+      <c r="W37" s="4">
         <f t="shared" si="19"/>
         <v>2</v>
       </c>
-      <c r="X37" s="5" t="str">
+      <c r="X37" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:9::/112</v>
       </c>
-      <c r="Y37" s="5" t="str">
+      <c r="Y37" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:9::3</v>
       </c>
-      <c r="Z37" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA37" s="5" t="str">
+      <c r="Z37" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA37" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:9::1</v>
       </c>
     </row>
     <row r="38" spans="11:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T38" s="5">
+      <c r="T38" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U38" s="5">
+      <c r="U38" s="4">
         <f t="shared" si="18"/>
         <v>8</v>
       </c>
-      <c r="V38" s="5" t="str">
+      <c r="V38" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-86</v>
       </c>
-      <c r="W38" s="5">
+      <c r="W38" s="4">
         <f t="shared" si="19"/>
         <v>3</v>
       </c>
-      <c r="X38" s="5" t="str">
+      <c r="X38" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:9::/112</v>
       </c>
-      <c r="Y38" s="5" t="str">
+      <c r="Y38" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:9::4</v>
       </c>
-      <c r="Z38" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA38" s="5" t="str">
+      <c r="Z38" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA38" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:9::1</v>
       </c>
     </row>
     <row r="39" spans="11:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T39" s="5">
+      <c r="T39" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U39" s="5">
+      <c r="U39" s="4">
         <f t="shared" si="18"/>
         <v>8</v>
       </c>
-      <c r="V39" s="5" t="str">
+      <c r="V39" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-87</v>
       </c>
-      <c r="W39" s="5">
+      <c r="W39" s="4">
         <f t="shared" si="19"/>
         <v>4</v>
       </c>
-      <c r="X39" s="5" t="str">
+      <c r="X39" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:9::/112</v>
       </c>
-      <c r="Y39" s="5" t="str">
+      <c r="Y39" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:9::5</v>
       </c>
-      <c r="Z39" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA39" s="5" t="str">
+      <c r="Z39" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA39" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:9::1</v>
       </c>
     </row>
     <row r="40" spans="11:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T40" s="5">
+      <c r="T40" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U40" s="5">
+      <c r="U40" s="4">
         <f t="shared" si="18"/>
         <v>9</v>
       </c>
-      <c r="V40" s="5" t="str">
+      <c r="V40" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-88</v>
       </c>
-      <c r="W40" s="5">
+      <c r="W40" s="4">
         <f t="shared" si="19"/>
         <v>1</v>
       </c>
-      <c r="X40" s="5" t="str">
+      <c r="X40" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:10::/112</v>
       </c>
-      <c r="Y40" s="5" t="str">
+      <c r="Y40" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:10::2</v>
       </c>
-      <c r="Z40" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA40" s="5" t="str">
+      <c r="Z40" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA40" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:10::1</v>
       </c>
     </row>
     <row r="41" spans="11:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T41" s="5">
+      <c r="T41" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U41" s="5">
+      <c r="U41" s="4">
         <f t="shared" si="18"/>
         <v>9</v>
       </c>
-      <c r="V41" s="5" t="str">
+      <c r="V41" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-89</v>
       </c>
-      <c r="W41" s="5">
+      <c r="W41" s="4">
         <f t="shared" si="19"/>
         <v>2</v>
       </c>
-      <c r="X41" s="5" t="str">
+      <c r="X41" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:10::/112</v>
       </c>
-      <c r="Y41" s="5" t="str">
+      <c r="Y41" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:10::3</v>
       </c>
-      <c r="Z41" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA41" s="5" t="str">
+      <c r="Z41" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA41" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:10::1</v>
       </c>
     </row>
     <row r="42" spans="11:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T42" s="5">
+      <c r="T42" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U42" s="5">
+      <c r="U42" s="4">
         <f t="shared" si="18"/>
         <v>9</v>
       </c>
-      <c r="V42" s="5" t="str">
+      <c r="V42" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-90</v>
       </c>
-      <c r="W42" s="5">
+      <c r="W42" s="4">
         <f t="shared" si="19"/>
         <v>3</v>
       </c>
-      <c r="X42" s="5" t="str">
+      <c r="X42" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:10::/112</v>
       </c>
-      <c r="Y42" s="5" t="str">
+      <c r="Y42" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:10::4</v>
       </c>
-      <c r="Z42" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA42" s="5" t="str">
+      <c r="Z42" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA42" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:10::1</v>
       </c>
     </row>
     <row r="43" spans="11:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T43" s="5">
+      <c r="T43" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U43" s="5">
+      <c r="U43" s="4">
         <f t="shared" si="18"/>
         <v>9</v>
       </c>
-      <c r="V43" s="5" t="str">
+      <c r="V43" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-91</v>
       </c>
-      <c r="W43" s="5">
+      <c r="W43" s="4">
         <f t="shared" si="19"/>
         <v>4</v>
       </c>
-      <c r="X43" s="5" t="str">
+      <c r="X43" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:10::/112</v>
       </c>
-      <c r="Y43" s="5" t="str">
+      <c r="Y43" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:10::5</v>
       </c>
-      <c r="Z43" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA43" s="5" t="str">
+      <c r="Z43" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA43" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:10::1</v>
       </c>
     </row>
     <row r="44" spans="11:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T44" s="5">
+      <c r="T44" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U44" s="5">
+      <c r="U44" s="4">
         <f t="shared" si="18"/>
         <v>10</v>
       </c>
-      <c r="V44" s="5" t="str">
+      <c r="V44" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-92</v>
       </c>
-      <c r="W44" s="5">
+      <c r="W44" s="4">
         <f t="shared" si="19"/>
         <v>1</v>
       </c>
-      <c r="X44" s="5" t="str">
+      <c r="X44" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:11::/112</v>
       </c>
-      <c r="Y44" s="5" t="str">
+      <c r="Y44" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:11::2</v>
       </c>
-      <c r="Z44" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA44" s="5" t="str">
+      <c r="Z44" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA44" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:11::1</v>
       </c>
     </row>
     <row r="45" spans="11:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T45" s="5">
+      <c r="T45" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U45" s="5">
+      <c r="U45" s="4">
         <f t="shared" si="18"/>
         <v>10</v>
       </c>
-      <c r="V45" s="5" t="str">
+      <c r="V45" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-93</v>
       </c>
-      <c r="W45" s="5">
+      <c r="W45" s="4">
         <f t="shared" si="19"/>
         <v>2</v>
       </c>
-      <c r="X45" s="5" t="str">
+      <c r="X45" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:11::/112</v>
       </c>
-      <c r="Y45" s="5" t="str">
+      <c r="Y45" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:11::3</v>
       </c>
-      <c r="Z45" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA45" s="5" t="str">
+      <c r="Z45" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA45" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:11::1</v>
       </c>
     </row>
     <row r="46" spans="11:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T46" s="5">
+      <c r="T46" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U46" s="5">
+      <c r="U46" s="4">
         <f t="shared" si="18"/>
         <v>10</v>
       </c>
-      <c r="V46" s="5" t="str">
+      <c r="V46" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-94</v>
       </c>
-      <c r="W46" s="5">
+      <c r="W46" s="4">
         <f t="shared" si="19"/>
         <v>3</v>
       </c>
-      <c r="X46" s="5" t="str">
+      <c r="X46" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:11::/112</v>
       </c>
-      <c r="Y46" s="5" t="str">
+      <c r="Y46" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:11::4</v>
       </c>
-      <c r="Z46" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA46" s="5" t="str">
+      <c r="Z46" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA46" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:11::1</v>
       </c>
     </row>
     <row r="47" spans="11:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T47" s="5">
+      <c r="T47" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U47" s="5">
+      <c r="U47" s="4">
         <f t="shared" si="18"/>
         <v>10</v>
       </c>
-      <c r="V47" s="5" t="str">
+      <c r="V47" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-95</v>
       </c>
-      <c r="W47" s="5">
+      <c r="W47" s="4">
         <f t="shared" si="19"/>
         <v>4</v>
       </c>
-      <c r="X47" s="5" t="str">
+      <c r="X47" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:11::/112</v>
       </c>
-      <c r="Y47" s="5" t="str">
+      <c r="Y47" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:11::5</v>
       </c>
-      <c r="Z47" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA47" s="5" t="str">
+      <c r="Z47" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA47" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:11::1</v>
       </c>
     </row>
     <row r="48" spans="11:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T48" s="5">
+      <c r="T48" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U48" s="5">
+      <c r="U48" s="4">
         <f t="shared" si="18"/>
         <v>11</v>
       </c>
-      <c r="V48" s="5" t="str">
+      <c r="V48" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-96</v>
       </c>
-      <c r="W48" s="5">
+      <c r="W48" s="4">
         <f t="shared" si="19"/>
         <v>1</v>
       </c>
-      <c r="X48" s="5" t="str">
+      <c r="X48" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:12::/112</v>
       </c>
-      <c r="Y48" s="5" t="str">
+      <c r="Y48" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:12::2</v>
       </c>
-      <c r="Z48" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA48" s="5" t="str">
+      <c r="Z48" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA48" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:12::1</v>
       </c>
     </row>
     <row r="49" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T49" s="5">
+      <c r="T49" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U49" s="5">
+      <c r="U49" s="4">
         <f t="shared" si="18"/>
         <v>11</v>
       </c>
-      <c r="V49" s="5" t="str">
+      <c r="V49" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-97</v>
       </c>
-      <c r="W49" s="5">
+      <c r="W49" s="4">
         <f t="shared" si="19"/>
         <v>2</v>
       </c>
-      <c r="X49" s="5" t="str">
+      <c r="X49" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:12::/112</v>
       </c>
-      <c r="Y49" s="5" t="str">
+      <c r="Y49" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:12::3</v>
       </c>
-      <c r="Z49" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA49" s="5" t="str">
+      <c r="Z49" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA49" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:12::1</v>
       </c>
     </row>
     <row r="50" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T50" s="5">
+      <c r="T50" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U50" s="5">
+      <c r="U50" s="4">
         <f t="shared" si="18"/>
         <v>11</v>
       </c>
-      <c r="V50" s="5" t="str">
+      <c r="V50" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-98</v>
       </c>
-      <c r="W50" s="5">
+      <c r="W50" s="4">
         <f t="shared" si="19"/>
         <v>3</v>
       </c>
-      <c r="X50" s="5" t="str">
+      <c r="X50" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:12::/112</v>
       </c>
-      <c r="Y50" s="5" t="str">
+      <c r="Y50" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:12::4</v>
       </c>
-      <c r="Z50" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA50" s="5" t="str">
+      <c r="Z50" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA50" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:12::1</v>
       </c>
     </row>
     <row r="51" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T51" s="5">
+      <c r="T51" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U51" s="5">
+      <c r="U51" s="4">
         <f t="shared" si="18"/>
         <v>11</v>
       </c>
-      <c r="V51" s="5" t="str">
+      <c r="V51" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-99</v>
       </c>
-      <c r="W51" s="5">
+      <c r="W51" s="4">
         <f t="shared" si="19"/>
         <v>4</v>
       </c>
-      <c r="X51" s="5" t="str">
+      <c r="X51" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:12::/112</v>
       </c>
-      <c r="Y51" s="5" t="str">
+      <c r="Y51" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:12::5</v>
       </c>
-      <c r="Z51" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA51" s="5" t="str">
+      <c r="Z51" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA51" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:12::1</v>
       </c>
     </row>
     <row r="52" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T52" s="5">
+      <c r="T52" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U52" s="5">
+      <c r="U52" s="4">
         <f t="shared" si="18"/>
         <v>12</v>
       </c>
-      <c r="V52" s="5" t="str">
+      <c r="V52" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-100</v>
       </c>
-      <c r="W52" s="5">
+      <c r="W52" s="4">
         <f t="shared" si="19"/>
         <v>1</v>
       </c>
-      <c r="X52" s="5" t="str">
+      <c r="X52" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:13::/112</v>
       </c>
-      <c r="Y52" s="5" t="str">
+      <c r="Y52" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:13::2</v>
       </c>
-      <c r="Z52" s="5">
-        <v>112</v>
-      </c>
-      <c r="AA52" s="5" t="str">
+      <c r="Z52" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA52" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:13::1</v>
       </c>
     </row>
     <row r="53" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T53" s="2">
+      <c r="T53" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U53" s="2">
+      <c r="U53" s="4">
         <f t="shared" si="18"/>
         <v>12</v>
       </c>
-      <c r="V53" s="2" t="str">
+      <c r="V53" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-101</v>
       </c>
-      <c r="W53" s="2">
+      <c r="W53" s="4">
         <f t="shared" si="19"/>
         <v>2</v>
       </c>
-      <c r="X53" s="2" t="str">
+      <c r="X53" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:13::/112</v>
       </c>
-      <c r="Y53" s="2" t="str">
+      <c r="Y53" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:13::3</v>
       </c>
-      <c r="Z53" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA53" s="2" t="str">
+      <c r="Z53" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA53" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:13::1</v>
       </c>
     </row>
     <row r="54" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T54" s="2">
+      <c r="T54" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U54" s="2">
+      <c r="U54" s="4">
         <f t="shared" si="18"/>
         <v>12</v>
       </c>
-      <c r="V54" s="2" t="str">
+      <c r="V54" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-102</v>
       </c>
-      <c r="W54" s="2">
+      <c r="W54" s="4">
         <f t="shared" si="19"/>
         <v>3</v>
       </c>
-      <c r="X54" s="2" t="str">
+      <c r="X54" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:13::/112</v>
       </c>
-      <c r="Y54" s="2" t="str">
+      <c r="Y54" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:13::4</v>
       </c>
-      <c r="Z54" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA54" s="2" t="str">
+      <c r="Z54" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA54" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:13::1</v>
       </c>
     </row>
     <row r="55" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T55" s="2">
+      <c r="T55" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U55" s="2">
+      <c r="U55" s="4">
         <f t="shared" si="18"/>
         <v>12</v>
       </c>
-      <c r="V55" s="2" t="str">
+      <c r="V55" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-103</v>
       </c>
-      <c r="W55" s="2">
+      <c r="W55" s="4">
         <f t="shared" si="19"/>
         <v>4</v>
       </c>
-      <c r="X55" s="2" t="str">
+      <c r="X55" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:13::/112</v>
       </c>
-      <c r="Y55" s="2" t="str">
+      <c r="Y55" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:13::5</v>
       </c>
-      <c r="Z55" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA55" s="2" t="str">
+      <c r="Z55" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA55" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:13::1</v>
       </c>
     </row>
     <row r="56" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T56" s="2">
+      <c r="T56" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U56" s="2">
+      <c r="U56" s="4">
         <f t="shared" si="18"/>
         <v>13</v>
       </c>
-      <c r="V56" s="2" t="str">
+      <c r="V56" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-104</v>
       </c>
-      <c r="W56" s="2">
+      <c r="W56" s="4">
         <f t="shared" si="19"/>
         <v>1</v>
       </c>
-      <c r="X56" s="2" t="str">
+      <c r="X56" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:14::/112</v>
       </c>
-      <c r="Y56" s="2" t="str">
+      <c r="Y56" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:14::2</v>
       </c>
-      <c r="Z56" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA56" s="2" t="str">
+      <c r="Z56" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA56" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:14::1</v>
       </c>
     </row>
     <row r="57" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T57" s="2">
+      <c r="T57" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U57" s="2">
+      <c r="U57" s="4">
         <f t="shared" si="18"/>
         <v>13</v>
       </c>
-      <c r="V57" s="2" t="str">
+      <c r="V57" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-105</v>
       </c>
-      <c r="W57" s="2">
+      <c r="W57" s="4">
         <f t="shared" si="19"/>
         <v>2</v>
       </c>
-      <c r="X57" s="2" t="str">
+      <c r="X57" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:14::/112</v>
       </c>
-      <c r="Y57" s="2" t="str">
+      <c r="Y57" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:14::3</v>
       </c>
-      <c r="Z57" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA57" s="2" t="str">
+      <c r="Z57" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA57" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:14::1</v>
       </c>
     </row>
     <row r="58" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T58" s="2">
+      <c r="T58" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U58" s="2">
+      <c r="U58" s="4">
         <f t="shared" si="18"/>
         <v>13</v>
       </c>
-      <c r="V58" s="2" t="str">
+      <c r="V58" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-106</v>
       </c>
-      <c r="W58" s="2">
+      <c r="W58" s="4">
         <f t="shared" si="19"/>
         <v>3</v>
       </c>
-      <c r="X58" s="2" t="str">
+      <c r="X58" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:14::/112</v>
       </c>
-      <c r="Y58" s="2" t="str">
+      <c r="Y58" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:14::4</v>
       </c>
-      <c r="Z58" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA58" s="2" t="str">
+      <c r="Z58" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA58" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:14::1</v>
       </c>
     </row>
     <row r="59" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T59" s="2">
+      <c r="T59" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U59" s="2">
+      <c r="U59" s="4">
         <f t="shared" si="18"/>
         <v>13</v>
       </c>
-      <c r="V59" s="2" t="str">
+      <c r="V59" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-107</v>
       </c>
-      <c r="W59" s="2">
+      <c r="W59" s="4">
         <f t="shared" si="19"/>
         <v>4</v>
       </c>
-      <c r="X59" s="2" t="str">
+      <c r="X59" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:14::/112</v>
       </c>
-      <c r="Y59" s="2" t="str">
+      <c r="Y59" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:14::5</v>
       </c>
-      <c r="Z59" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA59" s="2" t="str">
+      <c r="Z59" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA59" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:14::1</v>
       </c>
     </row>
     <row r="60" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T60" s="2">
+      <c r="T60" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U60" s="2">
+      <c r="U60" s="4">
         <f t="shared" si="18"/>
         <v>14</v>
       </c>
-      <c r="V60" s="2" t="str">
+      <c r="V60" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-108</v>
       </c>
-      <c r="W60" s="2">
+      <c r="W60" s="4">
         <f t="shared" si="19"/>
         <v>1</v>
       </c>
-      <c r="X60" s="2" t="str">
+      <c r="X60" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:15::/112</v>
       </c>
-      <c r="Y60" s="2" t="str">
+      <c r="Y60" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:15::2</v>
       </c>
-      <c r="Z60" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA60" s="2" t="str">
+      <c r="Z60" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA60" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:15::1</v>
       </c>
     </row>
     <row r="61" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T61" s="2">
+      <c r="T61" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U61" s="2">
+      <c r="U61" s="4">
         <f t="shared" si="18"/>
         <v>14</v>
       </c>
-      <c r="V61" s="2" t="str">
+      <c r="V61" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-109</v>
       </c>
-      <c r="W61" s="2">
+      <c r="W61" s="4">
         <f t="shared" si="19"/>
         <v>2</v>
       </c>
-      <c r="X61" s="2" t="str">
+      <c r="X61" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:15::/112</v>
       </c>
-      <c r="Y61" s="2" t="str">
+      <c r="Y61" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:15::3</v>
       </c>
-      <c r="Z61" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA61" s="2" t="str">
+      <c r="Z61" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA61" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:15::1</v>
       </c>
     </row>
     <row r="62" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T62" s="2">
+      <c r="T62" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U62" s="2">
+      <c r="U62" s="4">
         <f t="shared" si="18"/>
         <v>14</v>
       </c>
-      <c r="V62" s="2" t="str">
+      <c r="V62" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-110</v>
       </c>
-      <c r="W62" s="2">
+      <c r="W62" s="4">
         <f t="shared" si="19"/>
         <v>3</v>
       </c>
-      <c r="X62" s="2" t="str">
+      <c r="X62" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:15::/112</v>
       </c>
-      <c r="Y62" s="2" t="str">
+      <c r="Y62" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:15::4</v>
       </c>
-      <c r="Z62" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA62" s="2" t="str">
+      <c r="Z62" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA62" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:15::1</v>
       </c>
     </row>
     <row r="63" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T63" s="2">
+      <c r="T63" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U63" s="2">
+      <c r="U63" s="4">
         <f t="shared" si="18"/>
         <v>14</v>
       </c>
-      <c r="V63" s="2" t="str">
+      <c r="V63" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-111</v>
       </c>
-      <c r="W63" s="2">
+      <c r="W63" s="4">
         <f t="shared" si="19"/>
         <v>4</v>
       </c>
-      <c r="X63" s="2" t="str">
+      <c r="X63" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:15::/112</v>
       </c>
-      <c r="Y63" s="2" t="str">
+      <c r="Y63" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:15::5</v>
       </c>
-      <c r="Z63" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA63" s="2" t="str">
+      <c r="Z63" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA63" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:15::1</v>
       </c>
     </row>
     <row r="64" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T64" s="2">
+      <c r="T64" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U64" s="2">
+      <c r="U64" s="4">
         <f t="shared" si="18"/>
         <v>15</v>
       </c>
-      <c r="V64" s="2" t="str">
+      <c r="V64" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-112</v>
       </c>
-      <c r="W64" s="2">
+      <c r="W64" s="4">
         <f t="shared" si="19"/>
         <v>1</v>
       </c>
-      <c r="X64" s="2" t="str">
+      <c r="X64" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:16::/112</v>
       </c>
-      <c r="Y64" s="2" t="str">
+      <c r="Y64" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:16::2</v>
       </c>
-      <c r="Z64" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA64" s="2" t="str">
+      <c r="Z64" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA64" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:16::1</v>
       </c>
     </row>
     <row r="65" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T65" s="2">
+      <c r="T65" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U65" s="2">
+      <c r="U65" s="4">
         <f t="shared" si="18"/>
         <v>15</v>
       </c>
-      <c r="V65" s="2" t="str">
+      <c r="V65" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-113</v>
       </c>
-      <c r="W65" s="2">
+      <c r="W65" s="4">
         <f t="shared" si="19"/>
         <v>2</v>
       </c>
-      <c r="X65" s="2" t="str">
+      <c r="X65" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:16::/112</v>
       </c>
-      <c r="Y65" s="2" t="str">
+      <c r="Y65" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:16::3</v>
       </c>
-      <c r="Z65" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA65" s="2" t="str">
+      <c r="Z65" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA65" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:16::1</v>
       </c>
     </row>
     <row r="66" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T66" s="2">
+      <c r="T66" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U66" s="2">
+      <c r="U66" s="4">
         <f t="shared" si="18"/>
         <v>15</v>
       </c>
-      <c r="V66" s="2" t="str">
+      <c r="V66" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-114</v>
       </c>
-      <c r="W66" s="2">
+      <c r="W66" s="4">
         <f t="shared" si="19"/>
         <v>3</v>
       </c>
-      <c r="X66" s="2" t="str">
+      <c r="X66" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:16::/112</v>
       </c>
-      <c r="Y66" s="2" t="str">
+      <c r="Y66" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:16::4</v>
       </c>
-      <c r="Z66" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA66" s="2" t="str">
+      <c r="Z66" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA66" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:16::1</v>
       </c>
     </row>
     <row r="67" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T67" s="2">
+      <c r="T67" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U67" s="2">
+      <c r="U67" s="4">
         <f t="shared" si="18"/>
         <v>15</v>
       </c>
-      <c r="V67" s="2" t="str">
+      <c r="V67" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-115</v>
       </c>
-      <c r="W67" s="2">
+      <c r="W67" s="4">
         <f t="shared" si="19"/>
         <v>4</v>
       </c>
-      <c r="X67" s="2" t="str">
+      <c r="X67" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:16::/112</v>
       </c>
-      <c r="Y67" s="2" t="str">
+      <c r="Y67" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:16::5</v>
       </c>
-      <c r="Z67" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA67" s="2" t="str">
+      <c r="Z67" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA67" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:16::1</v>
       </c>
     </row>
     <row r="68" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T68" s="2">
+      <c r="T68" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U68" s="2">
+      <c r="U68" s="4">
         <f t="shared" si="18"/>
         <v>16</v>
       </c>
-      <c r="V68" s="2" t="str">
+      <c r="V68" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-116</v>
       </c>
-      <c r="W68" s="2">
+      <c r="W68" s="4">
         <f t="shared" si="19"/>
         <v>1</v>
       </c>
-      <c r="X68" s="2" t="str">
+      <c r="X68" s="4" t="str">
         <f t="shared" si="6"/>
         <v>2001:3:17::/112</v>
       </c>
-      <c r="Y68" s="2" t="str">
+      <c r="Y68" s="4" t="str">
         <f t="shared" si="7"/>
         <v>2001:3:17::2</v>
       </c>
-      <c r="Z68" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA68" s="2" t="str">
+      <c r="Z68" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA68" s="4" t="str">
         <f t="shared" si="8"/>
         <v>2001:3:17::1</v>
       </c>
     </row>
     <row r="69" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T69" s="2">
+      <c r="T69" s="4">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="U69" s="2">
+      <c r="U69" s="4">
         <f t="shared" si="18"/>
         <v>16</v>
       </c>
-      <c r="V69" s="2" t="str">
+      <c r="V69" s="4" t="str">
         <f t="shared" si="13"/>
         <v>PC-117</v>
       </c>
-      <c r="W69" s="2">
+      <c r="W69" s="4">
         <f t="shared" si="19"/>
         <v>2</v>
       </c>
-      <c r="X69" s="2" t="str">
+      <c r="X69" s="4" t="str">
         <f t="shared" ref="X69:X87" si="20">_xlfn.CONCAT("2001:",T69,":",U69 + 1,"::/112")</f>
         <v>2001:3:17::/112</v>
       </c>
-      <c r="Y69" s="2" t="str">
+      <c r="Y69" s="4" t="str">
         <f t="shared" ref="Y69:Y87" si="21">_xlfn.CONCAT("2001:",T69,":",U69+1,"::",W69 + 1)</f>
         <v>2001:3:17::3</v>
       </c>
-      <c r="Z69" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA69" s="2" t="str">
+      <c r="Z69" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA69" s="4" t="str">
         <f t="shared" ref="AA69:AA87" si="22">_xlfn.CONCAT("2001:",T69,":",U69+1,"::1")</f>
         <v>2001:3:17::1</v>
       </c>
     </row>
     <row r="70" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T70" s="2">
+      <c r="T70" s="4">
         <f t="shared" ref="T70:T87" si="23">T69</f>
         <v>3</v>
       </c>
-      <c r="U70" s="2">
+      <c r="U70" s="4">
         <f t="shared" si="18"/>
         <v>16</v>
       </c>
-      <c r="V70" s="2" t="str">
+      <c r="V70" s="4" t="str">
         <f t="shared" ref="V70:V87" si="24">_xlfn.CONCAT("PC-",MID(V69,FIND("-",V69)+ 1, LEN(V69))+1)</f>
         <v>PC-118</v>
       </c>
-      <c r="W70" s="2">
+      <c r="W70" s="4">
         <f t="shared" si="19"/>
         <v>3</v>
       </c>
-      <c r="X70" s="2" t="str">
+      <c r="X70" s="4" t="str">
         <f t="shared" si="20"/>
         <v>2001:3:17::/112</v>
       </c>
-      <c r="Y70" s="2" t="str">
+      <c r="Y70" s="4" t="str">
         <f t="shared" si="21"/>
         <v>2001:3:17::4</v>
       </c>
-      <c r="Z70" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA70" s="2" t="str">
+      <c r="Z70" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA70" s="4" t="str">
         <f t="shared" si="22"/>
         <v>2001:3:17::1</v>
       </c>
     </row>
     <row r="71" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T71" s="2">
+      <c r="T71" s="4">
         <f t="shared" si="23"/>
         <v>3</v>
       </c>
-      <c r="U71" s="2">
+      <c r="U71" s="4">
         <f t="shared" si="18"/>
         <v>16</v>
       </c>
-      <c r="V71" s="2" t="str">
+      <c r="V71" s="4" t="str">
         <f t="shared" si="24"/>
         <v>PC-119</v>
       </c>
-      <c r="W71" s="2">
+      <c r="W71" s="4">
         <f t="shared" si="19"/>
         <v>4</v>
       </c>
-      <c r="X71" s="2" t="str">
+      <c r="X71" s="4" t="str">
         <f t="shared" si="20"/>
         <v>2001:3:17::/112</v>
       </c>
-      <c r="Y71" s="2" t="str">
+      <c r="Y71" s="4" t="str">
         <f t="shared" si="21"/>
         <v>2001:3:17::5</v>
       </c>
-      <c r="Z71" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA71" s="2" t="str">
+      <c r="Z71" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA71" s="4" t="str">
         <f t="shared" si="22"/>
         <v>2001:3:17::1</v>
       </c>
     </row>
     <row r="72" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T72" s="2">
+      <c r="T72" s="4">
         <f t="shared" si="23"/>
         <v>3</v>
       </c>
-      <c r="U72" s="2">
+      <c r="U72" s="4">
         <f t="shared" si="18"/>
         <v>17</v>
       </c>
-      <c r="V72" s="2" t="str">
+      <c r="V72" s="4" t="str">
         <f t="shared" si="24"/>
         <v>PC-120</v>
       </c>
-      <c r="W72" s="2">
+      <c r="W72" s="4">
         <f t="shared" si="19"/>
         <v>1</v>
       </c>
-      <c r="X72" s="2" t="str">
+      <c r="X72" s="4" t="str">
         <f t="shared" si="20"/>
         <v>2001:3:18::/112</v>
       </c>
-      <c r="Y72" s="2" t="str">
+      <c r="Y72" s="4" t="str">
         <f t="shared" si="21"/>
         <v>2001:3:18::2</v>
       </c>
-      <c r="Z72" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA72" s="2" t="str">
+      <c r="Z72" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA72" s="4" t="str">
         <f t="shared" si="22"/>
         <v>2001:3:18::1</v>
       </c>
     </row>
     <row r="73" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T73" s="2">
+      <c r="T73" s="4">
         <f t="shared" si="23"/>
         <v>3</v>
       </c>
-      <c r="U73" s="2">
+      <c r="U73" s="4">
         <f t="shared" ref="U73:U87" si="25">U69+1</f>
         <v>17</v>
       </c>
-      <c r="V73" s="2" t="str">
+      <c r="V73" s="4" t="str">
         <f t="shared" si="24"/>
         <v>PC-121</v>
       </c>
-      <c r="W73" s="2">
+      <c r="W73" s="4">
         <f t="shared" ref="W73:W87" si="26">W69</f>
         <v>2</v>
       </c>
-      <c r="X73" s="2" t="str">
+      <c r="X73" s="4" t="str">
         <f t="shared" si="20"/>
         <v>2001:3:18::/112</v>
       </c>
-      <c r="Y73" s="2" t="str">
+      <c r="Y73" s="4" t="str">
         <f t="shared" si="21"/>
         <v>2001:3:18::3</v>
       </c>
-      <c r="Z73" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA73" s="2" t="str">
+      <c r="Z73" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA73" s="4" t="str">
         <f t="shared" si="22"/>
         <v>2001:3:18::1</v>
       </c>
     </row>
     <row r="74" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T74" s="2">
+      <c r="T74" s="4">
         <f t="shared" si="23"/>
         <v>3</v>
       </c>
-      <c r="U74" s="2">
+      <c r="U74" s="4">
         <f t="shared" si="25"/>
         <v>17</v>
       </c>
-      <c r="V74" s="2" t="str">
+      <c r="V74" s="4" t="str">
         <f t="shared" si="24"/>
         <v>PC-122</v>
       </c>
-      <c r="W74" s="2">
+      <c r="W74" s="4">
         <f t="shared" si="26"/>
         <v>3</v>
       </c>
-      <c r="X74" s="2" t="str">
+      <c r="X74" s="4" t="str">
         <f t="shared" si="20"/>
         <v>2001:3:18::/112</v>
       </c>
-      <c r="Y74" s="2" t="str">
+      <c r="Y74" s="4" t="str">
         <f t="shared" si="21"/>
         <v>2001:3:18::4</v>
       </c>
-      <c r="Z74" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA74" s="2" t="str">
+      <c r="Z74" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA74" s="4" t="str">
         <f t="shared" si="22"/>
         <v>2001:3:18::1</v>
       </c>
     </row>
     <row r="75" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T75" s="2">
+      <c r="T75" s="4">
         <f t="shared" si="23"/>
         <v>3</v>
       </c>
-      <c r="U75" s="2">
+      <c r="U75" s="4">
         <f t="shared" si="25"/>
         <v>17</v>
       </c>
-      <c r="V75" s="2" t="str">
+      <c r="V75" s="4" t="str">
         <f t="shared" si="24"/>
         <v>PC-123</v>
       </c>
-      <c r="W75" s="2">
+      <c r="W75" s="4">
         <f t="shared" si="26"/>
         <v>4</v>
       </c>
-      <c r="X75" s="2" t="str">
+      <c r="X75" s="4" t="str">
         <f t="shared" si="20"/>
         <v>2001:3:18::/112</v>
       </c>
-      <c r="Y75" s="2" t="str">
+      <c r="Y75" s="4" t="str">
         <f t="shared" si="21"/>
         <v>2001:3:18::5</v>
       </c>
-      <c r="Z75" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA75" s="2" t="str">
+      <c r="Z75" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA75" s="4" t="str">
         <f t="shared" si="22"/>
         <v>2001:3:18::1</v>
       </c>
     </row>
     <row r="76" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T76" s="2">
+      <c r="T76" s="4">
         <f t="shared" si="23"/>
         <v>3</v>
       </c>
-      <c r="U76" s="2">
+      <c r="U76" s="4">
         <f t="shared" si="25"/>
         <v>18</v>
       </c>
-      <c r="V76" s="2" t="str">
+      <c r="V76" s="4" t="str">
         <f t="shared" si="24"/>
         <v>PC-124</v>
       </c>
-      <c r="W76" s="2">
+      <c r="W76" s="4">
         <f t="shared" si="26"/>
         <v>1</v>
       </c>
-      <c r="X76" s="2" t="str">
+      <c r="X76" s="4" t="str">
         <f t="shared" si="20"/>
         <v>2001:3:19::/112</v>
       </c>
-      <c r="Y76" s="2" t="str">
+      <c r="Y76" s="4" t="str">
         <f t="shared" si="21"/>
         <v>2001:3:19::2</v>
       </c>
-      <c r="Z76" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA76" s="2" t="str">
+      <c r="Z76" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA76" s="4" t="str">
         <f t="shared" si="22"/>
         <v>2001:3:19::1</v>
       </c>
     </row>
     <row r="77" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T77" s="2">
+      <c r="T77" s="4">
         <f t="shared" si="23"/>
         <v>3</v>
       </c>
-      <c r="U77" s="2">
+      <c r="U77" s="4">
         <f t="shared" si="25"/>
         <v>18</v>
       </c>
-      <c r="V77" s="2" t="str">
+      <c r="V77" s="4" t="str">
         <f t="shared" si="24"/>
         <v>PC-125</v>
       </c>
-      <c r="W77" s="2">
+      <c r="W77" s="4">
         <f t="shared" si="26"/>
         <v>2</v>
       </c>
-      <c r="X77" s="2" t="str">
+      <c r="X77" s="4" t="str">
         <f t="shared" si="20"/>
         <v>2001:3:19::/112</v>
       </c>
-      <c r="Y77" s="2" t="str">
+      <c r="Y77" s="4" t="str">
         <f t="shared" si="21"/>
         <v>2001:3:19::3</v>
       </c>
-      <c r="Z77" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA77" s="2" t="str">
+      <c r="Z77" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA77" s="4" t="str">
         <f t="shared" si="22"/>
         <v>2001:3:19::1</v>
       </c>
     </row>
     <row r="78" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T78" s="2">
+      <c r="T78" s="4">
         <f t="shared" si="23"/>
         <v>3</v>
       </c>
-      <c r="U78" s="2">
+      <c r="U78" s="4">
         <f t="shared" si="25"/>
         <v>18</v>
       </c>
-      <c r="V78" s="2" t="str">
+      <c r="V78" s="4" t="str">
         <f t="shared" si="24"/>
         <v>PC-126</v>
       </c>
-      <c r="W78" s="2">
+      <c r="W78" s="4">
         <f t="shared" si="26"/>
         <v>3</v>
       </c>
-      <c r="X78" s="2" t="str">
+      <c r="X78" s="4" t="str">
         <f t="shared" si="20"/>
         <v>2001:3:19::/112</v>
       </c>
-      <c r="Y78" s="2" t="str">
+      <c r="Y78" s="4" t="str">
         <f t="shared" si="21"/>
         <v>2001:3:19::4</v>
       </c>
-      <c r="Z78" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA78" s="2" t="str">
+      <c r="Z78" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA78" s="4" t="str">
         <f t="shared" si="22"/>
         <v>2001:3:19::1</v>
       </c>
     </row>
     <row r="79" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T79" s="2">
+      <c r="T79" s="4">
         <f t="shared" si="23"/>
         <v>3</v>
       </c>
-      <c r="U79" s="2">
+      <c r="U79" s="4">
         <f t="shared" si="25"/>
         <v>18</v>
       </c>
-      <c r="V79" s="2" t="str">
+      <c r="V79" s="4" t="str">
         <f t="shared" si="24"/>
         <v>PC-127</v>
       </c>
-      <c r="W79" s="2">
+      <c r="W79" s="4">
         <f t="shared" si="26"/>
         <v>4</v>
       </c>
-      <c r="X79" s="2" t="str">
+      <c r="X79" s="4" t="str">
         <f t="shared" si="20"/>
         <v>2001:3:19::/112</v>
       </c>
-      <c r="Y79" s="2" t="str">
+      <c r="Y79" s="4" t="str">
         <f t="shared" si="21"/>
         <v>2001:3:19::5</v>
       </c>
-      <c r="Z79" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA79" s="2" t="str">
+      <c r="Z79" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA79" s="4" t="str">
         <f t="shared" si="22"/>
         <v>2001:3:19::1</v>
       </c>
     </row>
     <row r="80" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T80" s="2">
+      <c r="T80" s="4">
         <f t="shared" si="23"/>
         <v>3</v>
       </c>
-      <c r="U80" s="2">
+      <c r="U80" s="4">
         <f t="shared" si="25"/>
         <v>19</v>
       </c>
-      <c r="V80" s="2" t="str">
+      <c r="V80" s="4" t="str">
         <f t="shared" si="24"/>
         <v>PC-128</v>
       </c>
-      <c r="W80" s="2">
+      <c r="W80" s="4">
         <f t="shared" si="26"/>
         <v>1</v>
       </c>
-      <c r="X80" s="2" t="str">
+      <c r="X80" s="4" t="str">
         <f t="shared" si="20"/>
         <v>2001:3:20::/112</v>
       </c>
-      <c r="Y80" s="2" t="str">
+      <c r="Y80" s="4" t="str">
         <f t="shared" si="21"/>
         <v>2001:3:20::2</v>
       </c>
-      <c r="Z80" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA80" s="2" t="str">
+      <c r="Z80" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA80" s="4" t="str">
         <f t="shared" si="22"/>
         <v>2001:3:20::1</v>
       </c>
     </row>
     <row r="81" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T81" s="2">
+      <c r="T81" s="4">
         <f t="shared" si="23"/>
         <v>3</v>
       </c>
-      <c r="U81" s="2">
+      <c r="U81" s="4">
         <f t="shared" si="25"/>
         <v>19</v>
       </c>
-      <c r="V81" s="2" t="str">
+      <c r="V81" s="4" t="str">
         <f t="shared" si="24"/>
         <v>PC-129</v>
       </c>
-      <c r="W81" s="2">
+      <c r="W81" s="4">
         <f t="shared" si="26"/>
         <v>2</v>
       </c>
-      <c r="X81" s="2" t="str">
+      <c r="X81" s="4" t="str">
         <f t="shared" si="20"/>
         <v>2001:3:20::/112</v>
       </c>
-      <c r="Y81" s="2" t="str">
+      <c r="Y81" s="4" t="str">
         <f t="shared" si="21"/>
         <v>2001:3:20::3</v>
       </c>
-      <c r="Z81" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA81" s="2" t="str">
+      <c r="Z81" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA81" s="4" t="str">
         <f t="shared" si="22"/>
         <v>2001:3:20::1</v>
       </c>
     </row>
     <row r="82" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T82" s="2">
+      <c r="T82" s="4">
         <f t="shared" si="23"/>
         <v>3</v>
       </c>
-      <c r="U82" s="2">
+      <c r="U82" s="4">
         <f t="shared" si="25"/>
         <v>19</v>
       </c>
-      <c r="V82" s="2" t="str">
+      <c r="V82" s="4" t="str">
         <f t="shared" si="24"/>
         <v>PC-130</v>
       </c>
-      <c r="W82" s="2">
+      <c r="W82" s="4">
         <f t="shared" si="26"/>
         <v>3</v>
       </c>
-      <c r="X82" s="2" t="str">
+      <c r="X82" s="4" t="str">
         <f t="shared" si="20"/>
         <v>2001:3:20::/112</v>
       </c>
-      <c r="Y82" s="2" t="str">
+      <c r="Y82" s="4" t="str">
         <f t="shared" si="21"/>
         <v>2001:3:20::4</v>
       </c>
-      <c r="Z82" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA82" s="2" t="str">
+      <c r="Z82" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA82" s="4" t="str">
         <f t="shared" si="22"/>
         <v>2001:3:20::1</v>
       </c>
     </row>
     <row r="83" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T83" s="2">
+      <c r="T83" s="4">
         <f t="shared" si="23"/>
         <v>3</v>
       </c>
-      <c r="U83" s="2">
+      <c r="U83" s="4">
         <f t="shared" si="25"/>
         <v>19</v>
       </c>
-      <c r="V83" s="2" t="str">
+      <c r="V83" s="4" t="str">
         <f t="shared" si="24"/>
         <v>PC-131</v>
       </c>
-      <c r="W83" s="2">
+      <c r="W83" s="4">
         <f t="shared" si="26"/>
         <v>4</v>
       </c>
-      <c r="X83" s="2" t="str">
+      <c r="X83" s="4" t="str">
         <f t="shared" si="20"/>
         <v>2001:3:20::/112</v>
       </c>
-      <c r="Y83" s="2" t="str">
+      <c r="Y83" s="4" t="str">
         <f t="shared" si="21"/>
         <v>2001:3:20::5</v>
       </c>
-      <c r="Z83" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA83" s="2" t="str">
+      <c r="Z83" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA83" s="4" t="str">
         <f t="shared" si="22"/>
         <v>2001:3:20::1</v>
       </c>
     </row>
     <row r="84" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T84" s="2">
+      <c r="T84" s="4">
         <f t="shared" si="23"/>
         <v>3</v>
       </c>
-      <c r="U84" s="2">
+      <c r="U84" s="4">
         <f t="shared" si="25"/>
         <v>20</v>
       </c>
-      <c r="V84" s="2" t="str">
+      <c r="V84" s="4" t="str">
         <f t="shared" si="24"/>
         <v>PC-132</v>
       </c>
-      <c r="W84" s="2">
+      <c r="W84" s="4">
         <f t="shared" si="26"/>
         <v>1</v>
       </c>
-      <c r="X84" s="2" t="str">
+      <c r="X84" s="4" t="str">
         <f t="shared" si="20"/>
         <v>2001:3:21::/112</v>
       </c>
-      <c r="Y84" s="2" t="str">
+      <c r="Y84" s="4" t="str">
         <f t="shared" si="21"/>
         <v>2001:3:21::2</v>
       </c>
-      <c r="Z84" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA84" s="2" t="str">
+      <c r="Z84" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA84" s="4" t="str">
         <f t="shared" si="22"/>
         <v>2001:3:21::1</v>
       </c>
     </row>
     <row r="85" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T85" s="2">
+      <c r="T85" s="4">
         <f t="shared" si="23"/>
         <v>3</v>
       </c>
-      <c r="U85" s="2">
+      <c r="U85" s="4">
         <f t="shared" si="25"/>
         <v>20</v>
       </c>
-      <c r="V85" s="2" t="str">
+      <c r="V85" s="4" t="str">
         <f t="shared" si="24"/>
         <v>PC-133</v>
       </c>
-      <c r="W85" s="2">
+      <c r="W85" s="4">
         <f t="shared" si="26"/>
         <v>2</v>
       </c>
-      <c r="X85" s="2" t="str">
+      <c r="X85" s="4" t="str">
         <f t="shared" si="20"/>
         <v>2001:3:21::/112</v>
       </c>
-      <c r="Y85" s="2" t="str">
+      <c r="Y85" s="4" t="str">
         <f t="shared" si="21"/>
         <v>2001:3:21::3</v>
       </c>
-      <c r="Z85" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA85" s="2" t="str">
+      <c r="Z85" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA85" s="4" t="str">
         <f t="shared" si="22"/>
         <v>2001:3:21::1</v>
       </c>
     </row>
     <row r="86" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T86" s="2">
+      <c r="T86" s="4">
         <f t="shared" si="23"/>
         <v>3</v>
       </c>
-      <c r="U86" s="2">
+      <c r="U86" s="4">
         <f t="shared" si="25"/>
         <v>20</v>
       </c>
-      <c r="V86" s="2" t="str">
+      <c r="V86" s="4" t="str">
         <f t="shared" si="24"/>
         <v>PC-134</v>
       </c>
-      <c r="W86" s="2">
+      <c r="W86" s="4">
         <f t="shared" si="26"/>
         <v>3</v>
       </c>
-      <c r="X86" s="2" t="str">
+      <c r="X86" s="4" t="str">
         <f t="shared" si="20"/>
         <v>2001:3:21::/112</v>
       </c>
-      <c r="Y86" s="2" t="str">
+      <c r="Y86" s="4" t="str">
         <f t="shared" si="21"/>
         <v>2001:3:21::4</v>
       </c>
-      <c r="Z86" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA86" s="2" t="str">
+      <c r="Z86" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA86" s="4" t="str">
         <f t="shared" si="22"/>
         <v>2001:3:21::1</v>
       </c>
     </row>
     <row r="87" spans="20:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="T87" s="2">
+      <c r="T87" s="4">
         <f t="shared" si="23"/>
         <v>3</v>
       </c>
-      <c r="U87" s="2">
+      <c r="U87" s="4">
         <f t="shared" si="25"/>
         <v>20</v>
       </c>
-      <c r="V87" s="2" t="str">
+      <c r="V87" s="4" t="str">
         <f t="shared" si="24"/>
         <v>PC-135</v>
       </c>
-      <c r="W87" s="2">
+      <c r="W87" s="4">
         <f t="shared" si="26"/>
         <v>4</v>
       </c>
-      <c r="X87" s="2" t="str">
+      <c r="X87" s="4" t="str">
         <f t="shared" si="20"/>
         <v>2001:3:21::/112</v>
       </c>
-      <c r="Y87" s="2" t="str">
+      <c r="Y87" s="4" t="str">
         <f t="shared" si="21"/>
         <v>2001:3:21::5</v>
       </c>
-      <c r="Z87" s="2">
-        <v>112</v>
-      </c>
-      <c r="AA87" s="2" t="str">
+      <c r="Z87" s="4">
+        <v>112</v>
+      </c>
+      <c r="AA87" s="4" t="str">
         <f t="shared" si="22"/>
         <v>2001:3:21::1</v>
       </c>

</xml_diff>

<commit_message>
Se termina enrutamiento static en edificio 3
</commit_message>
<xml_diff>
--- a/taller-2/Taller#2.xlsx
+++ b/taller-2/Taller#2.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivanbotero/Projects/interconexion/taller-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7565813F-8695-8C43-8159-837495F1EDC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAAC36B6-6DA0-454A-9284-342CED03E23D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="0" windowWidth="27320" windowHeight="15360" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25600" yWindow="0" windowWidth="27320" windowHeight="15360" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ipv4" sheetId="1" r:id="rId1"/>
     <sheet name="ipv6" sheetId="2" r:id="rId2"/>
     <sheet name="Enrutamiento4E1" sheetId="3" r:id="rId3"/>
+    <sheet name="Enrutamiento4E3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="37">
   <si>
     <t>#</t>
   </si>
@@ -150,7 +151,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,6 +190,12 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="Apple Braille Outline 8 Dot"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -9999,8 +10006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C98B32B-8108-7E4E-A7C9-5ADE5A4FC831}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -11139,4 +11146,1153 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C40AFAA-8036-5748-A687-D4A954FCC149}">
+  <dimension ref="A1:I34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.33203125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="2.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="13">
+        <v>3</v>
+      </c>
+      <c r="C1" s="7">
+        <v>20</v>
+      </c>
+      <c r="D1" s="8" t="str">
+        <f>_xlfn.CONCAT("172.",B1,".",C1,".0")</f>
+        <v>172.3.20.0</v>
+      </c>
+      <c r="E1" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>3</v>
+      </c>
+      <c r="F1" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>19</v>
+      </c>
+      <c r="G1" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H1" s="8" t="str">
+        <f ca="1">_xlfn.CONCAT("10.",E1,".",F1,".",G1)</f>
+        <v>10.3.19.1</v>
+      </c>
+      <c r="I1" t="str">
+        <f>IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D1, " ", "255.255.255.0"," ", H1))</f>
+        <v>#</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B2" s="13">
+        <v>3</v>
+      </c>
+      <c r="C2" s="7">
+        <f>C1-1</f>
+        <v>19</v>
+      </c>
+      <c r="D2" s="8" t="str">
+        <f>_xlfn.CONCAT("172.",B2,".",C2,".0")</f>
+        <v>172.3.19.0</v>
+      </c>
+      <c r="E2" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>3</v>
+      </c>
+      <c r="F2" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>19</v>
+      </c>
+      <c r="G2" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H2" s="8" t="str">
+        <f t="shared" ref="H2:H34" ca="1" si="0">_xlfn.CONCAT("10.",E2,".",F2,".",G2)</f>
+        <v>10.3.19.1</v>
+      </c>
+      <c r="I2" t="str">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D2, " ", "255.255.255.0"," ", H2))</f>
+        <v>ip route 172.3.19.0 255.255.255.0 10.3.19.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B3" s="13">
+        <v>3</v>
+      </c>
+      <c r="C3" s="7">
+        <f t="shared" ref="C3:C21" si="1">C2-1</f>
+        <v>18</v>
+      </c>
+      <c r="D3" s="8" t="str">
+        <f>_xlfn.CONCAT("172.",B3,".",C3,".0")</f>
+        <v>172.3.18.0</v>
+      </c>
+      <c r="E3" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>3</v>
+      </c>
+      <c r="F3" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>19</v>
+      </c>
+      <c r="G3" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H3" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.3.19.1</v>
+      </c>
+      <c r="I3" t="str">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D3, " ", "255.255.255.0"," ", H3))</f>
+        <v>ip route 172.3.18.0 255.255.255.0 10.3.19.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B4" s="13">
+        <v>3</v>
+      </c>
+      <c r="C4" s="7">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="D4" s="8" t="str">
+        <f>_xlfn.CONCAT("172.",B4,".",C4,".0")</f>
+        <v>172.3.17.0</v>
+      </c>
+      <c r="E4" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>3</v>
+      </c>
+      <c r="F4" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>19</v>
+      </c>
+      <c r="G4" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H4" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.3.19.1</v>
+      </c>
+      <c r="I4" t="str">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D4, " ", "255.255.255.0"," ", H4))</f>
+        <v>ip route 172.3.17.0 255.255.255.0 10.3.19.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B5" s="13">
+        <v>3</v>
+      </c>
+      <c r="C5" s="7">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="D5" s="8" t="str">
+        <f>_xlfn.CONCAT("172.",B5,".",C5,".0")</f>
+        <v>172.3.16.0</v>
+      </c>
+      <c r="E5" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>3</v>
+      </c>
+      <c r="F5" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>19</v>
+      </c>
+      <c r="G5" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H5" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.3.19.1</v>
+      </c>
+      <c r="I5" t="str">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D5, " ", "255.255.255.0"," ", H5))</f>
+        <v>ip route 172.3.16.0 255.255.255.0 10.3.19.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B6" s="13">
+        <v>3</v>
+      </c>
+      <c r="C6" s="7">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="D6" s="8" t="str">
+        <f>_xlfn.CONCAT("172.",B6,".",C6,".0")</f>
+        <v>172.3.15.0</v>
+      </c>
+      <c r="E6" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>3</v>
+      </c>
+      <c r="F6" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>19</v>
+      </c>
+      <c r="G6" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H6" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.3.19.1</v>
+      </c>
+      <c r="I6" t="str">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D6, " ", "255.255.255.0"," ", H6))</f>
+        <v>ip route 172.3.15.0 255.255.255.0 10.3.19.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B7" s="13">
+        <v>3</v>
+      </c>
+      <c r="C7" s="7">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="D7" s="8" t="str">
+        <f>_xlfn.CONCAT("172.",B7,".",C7,".0")</f>
+        <v>172.3.14.0</v>
+      </c>
+      <c r="E7" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>3</v>
+      </c>
+      <c r="F7" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>19</v>
+      </c>
+      <c r="G7" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H7" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.3.19.1</v>
+      </c>
+      <c r="I7" t="str">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D7, " ", "255.255.255.0"," ", H7))</f>
+        <v>ip route 172.3.14.0 255.255.255.0 10.3.19.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B8" s="13">
+        <v>3</v>
+      </c>
+      <c r="C8" s="7">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="D8" s="8" t="str">
+        <f>_xlfn.CONCAT("172.",B8,".",C8,".0")</f>
+        <v>172.3.13.0</v>
+      </c>
+      <c r="E8" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>3</v>
+      </c>
+      <c r="F8" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>19</v>
+      </c>
+      <c r="G8" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H8" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.3.19.1</v>
+      </c>
+      <c r="I8" t="str">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D8, " ", "255.255.255.0"," ", H8))</f>
+        <v>ip route 172.3.13.0 255.255.255.0 10.3.19.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B9" s="13">
+        <v>3</v>
+      </c>
+      <c r="C9" s="7">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="D9" s="8" t="str">
+        <f>_xlfn.CONCAT("172.",B9,".",C9,".0")</f>
+        <v>172.3.12.0</v>
+      </c>
+      <c r="E9" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>3</v>
+      </c>
+      <c r="F9" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>19</v>
+      </c>
+      <c r="G9" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H9" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.3.19.1</v>
+      </c>
+      <c r="I9" t="str">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D9, " ", "255.255.255.0"," ", H9))</f>
+        <v>ip route 172.3.12.0 255.255.255.0 10.3.19.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B10" s="13">
+        <v>3</v>
+      </c>
+      <c r="C10" s="7">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="D10" s="8" t="str">
+        <f>_xlfn.CONCAT("172.",B10,".",C10,".0")</f>
+        <v>172.3.11.0</v>
+      </c>
+      <c r="E10" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>3</v>
+      </c>
+      <c r="F10" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>19</v>
+      </c>
+      <c r="G10" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H10" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.3.19.1</v>
+      </c>
+      <c r="I10" t="str">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D10, " ", "255.255.255.0"," ", H10))</f>
+        <v>ip route 172.3.11.0 255.255.255.0 10.3.19.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B11" s="13">
+        <v>3</v>
+      </c>
+      <c r="C11" s="7">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="D11" s="8" t="str">
+        <f>_xlfn.CONCAT("172.",B11,".",C11,".0")</f>
+        <v>172.3.10.0</v>
+      </c>
+      <c r="E11" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>3</v>
+      </c>
+      <c r="F11" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>19</v>
+      </c>
+      <c r="G11" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H11" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.3.19.1</v>
+      </c>
+      <c r="I11" t="str">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D11, " ", "255.255.255.0"," ", H11))</f>
+        <v>ip route 172.3.10.0 255.255.255.0 10.3.19.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B12" s="13">
+        <v>3</v>
+      </c>
+      <c r="C12" s="7">
+        <f>C11-1</f>
+        <v>9</v>
+      </c>
+      <c r="D12" s="8" t="str">
+        <f>_xlfn.CONCAT("172.",B12,".",C12,".0")</f>
+        <v>172.3.9.0</v>
+      </c>
+      <c r="E12" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>3</v>
+      </c>
+      <c r="F12" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>19</v>
+      </c>
+      <c r="G12" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H12" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.3.19.1</v>
+      </c>
+      <c r="I12" t="str">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D12, " ", "255.255.255.0"," ", H12))</f>
+        <v>ip route 172.3.9.0 255.255.255.0 10.3.19.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B13" s="13">
+        <v>3</v>
+      </c>
+      <c r="C13" s="7">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="D13" s="8" t="str">
+        <f>_xlfn.CONCAT("172.",B13,".",C13,".0")</f>
+        <v>172.3.8.0</v>
+      </c>
+      <c r="E13" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>3</v>
+      </c>
+      <c r="F13" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>19</v>
+      </c>
+      <c r="G13" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H13" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.3.19.1</v>
+      </c>
+      <c r="I13" t="str">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D13, " ", "255.255.255.0"," ", H13))</f>
+        <v>ip route 172.3.8.0 255.255.255.0 10.3.19.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B14" s="13">
+        <v>3</v>
+      </c>
+      <c r="C14" s="7">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="D14" s="8" t="str">
+        <f>_xlfn.CONCAT("172.",B14,".",C14,".0")</f>
+        <v>172.3.7.0</v>
+      </c>
+      <c r="E14" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>3</v>
+      </c>
+      <c r="F14" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>19</v>
+      </c>
+      <c r="G14" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H14" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.3.19.1</v>
+      </c>
+      <c r="I14" t="str">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D14, " ", "255.255.255.0"," ", H14))</f>
+        <v>ip route 172.3.7.0 255.255.255.0 10.3.19.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B15" s="13">
+        <v>3</v>
+      </c>
+      <c r="C15" s="7">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="D15" s="8" t="str">
+        <f>_xlfn.CONCAT("172.",B15,".",C15,".0")</f>
+        <v>172.3.6.0</v>
+      </c>
+      <c r="E15" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>3</v>
+      </c>
+      <c r="F15" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>19</v>
+      </c>
+      <c r="G15" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H15" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.3.19.1</v>
+      </c>
+      <c r="I15" t="str">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D15, " ", "255.255.255.0"," ", H15))</f>
+        <v>ip route 172.3.6.0 255.255.255.0 10.3.19.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B16" s="13">
+        <v>3</v>
+      </c>
+      <c r="C16" s="7">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="D16" s="8" t="str">
+        <f>_xlfn.CONCAT("172.",B16,".",C16,".0")</f>
+        <v>172.3.5.0</v>
+      </c>
+      <c r="E16" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>3</v>
+      </c>
+      <c r="F16" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>19</v>
+      </c>
+      <c r="G16" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H16" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.3.19.1</v>
+      </c>
+      <c r="I16" t="str">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D16, " ", "255.255.255.0"," ", H16))</f>
+        <v>ip route 172.3.5.0 255.255.255.0 10.3.19.1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B17" s="13">
+        <v>3</v>
+      </c>
+      <c r="C17" s="7">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="D17" s="8" t="str">
+        <f>_xlfn.CONCAT("172.",B17,".",C17,".0")</f>
+        <v>172.3.4.0</v>
+      </c>
+      <c r="E17" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>3</v>
+      </c>
+      <c r="F17" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>19</v>
+      </c>
+      <c r="G17" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H17" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.3.19.1</v>
+      </c>
+      <c r="I17" t="str">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D17, " ", "255.255.255.0"," ", H17))</f>
+        <v>ip route 172.3.4.0 255.255.255.0 10.3.19.1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B18" s="13">
+        <v>3</v>
+      </c>
+      <c r="C18" s="7">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="D18" s="8" t="str">
+        <f>_xlfn.CONCAT("172.",B18,".",C18,".0")</f>
+        <v>172.3.3.0</v>
+      </c>
+      <c r="E18" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>3</v>
+      </c>
+      <c r="F18" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>19</v>
+      </c>
+      <c r="G18" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H18" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.3.19.1</v>
+      </c>
+      <c r="I18" t="str">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D18, " ", "255.255.255.0"," ", H18))</f>
+        <v>ip route 172.3.3.0 255.255.255.0 10.3.19.1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B19" s="13">
+        <v>3</v>
+      </c>
+      <c r="C19" s="7">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="D19" s="8" t="str">
+        <f>_xlfn.CONCAT("172.",B19,".",C19,".0")</f>
+        <v>172.3.2.0</v>
+      </c>
+      <c r="E19" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>3</v>
+      </c>
+      <c r="F19" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>19</v>
+      </c>
+      <c r="G19" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H19" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.3.19.1</v>
+      </c>
+      <c r="I19" t="str">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D19, " ", "255.255.255.0"," ", H19))</f>
+        <v>ip route 172.3.2.0 255.255.255.0 10.3.19.1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B20" s="13">
+        <v>3</v>
+      </c>
+      <c r="C20" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D20" s="8" t="str">
+        <f>_xlfn.CONCAT("172.",B20,".",C20,".0")</f>
+        <v>172.3.1.0</v>
+      </c>
+      <c r="E20" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>3</v>
+      </c>
+      <c r="F20" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>19</v>
+      </c>
+      <c r="G20" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H20" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.3.19.1</v>
+      </c>
+      <c r="I20" t="str">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D20, " ", "255.255.255.0"," ", H20))</f>
+        <v>ip route 172.3.1.0 255.255.255.0 10.3.19.1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B21" s="13">
+        <v>3</v>
+      </c>
+      <c r="C21" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D21" s="8" t="str">
+        <f>_xlfn.CONCAT("172.",B21,".",C21,".0")</f>
+        <v>172.3.0.0</v>
+      </c>
+      <c r="E21" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>3</v>
+      </c>
+      <c r="F21" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>19</v>
+      </c>
+      <c r="G21" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H21" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.3.19.1</v>
+      </c>
+      <c r="I21" t="str">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D21, " ", "255.255.255.0"," ", H21))</f>
+        <v>ip route 172.3.0.0 255.255.255.0 10.3.19.1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B22" s="11">
+        <v>1</v>
+      </c>
+      <c r="C22" s="7">
+        <v>5</v>
+      </c>
+      <c r="D22" s="8" t="str">
+        <f>_xlfn.CONCAT("172.",B22,".",C22,".0")</f>
+        <v>172.1.5.0</v>
+      </c>
+      <c r="E22" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>3</v>
+      </c>
+      <c r="F22" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>19</v>
+      </c>
+      <c r="G22" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H22" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.3.19.1</v>
+      </c>
+      <c r="I22" t="str">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D22, " ", "255.255.255.0"," ", H22))</f>
+        <v>ip route 172.1.5.0 255.255.255.0 10.3.19.1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B23" s="11">
+        <v>1</v>
+      </c>
+      <c r="C23" s="7">
+        <f>C22-1</f>
+        <v>4</v>
+      </c>
+      <c r="D23" s="8" t="str">
+        <f t="shared" ref="D23:D34" si="2">_xlfn.CONCAT("172.",B23,".",C23,".0")</f>
+        <v>172.1.4.0</v>
+      </c>
+      <c r="E23" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>3</v>
+      </c>
+      <c r="F23" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>19</v>
+      </c>
+      <c r="G23" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H23" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.3.19.1</v>
+      </c>
+      <c r="I23" t="str">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D23, " ", "255.255.255.0"," ", H23))</f>
+        <v>ip route 172.1.4.0 255.255.255.0 10.3.19.1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B24" s="11">
+        <v>1</v>
+      </c>
+      <c r="C24" s="7">
+        <f t="shared" ref="C24:C27" si="3">C23-1</f>
+        <v>3</v>
+      </c>
+      <c r="D24" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>172.1.3.0</v>
+      </c>
+      <c r="E24" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>3</v>
+      </c>
+      <c r="F24" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>19</v>
+      </c>
+      <c r="G24" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H24" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.3.19.1</v>
+      </c>
+      <c r="I24" t="str">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D24, " ", "255.255.255.0"," ", H24))</f>
+        <v>ip route 172.1.3.0 255.255.255.0 10.3.19.1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B25" s="11">
+        <v>1</v>
+      </c>
+      <c r="C25" s="7">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D25" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>172.1.2.0</v>
+      </c>
+      <c r="E25" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>3</v>
+      </c>
+      <c r="F25" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>19</v>
+      </c>
+      <c r="G25" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H25" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.3.19.1</v>
+      </c>
+      <c r="I25" t="str">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D25, " ", "255.255.255.0"," ", H25))</f>
+        <v>ip route 172.1.2.0 255.255.255.0 10.3.19.1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B26" s="11">
+        <v>1</v>
+      </c>
+      <c r="C26" s="7">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D26" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>172.1.1.0</v>
+      </c>
+      <c r="E26" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>3</v>
+      </c>
+      <c r="F26" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>19</v>
+      </c>
+      <c r="G26" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H26" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.3.19.1</v>
+      </c>
+      <c r="I26" t="str">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D26, " ", "255.255.255.0"," ", H26))</f>
+        <v>ip route 172.1.1.0 255.255.255.0 10.3.19.1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B27" s="11">
+        <v>1</v>
+      </c>
+      <c r="C27" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D27" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>172.1.0.0</v>
+      </c>
+      <c r="E27" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>3</v>
+      </c>
+      <c r="F27" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>19</v>
+      </c>
+      <c r="G27" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H27" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.3.19.1</v>
+      </c>
+      <c r="I27" t="str">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D27, " ", "255.255.255.0"," ", H27))</f>
+        <v>ip route 172.1.0.0 255.255.255.0 10.3.19.1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B28" s="12">
+        <v>2</v>
+      </c>
+      <c r="C28" s="7">
+        <v>6</v>
+      </c>
+      <c r="D28" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>172.2.6.0</v>
+      </c>
+      <c r="E28" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>3</v>
+      </c>
+      <c r="F28" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>19</v>
+      </c>
+      <c r="G28" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H28" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.3.19.1</v>
+      </c>
+      <c r="I28" t="str">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D28, " ", "255.255.255.0"," ", H28))</f>
+        <v>ip route 172.2.6.0 255.255.255.0 10.3.19.1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B29" s="12">
+        <v>2</v>
+      </c>
+      <c r="C29" s="7">
+        <f>C28-1</f>
+        <v>5</v>
+      </c>
+      <c r="D29" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>172.2.5.0</v>
+      </c>
+      <c r="E29" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>3</v>
+      </c>
+      <c r="F29" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>19</v>
+      </c>
+      <c r="G29" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H29" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.3.19.1</v>
+      </c>
+      <c r="I29" t="str">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D29, " ", "255.255.255.0"," ", H29))</f>
+        <v>ip route 172.2.5.0 255.255.255.0 10.3.19.1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B30" s="12">
+        <v>2</v>
+      </c>
+      <c r="C30" s="7">
+        <f t="shared" ref="C30:C34" si="4">C29-1</f>
+        <v>4</v>
+      </c>
+      <c r="D30" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>172.2.4.0</v>
+      </c>
+      <c r="E30" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>3</v>
+      </c>
+      <c r="F30" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>19</v>
+      </c>
+      <c r="G30" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H30" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.3.19.1</v>
+      </c>
+      <c r="I30" t="str">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D30, " ", "255.255.255.0"," ", H30))</f>
+        <v>ip route 172.2.4.0 255.255.255.0 10.3.19.1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B31" s="12">
+        <v>2</v>
+      </c>
+      <c r="C31" s="7">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="D31" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>172.2.3.0</v>
+      </c>
+      <c r="E31" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>3</v>
+      </c>
+      <c r="F31" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>19</v>
+      </c>
+      <c r="G31" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H31" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.3.19.1</v>
+      </c>
+      <c r="I31" t="str">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D31, " ", "255.255.255.0"," ", H31))</f>
+        <v>ip route 172.2.3.0 255.255.255.0 10.3.19.1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B32" s="12">
+        <v>2</v>
+      </c>
+      <c r="C32" s="7">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="D32" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>172.2.2.0</v>
+      </c>
+      <c r="E32" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>3</v>
+      </c>
+      <c r="F32" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>19</v>
+      </c>
+      <c r="G32" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H32" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.3.19.1</v>
+      </c>
+      <c r="I32" t="str">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D32, " ", "255.255.255.0"," ", H32))</f>
+        <v>ip route 172.2.2.0 255.255.255.0 10.3.19.1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B33" s="12">
+        <v>2</v>
+      </c>
+      <c r="C33" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D33" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>172.2.1.0</v>
+      </c>
+      <c r="E33" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>3</v>
+      </c>
+      <c r="F33" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>19</v>
+      </c>
+      <c r="G33" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H33" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.3.19.1</v>
+      </c>
+      <c r="I33" t="str">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D33, " ", "255.255.255.0"," ", H33))</f>
+        <v>ip route 172.2.1.0 255.255.255.0 10.3.19.1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B34" s="12">
+        <v>2</v>
+      </c>
+      <c r="C34" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D34" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>172.2.0.0</v>
+      </c>
+      <c r="E34" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>3</v>
+      </c>
+      <c r="F34" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>19</v>
+      </c>
+      <c r="G34" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H34" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.3.19.1</v>
+      </c>
+      <c r="I34" t="str">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D34, " ", "255.255.255.0"," ", H34))</f>
+        <v>ip route 172.2.0.0 255.255.255.0 10.3.19.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se termina enrutamiento static en ipv4
</commit_message>
<xml_diff>
--- a/taller-2/Taller#2.xlsx
+++ b/taller-2/Taller#2.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivanbotero/Projects/interconexion/taller-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAAC36B6-6DA0-454A-9284-342CED03E23D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA4EC18-0691-2242-ABD5-747E6816C284}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="0" windowWidth="27320" windowHeight="15360" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25600" yWindow="0" windowWidth="27320" windowHeight="15360" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ipv4" sheetId="1" r:id="rId1"/>
     <sheet name="ipv6" sheetId="2" r:id="rId2"/>
     <sheet name="Enrutamiento4E1" sheetId="3" r:id="rId3"/>
-    <sheet name="Enrutamiento4E3" sheetId="4" r:id="rId4"/>
+    <sheet name="Enrutamiento4E2" sheetId="5" r:id="rId4"/>
+    <sheet name="Enrutamiento4E3" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="37">
   <si>
     <t>#</t>
   </si>
@@ -260,12 +261,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -274,6 +269,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -625,36 +626,36 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:27" ht="18" x14ac:dyDescent="0.2">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="K2" s="9" t="s">
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="K2" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="T2" s="9" t="s">
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
+      <c r="T2" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="U2" s="9"/>
-      <c r="V2" s="9"/>
-      <c r="W2" s="9"/>
-      <c r="X2" s="9"/>
-      <c r="Y2" s="9"/>
-      <c r="Z2" s="9"/>
-      <c r="AA2" s="9"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="12"/>
+      <c r="W2" s="12"/>
+      <c r="X2" s="12"/>
+      <c r="Y2" s="12"/>
+      <c r="Z2" s="12"/>
+      <c r="AA2" s="12"/>
     </row>
     <row r="3" spans="2:27" ht="16" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
@@ -5401,36 +5402,36 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:27" ht="18" x14ac:dyDescent="0.2">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="K2" s="10" t="s">
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="K2" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="T2" s="9" t="s">
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
+      <c r="T2" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="U2" s="9"/>
-      <c r="V2" s="9"/>
-      <c r="W2" s="9"/>
-      <c r="X2" s="9"/>
-      <c r="Y2" s="9"/>
-      <c r="Z2" s="9"/>
-      <c r="AA2" s="9"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="12"/>
+      <c r="W2" s="12"/>
+      <c r="X2" s="12"/>
+      <c r="Y2" s="12"/>
+      <c r="Z2" s="12"/>
+      <c r="AA2" s="12"/>
     </row>
     <row r="3" spans="2:27" ht="16" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
@@ -10007,7 +10008,7 @@
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -10025,7 +10026,7 @@
       <c r="A1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="11">
+      <c r="B1" s="9">
         <v>1</v>
       </c>
       <c r="C1" s="7">
@@ -10052,12 +10053,12 @@
         <v>10.1.4.1</v>
       </c>
       <c r="I1" t="str">
-        <f>IF(MATCH("*",$A$1:$A$34) = ROW(),"",_xlfn.CONCAT("ip route", " ", D1, " ", "255.255.255.0"," ", H1))</f>
-        <v/>
+        <f>IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D1, " ", "255.255.255.0"," ", H1))</f>
+        <v>#</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="11">
+      <c r="B2" s="9">
         <v>1</v>
       </c>
       <c r="C2" s="7">
@@ -10085,12 +10086,12 @@
         <v>10.1.4.1</v>
       </c>
       <c r="I2" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"",_xlfn.CONCAT("ip route", " ", D2, " ", "255.255.255.0"," ", H2))</f>
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D2, " ", "255.255.255.0"," ", H2))</f>
         <v>ip route 172.1.4.0 255.255.255.0 10.1.4.1</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="11">
+      <c r="B3" s="9">
         <v>1</v>
       </c>
       <c r="C3" s="7">
@@ -10118,12 +10119,12 @@
         <v>10.1.4.1</v>
       </c>
       <c r="I3" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"",_xlfn.CONCAT("ip route", " ", D3, " ", "255.255.255.0"," ", H3))</f>
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D3, " ", "255.255.255.0"," ", H3))</f>
         <v>ip route 172.1.3.0 255.255.255.0 10.1.4.1</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="11">
+      <c r="B4" s="9">
         <v>1</v>
       </c>
       <c r="C4" s="7">
@@ -10151,12 +10152,12 @@
         <v>10.1.4.1</v>
       </c>
       <c r="I4" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"",_xlfn.CONCAT("ip route", " ", D4, " ", "255.255.255.0"," ", H4))</f>
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D4, " ", "255.255.255.0"," ", H4))</f>
         <v>ip route 172.1.2.0 255.255.255.0 10.1.4.1</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="11">
+      <c r="B5" s="9">
         <v>1</v>
       </c>
       <c r="C5" s="7">
@@ -10184,12 +10185,12 @@
         <v>10.1.4.1</v>
       </c>
       <c r="I5" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"",_xlfn.CONCAT("ip route", " ", D5, " ", "255.255.255.0"," ", H5))</f>
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D5, " ", "255.255.255.0"," ", H5))</f>
         <v>ip route 172.1.1.0 255.255.255.0 10.1.4.1</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="11">
+      <c r="B6" s="9">
         <v>1</v>
       </c>
       <c r="C6" s="7">
@@ -10217,19 +10218,19 @@
         <v>10.1.4.1</v>
       </c>
       <c r="I6" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"",_xlfn.CONCAT("ip route", " ", D6, " ", "255.255.255.0"," ", H6))</f>
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D6, " ", "255.255.255.0"," ", H6))</f>
         <v>ip route 172.1.0.0 255.255.255.0 10.1.4.1</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="12">
+      <c r="B7" s="10">
         <v>2</v>
       </c>
       <c r="C7" s="7">
         <v>6</v>
       </c>
       <c r="D7" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("172.",B7,".",C7,".0")</f>
         <v>172.2.6.0</v>
       </c>
       <c r="E7" s="8">
@@ -10245,16 +10246,16 @@
         <v>1</v>
       </c>
       <c r="H7" s="8" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">_xlfn.CONCAT("10.",E7,".",F7,".",G7)</f>
         <v>10.1.4.1</v>
       </c>
       <c r="I7" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"",_xlfn.CONCAT("ip route", " ", D7, " ", "255.255.255.0"," ", H7))</f>
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D7, " ", "255.255.255.0"," ", H7))</f>
         <v>ip route 172.2.6.0 255.255.255.0 10.1.4.1</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B8" s="12">
+      <c r="B8" s="10">
         <v>2</v>
       </c>
       <c r="C8" s="7">
@@ -10262,7 +10263,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("172.",B8,".",C8,".0")</f>
         <v>172.2.5.0</v>
       </c>
       <c r="E8" s="8">
@@ -10278,24 +10279,24 @@
         <v>1</v>
       </c>
       <c r="H8" s="8" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">_xlfn.CONCAT("10.",E8,".",F8,".",G8)</f>
         <v>10.1.4.1</v>
       </c>
       <c r="I8" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"",_xlfn.CONCAT("ip route", " ", D8, " ", "255.255.255.0"," ", H8))</f>
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D8, " ", "255.255.255.0"," ", H8))</f>
         <v>ip route 172.2.5.0 255.255.255.0 10.1.4.1</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B9" s="12">
+      <c r="B9" s="10">
         <v>2</v>
       </c>
       <c r="C9" s="7">
-        <f t="shared" ref="C9:C13" si="3">C8-1</f>
+        <f>C8-1</f>
         <v>4</v>
       </c>
       <c r="D9" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("172.",B9,".",C9,".0")</f>
         <v>172.2.4.0</v>
       </c>
       <c r="E9" s="8">
@@ -10311,24 +10312,24 @@
         <v>1</v>
       </c>
       <c r="H9" s="8" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">_xlfn.CONCAT("10.",E9,".",F9,".",G9)</f>
         <v>10.1.4.1</v>
       </c>
       <c r="I9" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"",_xlfn.CONCAT("ip route", " ", D9, " ", "255.255.255.0"," ", H9))</f>
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D9, " ", "255.255.255.0"," ", H9))</f>
         <v>ip route 172.2.4.0 255.255.255.0 10.1.4.1</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="12">
+      <c r="B10" s="10">
         <v>2</v>
       </c>
       <c r="C10" s="7">
-        <f t="shared" si="3"/>
+        <f>C9-1</f>
         <v>3</v>
       </c>
       <c r="D10" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("172.",B10,".",C10,".0")</f>
         <v>172.2.3.0</v>
       </c>
       <c r="E10" s="8">
@@ -10344,24 +10345,24 @@
         <v>1</v>
       </c>
       <c r="H10" s="8" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">_xlfn.CONCAT("10.",E10,".",F10,".",G10)</f>
         <v>10.1.4.1</v>
       </c>
       <c r="I10" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"",_xlfn.CONCAT("ip route", " ", D10, " ", "255.255.255.0"," ", H10))</f>
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D10, " ", "255.255.255.0"," ", H10))</f>
         <v>ip route 172.2.3.0 255.255.255.0 10.1.4.1</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="12">
+      <c r="B11" s="10">
         <v>2</v>
       </c>
       <c r="C11" s="7">
-        <f t="shared" si="3"/>
+        <f>C10-1</f>
         <v>2</v>
       </c>
       <c r="D11" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("172.",B11,".",C11,".0")</f>
         <v>172.2.2.0</v>
       </c>
       <c r="E11" s="8">
@@ -10377,24 +10378,24 @@
         <v>1</v>
       </c>
       <c r="H11" s="8" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">_xlfn.CONCAT("10.",E11,".",F11,".",G11)</f>
         <v>10.1.4.1</v>
       </c>
       <c r="I11" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"",_xlfn.CONCAT("ip route", " ", D11, " ", "255.255.255.0"," ", H11))</f>
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D11, " ", "255.255.255.0"," ", H11))</f>
         <v>ip route 172.2.2.0 255.255.255.0 10.1.4.1</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="12">
+      <c r="B12" s="10">
         <v>2</v>
       </c>
       <c r="C12" s="7">
-        <f t="shared" si="3"/>
+        <f>C11-1</f>
         <v>1</v>
       </c>
       <c r="D12" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("172.",B12,".",C12,".0")</f>
         <v>172.2.1.0</v>
       </c>
       <c r="E12" s="8">
@@ -10410,24 +10411,24 @@
         <v>1</v>
       </c>
       <c r="H12" s="8" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">_xlfn.CONCAT("10.",E12,".",F12,".",G12)</f>
         <v>10.1.4.1</v>
       </c>
       <c r="I12" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"",_xlfn.CONCAT("ip route", " ", D12, " ", "255.255.255.0"," ", H12))</f>
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D12, " ", "255.255.255.0"," ", H12))</f>
         <v>ip route 172.2.1.0 255.255.255.0 10.1.4.1</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B13" s="12">
+      <c r="B13" s="10">
         <v>2</v>
       </c>
       <c r="C13" s="7">
-        <f t="shared" si="3"/>
+        <f>C12-1</f>
         <v>0</v>
       </c>
       <c r="D13" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("172.",B13,".",C13,".0")</f>
         <v>172.2.0.0</v>
       </c>
       <c r="E13" s="8">
@@ -10443,16 +10444,16 @@
         <v>1</v>
       </c>
       <c r="H13" s="8" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">_xlfn.CONCAT("10.",E13,".",F13,".",G13)</f>
         <v>10.1.4.1</v>
       </c>
       <c r="I13" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"",_xlfn.CONCAT("ip route", " ", D13, " ", "255.255.255.0"," ", H13))</f>
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D13, " ", "255.255.255.0"," ", H13))</f>
         <v>ip route 172.2.0.0 255.255.255.0 10.1.4.1</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="13">
+      <c r="B14" s="11">
         <v>3</v>
       </c>
       <c r="C14" s="7">
@@ -10479,12 +10480,12 @@
         <v>10.1.4.1</v>
       </c>
       <c r="I14" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"",_xlfn.CONCAT("ip route", " ", D14, " ", "255.255.255.0"," ", H14))</f>
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D14, " ", "255.255.255.0"," ", H14))</f>
         <v>ip route 172.3.20.0 255.255.255.0 10.1.4.1</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B15" s="13">
+      <c r="B15" s="11">
         <v>3</v>
       </c>
       <c r="C15" s="7">
@@ -10512,16 +10513,16 @@
         <v>10.1.4.1</v>
       </c>
       <c r="I15" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"",_xlfn.CONCAT("ip route", " ", D15, " ", "255.255.255.0"," ", H15))</f>
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D15, " ", "255.255.255.0"," ", H15))</f>
         <v>ip route 172.3.19.0 255.255.255.0 10.1.4.1</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B16" s="13">
+      <c r="B16" s="11">
         <v>3</v>
       </c>
       <c r="C16" s="7">
-        <f t="shared" ref="C16:C34" si="4">C15-1</f>
+        <f t="shared" ref="C16:C34" si="3">C15-1</f>
         <v>18</v>
       </c>
       <c r="D16" s="8" t="str">
@@ -10545,16 +10546,16 @@
         <v>10.1.4.1</v>
       </c>
       <c r="I16" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"",_xlfn.CONCAT("ip route", " ", D16, " ", "255.255.255.0"," ", H16))</f>
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D16, " ", "255.255.255.0"," ", H16))</f>
         <v>ip route 172.3.18.0 255.255.255.0 10.1.4.1</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B17" s="13">
+      <c r="B17" s="11">
         <v>3</v>
       </c>
       <c r="C17" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="D17" s="8" t="str">
@@ -10578,16 +10579,16 @@
         <v>10.1.4.1</v>
       </c>
       <c r="I17" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"",_xlfn.CONCAT("ip route", " ", D17, " ", "255.255.255.0"," ", H17))</f>
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D17, " ", "255.255.255.0"," ", H17))</f>
         <v>ip route 172.3.17.0 255.255.255.0 10.1.4.1</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B18" s="13">
+      <c r="B18" s="11">
         <v>3</v>
       </c>
       <c r="C18" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="D18" s="8" t="str">
@@ -10611,16 +10612,16 @@
         <v>10.1.4.1</v>
       </c>
       <c r="I18" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"",_xlfn.CONCAT("ip route", " ", D18, " ", "255.255.255.0"," ", H18))</f>
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D18, " ", "255.255.255.0"," ", H18))</f>
         <v>ip route 172.3.16.0 255.255.255.0 10.1.4.1</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B19" s="13">
+      <c r="B19" s="11">
         <v>3</v>
       </c>
       <c r="C19" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="D19" s="8" t="str">
@@ -10644,16 +10645,16 @@
         <v>10.1.4.1</v>
       </c>
       <c r="I19" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"",_xlfn.CONCAT("ip route", " ", D19, " ", "255.255.255.0"," ", H19))</f>
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D19, " ", "255.255.255.0"," ", H19))</f>
         <v>ip route 172.3.15.0 255.255.255.0 10.1.4.1</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B20" s="13">
+      <c r="B20" s="11">
         <v>3</v>
       </c>
       <c r="C20" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="D20" s="8" t="str">
@@ -10677,16 +10678,16 @@
         <v>10.1.4.1</v>
       </c>
       <c r="I20" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"",_xlfn.CONCAT("ip route", " ", D20, " ", "255.255.255.0"," ", H20))</f>
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D20, " ", "255.255.255.0"," ", H20))</f>
         <v>ip route 172.3.14.0 255.255.255.0 10.1.4.1</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B21" s="13">
+      <c r="B21" s="11">
         <v>3</v>
       </c>
       <c r="C21" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="D21" s="8" t="str">
@@ -10710,16 +10711,16 @@
         <v>10.1.4.1</v>
       </c>
       <c r="I21" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"",_xlfn.CONCAT("ip route", " ", D21, " ", "255.255.255.0"," ", H21))</f>
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D21, " ", "255.255.255.0"," ", H21))</f>
         <v>ip route 172.3.13.0 255.255.255.0 10.1.4.1</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B22" s="13">
+      <c r="B22" s="11">
         <v>3</v>
       </c>
       <c r="C22" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="D22" s="8" t="str">
@@ -10743,16 +10744,16 @@
         <v>10.1.4.1</v>
       </c>
       <c r="I22" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"",_xlfn.CONCAT("ip route", " ", D22, " ", "255.255.255.0"," ", H22))</f>
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D22, " ", "255.255.255.0"," ", H22))</f>
         <v>ip route 172.3.12.0 255.255.255.0 10.1.4.1</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B23" s="13">
+      <c r="B23" s="11">
         <v>3</v>
       </c>
       <c r="C23" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="D23" s="8" t="str">
@@ -10776,16 +10777,16 @@
         <v>10.1.4.1</v>
       </c>
       <c r="I23" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"",_xlfn.CONCAT("ip route", " ", D23, " ", "255.255.255.0"," ", H23))</f>
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D23, " ", "255.255.255.0"," ", H23))</f>
         <v>ip route 172.3.11.0 255.255.255.0 10.1.4.1</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B24" s="13">
+      <c r="B24" s="11">
         <v>3</v>
       </c>
       <c r="C24" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="D24" s="8" t="str">
@@ -10809,12 +10810,12 @@
         <v>10.1.4.1</v>
       </c>
       <c r="I24" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"",_xlfn.CONCAT("ip route", " ", D24, " ", "255.255.255.0"," ", H24))</f>
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D24, " ", "255.255.255.0"," ", H24))</f>
         <v>ip route 172.3.10.0 255.255.255.0 10.1.4.1</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B25" s="13">
+      <c r="B25" s="11">
         <v>3</v>
       </c>
       <c r="C25" s="7">
@@ -10842,16 +10843,16 @@
         <v>10.1.4.1</v>
       </c>
       <c r="I25" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"",_xlfn.CONCAT("ip route", " ", D25, " ", "255.255.255.0"," ", H25))</f>
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D25, " ", "255.255.255.0"," ", H25))</f>
         <v>ip route 172.3.9.0 255.255.255.0 10.1.4.1</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B26" s="13">
+      <c r="B26" s="11">
         <v>3</v>
       </c>
       <c r="C26" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="D26" s="8" t="str">
@@ -10875,16 +10876,16 @@
         <v>10.1.4.1</v>
       </c>
       <c r="I26" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"",_xlfn.CONCAT("ip route", " ", D26, " ", "255.255.255.0"," ", H26))</f>
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D26, " ", "255.255.255.0"," ", H26))</f>
         <v>ip route 172.3.8.0 255.255.255.0 10.1.4.1</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B27" s="13">
+      <c r="B27" s="11">
         <v>3</v>
       </c>
       <c r="C27" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="D27" s="8" t="str">
@@ -10908,16 +10909,16 @@
         <v>10.1.4.1</v>
       </c>
       <c r="I27" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"",_xlfn.CONCAT("ip route", " ", D27, " ", "255.255.255.0"," ", H27))</f>
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D27, " ", "255.255.255.0"," ", H27))</f>
         <v>ip route 172.3.7.0 255.255.255.0 10.1.4.1</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B28" s="13">
+      <c r="B28" s="11">
         <v>3</v>
       </c>
       <c r="C28" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="D28" s="8" t="str">
@@ -10941,16 +10942,16 @@
         <v>10.1.4.1</v>
       </c>
       <c r="I28" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"",_xlfn.CONCAT("ip route", " ", D28, " ", "255.255.255.0"," ", H28))</f>
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D28, " ", "255.255.255.0"," ", H28))</f>
         <v>ip route 172.3.6.0 255.255.255.0 10.1.4.1</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B29" s="13">
+      <c r="B29" s="11">
         <v>3</v>
       </c>
       <c r="C29" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="D29" s="8" t="str">
@@ -10974,16 +10975,16 @@
         <v>10.1.4.1</v>
       </c>
       <c r="I29" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"",_xlfn.CONCAT("ip route", " ", D29, " ", "255.255.255.0"," ", H29))</f>
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D29, " ", "255.255.255.0"," ", H29))</f>
         <v>ip route 172.3.5.0 255.255.255.0 10.1.4.1</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B30" s="13">
+      <c r="B30" s="11">
         <v>3</v>
       </c>
       <c r="C30" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="D30" s="8" t="str">
@@ -11007,16 +11008,16 @@
         <v>10.1.4.1</v>
       </c>
       <c r="I30" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"",_xlfn.CONCAT("ip route", " ", D30, " ", "255.255.255.0"," ", H30))</f>
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D30, " ", "255.255.255.0"," ", H30))</f>
         <v>ip route 172.3.4.0 255.255.255.0 10.1.4.1</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B31" s="13">
+      <c r="B31" s="11">
         <v>3</v>
       </c>
       <c r="C31" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="D31" s="8" t="str">
@@ -11040,16 +11041,16 @@
         <v>10.1.4.1</v>
       </c>
       <c r="I31" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"",_xlfn.CONCAT("ip route", " ", D31, " ", "255.255.255.0"," ", H31))</f>
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D31, " ", "255.255.255.0"," ", H31))</f>
         <v>ip route 172.3.3.0 255.255.255.0 10.1.4.1</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B32" s="13">
+      <c r="B32" s="11">
         <v>3</v>
       </c>
       <c r="C32" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="D32" s="8" t="str">
@@ -11073,16 +11074,16 @@
         <v>10.1.4.1</v>
       </c>
       <c r="I32" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"",_xlfn.CONCAT("ip route", " ", D32, " ", "255.255.255.0"," ", H32))</f>
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D32, " ", "255.255.255.0"," ", H32))</f>
         <v>ip route 172.3.2.0 255.255.255.0 10.1.4.1</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B33" s="13">
+      <c r="B33" s="11">
         <v>3</v>
       </c>
       <c r="C33" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="D33" s="8" t="str">
@@ -11106,16 +11107,16 @@
         <v>10.1.4.1</v>
       </c>
       <c r="I33" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"",_xlfn.CONCAT("ip route", " ", D33, " ", "255.255.255.0"," ", H33))</f>
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D33, " ", "255.255.255.0"," ", H33))</f>
         <v>ip route 172.3.1.0 255.255.255.0 10.1.4.1</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B34" s="13">
+      <c r="B34" s="11">
         <v>3</v>
       </c>
       <c r="C34" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D34" s="8" t="str">
@@ -11139,7 +11140,7 @@
         <v>10.1.4.1</v>
       </c>
       <c r="I34" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"",_xlfn.CONCAT("ip route", " ", D34, " ", "255.255.255.0"," ", H34))</f>
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D34, " ", "255.255.255.0"," ", H34))</f>
         <v>ip route 172.3.0.0 255.255.255.0 10.1.4.1</v>
       </c>
     </row>
@@ -11149,11 +11150,1157 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15AC86ED-47EC-674C-9F96-A9C20BDB7D73}">
+  <dimension ref="A1:I34"/>
+  <sheetViews>
+    <sheetView topLeftCell="A20" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.33203125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="2.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="2.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="10">
+        <v>2</v>
+      </c>
+      <c r="C1" s="7">
+        <v>6</v>
+      </c>
+      <c r="D1" s="8" t="str">
+        <f>_xlfn.CONCAT("172.",B1,".",C1,".0")</f>
+        <v>172.2.6.0</v>
+      </c>
+      <c r="E1" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>2</v>
+      </c>
+      <c r="F1" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>5</v>
+      </c>
+      <c r="G1" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H1" s="8" t="str">
+        <f ca="1">_xlfn.CONCAT("10.",E1,".",F1,".",G1)</f>
+        <v>10.2.5.1</v>
+      </c>
+      <c r="I1" t="str">
+        <f>IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D1, " ", "255.255.255.0"," ", H1))</f>
+        <v>#</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B2" s="10">
+        <v>2</v>
+      </c>
+      <c r="C2" s="7">
+        <f>C1-1</f>
+        <v>5</v>
+      </c>
+      <c r="D2" s="8" t="str">
+        <f>_xlfn.CONCAT("172.",B2,".",C2,".0")</f>
+        <v>172.2.5.0</v>
+      </c>
+      <c r="E2" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>2</v>
+      </c>
+      <c r="F2" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>5</v>
+      </c>
+      <c r="G2" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H2" s="8" t="str">
+        <f t="shared" ref="H2:H34" ca="1" si="0">_xlfn.CONCAT("10.",E2,".",F2,".",G2)</f>
+        <v>10.2.5.1</v>
+      </c>
+      <c r="I2" t="str">
+        <f t="shared" ref="I2:I34" ca="1" si="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D2, " ", "255.255.255.0"," ", H2))</f>
+        <v>ip route 172.2.5.0 255.255.255.0 10.2.5.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B3" s="10">
+        <v>2</v>
+      </c>
+      <c r="C3" s="7">
+        <f>C2-1</f>
+        <v>4</v>
+      </c>
+      <c r="D3" s="8" t="str">
+        <f>_xlfn.CONCAT("172.",B3,".",C3,".0")</f>
+        <v>172.2.4.0</v>
+      </c>
+      <c r="E3" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>2</v>
+      </c>
+      <c r="F3" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>5</v>
+      </c>
+      <c r="G3" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H3" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.2.5.1</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>ip route 172.2.4.0 255.255.255.0 10.2.5.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B4" s="10">
+        <v>2</v>
+      </c>
+      <c r="C4" s="7">
+        <f>C3-1</f>
+        <v>3</v>
+      </c>
+      <c r="D4" s="8" t="str">
+        <f>_xlfn.CONCAT("172.",B4,".",C4,".0")</f>
+        <v>172.2.3.0</v>
+      </c>
+      <c r="E4" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>2</v>
+      </c>
+      <c r="F4" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>5</v>
+      </c>
+      <c r="G4" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H4" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.2.5.1</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>ip route 172.2.3.0 255.255.255.0 10.2.5.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B5" s="10">
+        <v>2</v>
+      </c>
+      <c r="C5" s="7">
+        <f>C4-1</f>
+        <v>2</v>
+      </c>
+      <c r="D5" s="8" t="str">
+        <f>_xlfn.CONCAT("172.",B5,".",C5,".0")</f>
+        <v>172.2.2.0</v>
+      </c>
+      <c r="E5" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>2</v>
+      </c>
+      <c r="F5" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>5</v>
+      </c>
+      <c r="G5" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H5" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.2.5.1</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>ip route 172.2.2.0 255.255.255.0 10.2.5.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B6" s="10">
+        <v>2</v>
+      </c>
+      <c r="C6" s="7">
+        <f>C5-1</f>
+        <v>1</v>
+      </c>
+      <c r="D6" s="8" t="str">
+        <f>_xlfn.CONCAT("172.",B6,".",C6,".0")</f>
+        <v>172.2.1.0</v>
+      </c>
+      <c r="E6" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>2</v>
+      </c>
+      <c r="F6" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>5</v>
+      </c>
+      <c r="G6" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H6" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.2.5.1</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>ip route 172.2.1.0 255.255.255.0 10.2.5.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B7" s="10">
+        <v>2</v>
+      </c>
+      <c r="C7" s="7">
+        <f>C6-1</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="8" t="str">
+        <f>_xlfn.CONCAT("172.",B7,".",C7,".0")</f>
+        <v>172.2.0.0</v>
+      </c>
+      <c r="E7" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>2</v>
+      </c>
+      <c r="F7" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>5</v>
+      </c>
+      <c r="G7" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H7" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.2.5.1</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>ip route 172.2.0.0 255.255.255.0 10.2.5.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B8" s="9">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7">
+        <v>5</v>
+      </c>
+      <c r="D8" s="8" t="str">
+        <f>_xlfn.CONCAT("172.",B8,".",C8,".0")</f>
+        <v>172.1.5.0</v>
+      </c>
+      <c r="E8" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>2</v>
+      </c>
+      <c r="F8" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>5</v>
+      </c>
+      <c r="G8" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H8" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.2.5.1</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>ip route 172.1.5.0 255.255.255.0 10.2.5.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B9" s="9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="7">
+        <f>C8-1</f>
+        <v>4</v>
+      </c>
+      <c r="D9" s="8" t="str">
+        <f t="shared" ref="D9:D34" si="2">_xlfn.CONCAT("172.",B9,".",C9,".0")</f>
+        <v>172.1.4.0</v>
+      </c>
+      <c r="E9" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>2</v>
+      </c>
+      <c r="F9" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>5</v>
+      </c>
+      <c r="G9" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H9" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.2.5.1</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>ip route 172.1.4.0 255.255.255.0 10.2.5.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B10" s="9">
+        <v>1</v>
+      </c>
+      <c r="C10" s="7">
+        <f t="shared" ref="C10:C13" si="3">C9-1</f>
+        <v>3</v>
+      </c>
+      <c r="D10" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>172.1.3.0</v>
+      </c>
+      <c r="E10" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>2</v>
+      </c>
+      <c r="F10" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>5</v>
+      </c>
+      <c r="G10" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H10" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.2.5.1</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>ip route 172.1.3.0 255.255.255.0 10.2.5.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B11" s="9">
+        <v>1</v>
+      </c>
+      <c r="C11" s="7">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D11" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>172.1.2.0</v>
+      </c>
+      <c r="E11" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>2</v>
+      </c>
+      <c r="F11" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>5</v>
+      </c>
+      <c r="G11" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H11" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.2.5.1</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>ip route 172.1.2.0 255.255.255.0 10.2.5.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B12" s="9">
+        <v>1</v>
+      </c>
+      <c r="C12" s="7">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D12" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>172.1.1.0</v>
+      </c>
+      <c r="E12" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>2</v>
+      </c>
+      <c r="F12" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>5</v>
+      </c>
+      <c r="G12" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H12" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.2.5.1</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>ip route 172.1.1.0 255.255.255.0 10.2.5.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B13" s="9">
+        <v>1</v>
+      </c>
+      <c r="C13" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D13" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>172.1.0.0</v>
+      </c>
+      <c r="E13" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>2</v>
+      </c>
+      <c r="F13" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>5</v>
+      </c>
+      <c r="G13" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H13" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.2.5.1</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>ip route 172.1.0.0 255.255.255.0 10.2.5.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B14" s="11">
+        <v>3</v>
+      </c>
+      <c r="C14" s="7">
+        <v>20</v>
+      </c>
+      <c r="D14" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>172.3.20.0</v>
+      </c>
+      <c r="E14" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>2</v>
+      </c>
+      <c r="F14" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>5</v>
+      </c>
+      <c r="G14" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H14" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.2.5.1</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>ip route 172.3.20.0 255.255.255.0 10.2.5.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B15" s="11">
+        <v>3</v>
+      </c>
+      <c r="C15" s="7">
+        <f>C14-1</f>
+        <v>19</v>
+      </c>
+      <c r="D15" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>172.3.19.0</v>
+      </c>
+      <c r="E15" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>2</v>
+      </c>
+      <c r="F15" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>5</v>
+      </c>
+      <c r="G15" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H15" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.2.5.1</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>ip route 172.3.19.0 255.255.255.0 10.2.5.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B16" s="11">
+        <v>3</v>
+      </c>
+      <c r="C16" s="7">
+        <f t="shared" ref="C16:C34" si="4">C15-1</f>
+        <v>18</v>
+      </c>
+      <c r="D16" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>172.3.18.0</v>
+      </c>
+      <c r="E16" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>2</v>
+      </c>
+      <c r="F16" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>5</v>
+      </c>
+      <c r="G16" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H16" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.2.5.1</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>ip route 172.3.18.0 255.255.255.0 10.2.5.1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B17" s="11">
+        <v>3</v>
+      </c>
+      <c r="C17" s="7">
+        <f t="shared" si="4"/>
+        <v>17</v>
+      </c>
+      <c r="D17" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>172.3.17.0</v>
+      </c>
+      <c r="E17" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>2</v>
+      </c>
+      <c r="F17" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>5</v>
+      </c>
+      <c r="G17" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H17" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.2.5.1</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>ip route 172.3.17.0 255.255.255.0 10.2.5.1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B18" s="11">
+        <v>3</v>
+      </c>
+      <c r="C18" s="7">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="D18" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>172.3.16.0</v>
+      </c>
+      <c r="E18" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>2</v>
+      </c>
+      <c r="F18" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>5</v>
+      </c>
+      <c r="G18" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H18" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.2.5.1</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>ip route 172.3.16.0 255.255.255.0 10.2.5.1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B19" s="11">
+        <v>3</v>
+      </c>
+      <c r="C19" s="7">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="D19" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>172.3.15.0</v>
+      </c>
+      <c r="E19" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>2</v>
+      </c>
+      <c r="F19" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>5</v>
+      </c>
+      <c r="G19" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H19" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.2.5.1</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>ip route 172.3.15.0 255.255.255.0 10.2.5.1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B20" s="11">
+        <v>3</v>
+      </c>
+      <c r="C20" s="7">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="D20" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>172.3.14.0</v>
+      </c>
+      <c r="E20" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>2</v>
+      </c>
+      <c r="F20" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>5</v>
+      </c>
+      <c r="G20" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H20" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.2.5.1</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>ip route 172.3.14.0 255.255.255.0 10.2.5.1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B21" s="11">
+        <v>3</v>
+      </c>
+      <c r="C21" s="7">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="D21" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>172.3.13.0</v>
+      </c>
+      <c r="E21" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>2</v>
+      </c>
+      <c r="F21" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>5</v>
+      </c>
+      <c r="G21" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H21" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.2.5.1</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>ip route 172.3.13.0 255.255.255.0 10.2.5.1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B22" s="11">
+        <v>3</v>
+      </c>
+      <c r="C22" s="7">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="D22" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>172.3.12.0</v>
+      </c>
+      <c r="E22" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>2</v>
+      </c>
+      <c r="F22" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>5</v>
+      </c>
+      <c r="G22" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H22" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.2.5.1</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>ip route 172.3.12.0 255.255.255.0 10.2.5.1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B23" s="11">
+        <v>3</v>
+      </c>
+      <c r="C23" s="7">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="D23" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>172.3.11.0</v>
+      </c>
+      <c r="E23" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>2</v>
+      </c>
+      <c r="F23" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>5</v>
+      </c>
+      <c r="G23" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H23" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.2.5.1</v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>ip route 172.3.11.0 255.255.255.0 10.2.5.1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B24" s="11">
+        <v>3</v>
+      </c>
+      <c r="C24" s="7">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="D24" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>172.3.10.0</v>
+      </c>
+      <c r="E24" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>2</v>
+      </c>
+      <c r="F24" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>5</v>
+      </c>
+      <c r="G24" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H24" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.2.5.1</v>
+      </c>
+      <c r="I24" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>ip route 172.3.10.0 255.255.255.0 10.2.5.1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B25" s="11">
+        <v>3</v>
+      </c>
+      <c r="C25" s="7">
+        <f>C24-1</f>
+        <v>9</v>
+      </c>
+      <c r="D25" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>172.3.9.0</v>
+      </c>
+      <c r="E25" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>2</v>
+      </c>
+      <c r="F25" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>5</v>
+      </c>
+      <c r="G25" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H25" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.2.5.1</v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>ip route 172.3.9.0 255.255.255.0 10.2.5.1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B26" s="11">
+        <v>3</v>
+      </c>
+      <c r="C26" s="7">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="D26" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>172.3.8.0</v>
+      </c>
+      <c r="E26" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>2</v>
+      </c>
+      <c r="F26" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>5</v>
+      </c>
+      <c r="G26" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H26" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.2.5.1</v>
+      </c>
+      <c r="I26" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>ip route 172.3.8.0 255.255.255.0 10.2.5.1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B27" s="11">
+        <v>3</v>
+      </c>
+      <c r="C27" s="7">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="D27" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>172.3.7.0</v>
+      </c>
+      <c r="E27" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>2</v>
+      </c>
+      <c r="F27" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>5</v>
+      </c>
+      <c r="G27" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H27" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.2.5.1</v>
+      </c>
+      <c r="I27" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>ip route 172.3.7.0 255.255.255.0 10.2.5.1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B28" s="11">
+        <v>3</v>
+      </c>
+      <c r="C28" s="7">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="D28" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>172.3.6.0</v>
+      </c>
+      <c r="E28" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>2</v>
+      </c>
+      <c r="F28" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>5</v>
+      </c>
+      <c r="G28" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H28" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.2.5.1</v>
+      </c>
+      <c r="I28" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>ip route 172.3.6.0 255.255.255.0 10.2.5.1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B29" s="11">
+        <v>3</v>
+      </c>
+      <c r="C29" s="7">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="D29" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>172.3.5.0</v>
+      </c>
+      <c r="E29" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>2</v>
+      </c>
+      <c r="F29" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>5</v>
+      </c>
+      <c r="G29" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H29" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.2.5.1</v>
+      </c>
+      <c r="I29" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>ip route 172.3.5.0 255.255.255.0 10.2.5.1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B30" s="11">
+        <v>3</v>
+      </c>
+      <c r="C30" s="7">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="D30" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>172.3.4.0</v>
+      </c>
+      <c r="E30" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>2</v>
+      </c>
+      <c r="F30" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>5</v>
+      </c>
+      <c r="G30" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H30" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.2.5.1</v>
+      </c>
+      <c r="I30" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>ip route 172.3.4.0 255.255.255.0 10.2.5.1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B31" s="11">
+        <v>3</v>
+      </c>
+      <c r="C31" s="7">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="D31" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>172.3.3.0</v>
+      </c>
+      <c r="E31" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>2</v>
+      </c>
+      <c r="F31" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>5</v>
+      </c>
+      <c r="G31" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H31" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.2.5.1</v>
+      </c>
+      <c r="I31" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>ip route 172.3.3.0 255.255.255.0 10.2.5.1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B32" s="11">
+        <v>3</v>
+      </c>
+      <c r="C32" s="7">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="D32" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>172.3.2.0</v>
+      </c>
+      <c r="E32" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>2</v>
+      </c>
+      <c r="F32" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>5</v>
+      </c>
+      <c r="G32" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H32" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.2.5.1</v>
+      </c>
+      <c r="I32" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>ip route 172.3.2.0 255.255.255.0 10.2.5.1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B33" s="11">
+        <v>3</v>
+      </c>
+      <c r="C33" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D33" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>172.3.1.0</v>
+      </c>
+      <c r="E33" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>2</v>
+      </c>
+      <c r="F33" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>5</v>
+      </c>
+      <c r="G33" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H33" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.2.5.1</v>
+      </c>
+      <c r="I33" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>ip route 172.3.1.0 255.255.255.0 10.2.5.1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B34" s="11">
+        <v>3</v>
+      </c>
+      <c r="C34" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D34" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>172.3.0.0</v>
+      </c>
+      <c r="E34" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>2</v>
+      </c>
+      <c r="F34" s="8">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>5</v>
+      </c>
+      <c r="G34" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H34" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.2.5.1</v>
+      </c>
+      <c r="I34" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>ip route 172.3.0.0 255.255.255.0 10.2.5.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C40AFAA-8036-5748-A687-D4A954FCC149}">
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -11173,26 +12320,26 @@
       <c r="A1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="13">
+      <c r="B1" s="11">
         <v>3</v>
       </c>
       <c r="C1" s="7">
         <v>20</v>
       </c>
       <c r="D1" s="8" t="str">
-        <f>_xlfn.CONCAT("172.",B1,".",C1,".0")</f>
+        <f t="shared" ref="D1:D22" si="0">_xlfn.CONCAT("172.",B1,".",C1,".0")</f>
         <v>172.3.20.0</v>
       </c>
       <c r="E1" s="8">
-        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <f t="shared" ref="E1:E34" ca="1" si="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
         <v>3</v>
       </c>
       <c r="F1" s="8">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <f t="shared" ref="F1:F34" ca="1" si="2">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
         <v>19</v>
       </c>
       <c r="G1" s="8">
-        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <f t="shared" ref="G1:G34" si="3">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
         <v>1</v>
       </c>
       <c r="H1" s="8" t="str">
@@ -11200,12 +12347,12 @@
         <v>10.3.19.1</v>
       </c>
       <c r="I1" t="str">
-        <f>IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D1, " ", "255.255.255.0"," ", H1))</f>
+        <f t="shared" ref="I1:I34" si="4">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D1, " ", "255.255.255.0"," ", H1))</f>
         <v>#</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="13">
+      <c r="B2" s="11">
         <v>3</v>
       </c>
       <c r="C2" s="7">
@@ -11213,329 +12360,329 @@
         <v>19</v>
       </c>
       <c r="D2" s="8" t="str">
-        <f>_xlfn.CONCAT("172.",B2,".",C2,".0")</f>
+        <f t="shared" si="0"/>
         <v>172.3.19.0</v>
       </c>
       <c r="E2" s="8">
-        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
       <c r="F2" s="8">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>19</v>
       </c>
       <c r="G2" s="8">
-        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H2" s="8" t="str">
-        <f t="shared" ref="H2:H34" ca="1" si="0">_xlfn.CONCAT("10.",E2,".",F2,".",G2)</f>
+        <f t="shared" ref="H2:H34" ca="1" si="5">_xlfn.CONCAT("10.",E2,".",F2,".",G2)</f>
         <v>10.3.19.1</v>
       </c>
       <c r="I2" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D2, " ", "255.255.255.0"," ", H2))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>ip route 172.3.19.0 255.255.255.0 10.3.19.1</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="13">
+      <c r="B3" s="11">
         <v>3</v>
       </c>
       <c r="C3" s="7">
-        <f t="shared" ref="C3:C21" si="1">C2-1</f>
+        <f t="shared" ref="C3:C21" si="6">C2-1</f>
         <v>18</v>
       </c>
       <c r="D3" s="8" t="str">
-        <f>_xlfn.CONCAT("172.",B3,".",C3,".0")</f>
+        <f t="shared" si="0"/>
         <v>172.3.18.0</v>
       </c>
       <c r="E3" s="8">
-        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
       <c r="F3" s="8">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>19</v>
       </c>
       <c r="G3" s="8">
-        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H3" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>10.3.19.1</v>
       </c>
       <c r="I3" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D3, " ", "255.255.255.0"," ", H3))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>ip route 172.3.18.0 255.255.255.0 10.3.19.1</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="13">
+      <c r="B4" s="11">
         <v>3</v>
       </c>
       <c r="C4" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>17</v>
       </c>
       <c r="D4" s="8" t="str">
-        <f>_xlfn.CONCAT("172.",B4,".",C4,".0")</f>
+        <f t="shared" si="0"/>
         <v>172.3.17.0</v>
       </c>
       <c r="E4" s="8">
-        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
       <c r="F4" s="8">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>19</v>
       </c>
       <c r="G4" s="8">
-        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H4" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>10.3.19.1</v>
       </c>
       <c r="I4" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D4, " ", "255.255.255.0"," ", H4))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>ip route 172.3.17.0 255.255.255.0 10.3.19.1</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="13">
+      <c r="B5" s="11">
         <v>3</v>
       </c>
       <c r="C5" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="D5" s="8" t="str">
-        <f>_xlfn.CONCAT("172.",B5,".",C5,".0")</f>
+        <f t="shared" si="0"/>
         <v>172.3.16.0</v>
       </c>
       <c r="E5" s="8">
-        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
       <c r="F5" s="8">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>19</v>
       </c>
       <c r="G5" s="8">
-        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H5" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>10.3.19.1</v>
       </c>
       <c r="I5" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D5, " ", "255.255.255.0"," ", H5))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>ip route 172.3.16.0 255.255.255.0 10.3.19.1</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="13">
+      <c r="B6" s="11">
         <v>3</v>
       </c>
       <c r="C6" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="D6" s="8" t="str">
-        <f>_xlfn.CONCAT("172.",B6,".",C6,".0")</f>
+        <f t="shared" si="0"/>
         <v>172.3.15.0</v>
       </c>
       <c r="E6" s="8">
-        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
       <c r="F6" s="8">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>19</v>
       </c>
       <c r="G6" s="8">
-        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H6" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>10.3.19.1</v>
       </c>
       <c r="I6" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D6, " ", "255.255.255.0"," ", H6))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>ip route 172.3.15.0 255.255.255.0 10.3.19.1</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="13">
+      <c r="B7" s="11">
         <v>3</v>
       </c>
       <c r="C7" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="D7" s="8" t="str">
-        <f>_xlfn.CONCAT("172.",B7,".",C7,".0")</f>
+        <f t="shared" si="0"/>
         <v>172.3.14.0</v>
       </c>
       <c r="E7" s="8">
-        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
       <c r="F7" s="8">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>19</v>
       </c>
       <c r="G7" s="8">
-        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H7" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>10.3.19.1</v>
       </c>
       <c r="I7" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D7, " ", "255.255.255.0"," ", H7))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>ip route 172.3.14.0 255.255.255.0 10.3.19.1</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B8" s="13">
+      <c r="B8" s="11">
         <v>3</v>
       </c>
       <c r="C8" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>13</v>
       </c>
       <c r="D8" s="8" t="str">
-        <f>_xlfn.CONCAT("172.",B8,".",C8,".0")</f>
+        <f t="shared" si="0"/>
         <v>172.3.13.0</v>
       </c>
       <c r="E8" s="8">
-        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
       <c r="F8" s="8">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>19</v>
       </c>
       <c r="G8" s="8">
-        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H8" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>10.3.19.1</v>
       </c>
       <c r="I8" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D8, " ", "255.255.255.0"," ", H8))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>ip route 172.3.13.0 255.255.255.0 10.3.19.1</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B9" s="13">
+      <c r="B9" s="11">
         <v>3</v>
       </c>
       <c r="C9" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="D9" s="8" t="str">
-        <f>_xlfn.CONCAT("172.",B9,".",C9,".0")</f>
+        <f t="shared" si="0"/>
         <v>172.3.12.0</v>
       </c>
       <c r="E9" s="8">
-        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
       <c r="F9" s="8">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>19</v>
       </c>
       <c r="G9" s="8">
-        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H9" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>10.3.19.1</v>
       </c>
       <c r="I9" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D9, " ", "255.255.255.0"," ", H9))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>ip route 172.3.12.0 255.255.255.0 10.3.19.1</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="13">
+      <c r="B10" s="11">
         <v>3</v>
       </c>
       <c r="C10" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="D10" s="8" t="str">
-        <f>_xlfn.CONCAT("172.",B10,".",C10,".0")</f>
+        <f t="shared" si="0"/>
         <v>172.3.11.0</v>
       </c>
       <c r="E10" s="8">
-        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
       <c r="F10" s="8">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>19</v>
       </c>
       <c r="G10" s="8">
-        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H10" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>10.3.19.1</v>
       </c>
       <c r="I10" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D10, " ", "255.255.255.0"," ", H10))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>ip route 172.3.11.0 255.255.255.0 10.3.19.1</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="13">
+      <c r="B11" s="11">
         <v>3</v>
       </c>
       <c r="C11" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="D11" s="8" t="str">
-        <f>_xlfn.CONCAT("172.",B11,".",C11,".0")</f>
+        <f t="shared" si="0"/>
         <v>172.3.10.0</v>
       </c>
       <c r="E11" s="8">
-        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
       <c r="F11" s="8">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>19</v>
       </c>
       <c r="G11" s="8">
-        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H11" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>10.3.19.1</v>
       </c>
       <c r="I11" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D11, " ", "255.255.255.0"," ", H11))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>ip route 172.3.10.0 255.255.255.0 10.3.19.1</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="13">
+      <c r="B12" s="11">
         <v>3</v>
       </c>
       <c r="C12" s="7">
@@ -11543,361 +12690,361 @@
         <v>9</v>
       </c>
       <c r="D12" s="8" t="str">
-        <f>_xlfn.CONCAT("172.",B12,".",C12,".0")</f>
+        <f t="shared" si="0"/>
         <v>172.3.9.0</v>
       </c>
       <c r="E12" s="8">
-        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
       <c r="F12" s="8">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>19</v>
       </c>
       <c r="G12" s="8">
-        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H12" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>10.3.19.1</v>
       </c>
       <c r="I12" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D12, " ", "255.255.255.0"," ", H12))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>ip route 172.3.9.0 255.255.255.0 10.3.19.1</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B13" s="13">
+      <c r="B13" s="11">
         <v>3</v>
       </c>
       <c r="C13" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="D13" s="8" t="str">
-        <f>_xlfn.CONCAT("172.",B13,".",C13,".0")</f>
+        <f t="shared" si="0"/>
         <v>172.3.8.0</v>
       </c>
       <c r="E13" s="8">
-        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
       <c r="F13" s="8">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>19</v>
       </c>
       <c r="G13" s="8">
-        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H13" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>10.3.19.1</v>
       </c>
       <c r="I13" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D13, " ", "255.255.255.0"," ", H13))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>ip route 172.3.8.0 255.255.255.0 10.3.19.1</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="13">
+      <c r="B14" s="11">
         <v>3</v>
       </c>
       <c r="C14" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="D14" s="8" t="str">
-        <f>_xlfn.CONCAT("172.",B14,".",C14,".0")</f>
+        <f t="shared" si="0"/>
         <v>172.3.7.0</v>
       </c>
       <c r="E14" s="8">
-        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
       <c r="F14" s="8">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>19</v>
       </c>
       <c r="G14" s="8">
-        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H14" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>10.3.19.1</v>
       </c>
       <c r="I14" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D14, " ", "255.255.255.0"," ", H14))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>ip route 172.3.7.0 255.255.255.0 10.3.19.1</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B15" s="13">
+      <c r="B15" s="11">
         <v>3</v>
       </c>
       <c r="C15" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="D15" s="8" t="str">
-        <f>_xlfn.CONCAT("172.",B15,".",C15,".0")</f>
+        <f t="shared" si="0"/>
         <v>172.3.6.0</v>
       </c>
       <c r="E15" s="8">
-        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
       <c r="F15" s="8">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>19</v>
       </c>
       <c r="G15" s="8">
-        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H15" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>10.3.19.1</v>
       </c>
       <c r="I15" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D15, " ", "255.255.255.0"," ", H15))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>ip route 172.3.6.0 255.255.255.0 10.3.19.1</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B16" s="13">
+      <c r="B16" s="11">
         <v>3</v>
       </c>
       <c r="C16" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="D16" s="8" t="str">
-        <f>_xlfn.CONCAT("172.",B16,".",C16,".0")</f>
+        <f t="shared" si="0"/>
         <v>172.3.5.0</v>
       </c>
       <c r="E16" s="8">
-        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
       <c r="F16" s="8">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>19</v>
       </c>
       <c r="G16" s="8">
-        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H16" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>10.3.19.1</v>
       </c>
       <c r="I16" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D16, " ", "255.255.255.0"," ", H16))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>ip route 172.3.5.0 255.255.255.0 10.3.19.1</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B17" s="13">
+      <c r="B17" s="11">
         <v>3</v>
       </c>
       <c r="C17" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="D17" s="8" t="str">
-        <f>_xlfn.CONCAT("172.",B17,".",C17,".0")</f>
+        <f t="shared" si="0"/>
         <v>172.3.4.0</v>
       </c>
       <c r="E17" s="8">
-        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
       <c r="F17" s="8">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>19</v>
       </c>
       <c r="G17" s="8">
-        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H17" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>10.3.19.1</v>
       </c>
       <c r="I17" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D17, " ", "255.255.255.0"," ", H17))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>ip route 172.3.4.0 255.255.255.0 10.3.19.1</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B18" s="13">
+      <c r="B18" s="11">
         <v>3</v>
       </c>
       <c r="C18" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="D18" s="8" t="str">
-        <f>_xlfn.CONCAT("172.",B18,".",C18,".0")</f>
+        <f t="shared" si="0"/>
         <v>172.3.3.0</v>
       </c>
       <c r="E18" s="8">
-        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
       <c r="F18" s="8">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>19</v>
       </c>
       <c r="G18" s="8">
-        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H18" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>10.3.19.1</v>
       </c>
       <c r="I18" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D18, " ", "255.255.255.0"," ", H18))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>ip route 172.3.3.0 255.255.255.0 10.3.19.1</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B19" s="13">
+      <c r="B19" s="11">
         <v>3</v>
       </c>
       <c r="C19" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="D19" s="8" t="str">
-        <f>_xlfn.CONCAT("172.",B19,".",C19,".0")</f>
+        <f t="shared" si="0"/>
         <v>172.3.2.0</v>
       </c>
       <c r="E19" s="8">
-        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
       <c r="F19" s="8">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>19</v>
       </c>
       <c r="G19" s="8">
-        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H19" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>10.3.19.1</v>
       </c>
       <c r="I19" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D19, " ", "255.255.255.0"," ", H19))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>ip route 172.3.2.0 255.255.255.0 10.3.19.1</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B20" s="13">
+      <c r="B20" s="11">
         <v>3</v>
       </c>
       <c r="C20" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="D20" s="8" t="str">
-        <f>_xlfn.CONCAT("172.",B20,".",C20,".0")</f>
+        <f t="shared" si="0"/>
         <v>172.3.1.0</v>
       </c>
       <c r="E20" s="8">
-        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
       <c r="F20" s="8">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>19</v>
       </c>
       <c r="G20" s="8">
-        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H20" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>10.3.19.1</v>
       </c>
       <c r="I20" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D20, " ", "255.255.255.0"," ", H20))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>ip route 172.3.1.0 255.255.255.0 10.3.19.1</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B21" s="13">
+      <c r="B21" s="11">
         <v>3</v>
       </c>
       <c r="C21" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D21" s="8" t="str">
-        <f>_xlfn.CONCAT("172.",B21,".",C21,".0")</f>
+        <f t="shared" si="0"/>
         <v>172.3.0.0</v>
       </c>
       <c r="E21" s="8">
-        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
       <c r="F21" s="8">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>19</v>
       </c>
       <c r="G21" s="8">
-        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H21" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>10.3.19.1</v>
       </c>
       <c r="I21" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D21, " ", "255.255.255.0"," ", H21))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>ip route 172.3.0.0 255.255.255.0 10.3.19.1</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B22" s="11">
+      <c r="B22" s="9">
         <v>1</v>
       </c>
       <c r="C22" s="7">
         <v>5</v>
       </c>
       <c r="D22" s="8" t="str">
-        <f>_xlfn.CONCAT("172.",B22,".",C22,".0")</f>
+        <f t="shared" si="0"/>
         <v>172.1.5.0</v>
       </c>
       <c r="E22" s="8">
-        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
       <c r="F22" s="8">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>19</v>
       </c>
       <c r="G22" s="8">
-        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H22" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>10.3.19.1</v>
       </c>
       <c r="I22" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D22, " ", "255.255.255.0"," ", H22))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>ip route 172.1.5.0 255.255.255.0 10.3.19.1</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B23" s="11">
+      <c r="B23" s="9">
         <v>1</v>
       </c>
       <c r="C23" s="7">
@@ -11905,196 +13052,196 @@
         <v>4</v>
       </c>
       <c r="D23" s="8" t="str">
-        <f t="shared" ref="D23:D34" si="2">_xlfn.CONCAT("172.",B23,".",C23,".0")</f>
+        <f t="shared" ref="D23:D34" si="7">_xlfn.CONCAT("172.",B23,".",C23,".0")</f>
         <v>172.1.4.0</v>
       </c>
       <c r="E23" s="8">
-        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
       <c r="F23" s="8">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>19</v>
       </c>
       <c r="G23" s="8">
-        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H23" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>10.3.19.1</v>
       </c>
       <c r="I23" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D23, " ", "255.255.255.0"," ", H23))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>ip route 172.1.4.0 255.255.255.0 10.3.19.1</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B24" s="11">
+      <c r="B24" s="9">
         <v>1</v>
       </c>
       <c r="C24" s="7">
-        <f t="shared" ref="C24:C27" si="3">C23-1</f>
+        <f t="shared" ref="C24:C27" si="8">C23-1</f>
         <v>3</v>
       </c>
       <c r="D24" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>172.1.3.0</v>
       </c>
       <c r="E24" s="8">
-        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
       <c r="F24" s="8">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>19</v>
       </c>
       <c r="G24" s="8">
-        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H24" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>10.3.19.1</v>
       </c>
       <c r="I24" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D24, " ", "255.255.255.0"," ", H24))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>ip route 172.1.3.0 255.255.255.0 10.3.19.1</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B25" s="11">
+      <c r="B25" s="9">
         <v>1</v>
       </c>
       <c r="C25" s="7">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="D25" s="8" t="str">
+        <f t="shared" si="7"/>
+        <v>172.1.2.0</v>
+      </c>
+      <c r="E25" s="8">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F25" s="8">
+        <f t="shared" ca="1" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="G25" s="8">
         <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D25" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>172.1.2.0</v>
-      </c>
-      <c r="E25" s="8">
-        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
-        <v>3</v>
-      </c>
-      <c r="F25" s="8">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H25" s="8" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>10.3.19.1</v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>ip route 172.1.2.0 255.255.255.0 10.3.19.1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B26" s="9">
+        <v>1</v>
+      </c>
+      <c r="C26" s="7">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="D26" s="8" t="str">
+        <f t="shared" si="7"/>
+        <v>172.1.1.0</v>
+      </c>
+      <c r="E26" s="8">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F26" s="8">
+        <f t="shared" ca="1" si="2"/>
         <v>19</v>
       </c>
-      <c r="G25" s="8">
-        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
-        <v>1</v>
-      </c>
-      <c r="H25" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+      <c r="G26" s="8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="H26" s="8" t="str">
+        <f t="shared" ca="1" si="5"/>
         <v>10.3.19.1</v>
       </c>
-      <c r="I25" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D25, " ", "255.255.255.0"," ", H25))</f>
-        <v>ip route 172.1.2.0 255.255.255.0 10.3.19.1</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B26" s="11">
-        <v>1</v>
-      </c>
-      <c r="C26" s="7">
+      <c r="I26" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>ip route 172.1.1.0 255.255.255.0 10.3.19.1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B27" s="9">
+        <v>1</v>
+      </c>
+      <c r="C27" s="7">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="D27" s="8" t="str">
+        <f t="shared" si="7"/>
+        <v>172.1.0.0</v>
+      </c>
+      <c r="E27" s="8">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F27" s="8">
+        <f t="shared" ca="1" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="G27" s="8">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="D26" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>172.1.1.0</v>
-      </c>
-      <c r="E26" s="8">
-        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
-        <v>3</v>
-      </c>
-      <c r="F26" s="8">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
-        <v>19</v>
-      </c>
-      <c r="G26" s="8">
-        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
-        <v>1</v>
-      </c>
-      <c r="H26" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+      <c r="H27" s="8" t="str">
+        <f t="shared" ca="1" si="5"/>
         <v>10.3.19.1</v>
       </c>
-      <c r="I26" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D26, " ", "255.255.255.0"," ", H26))</f>
-        <v>ip route 172.1.1.0 255.255.255.0 10.3.19.1</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B27" s="11">
-        <v>1</v>
-      </c>
-      <c r="C27" s="7">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D27" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>172.1.0.0</v>
-      </c>
-      <c r="E27" s="8">
-        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
-        <v>3</v>
-      </c>
-      <c r="F27" s="8">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
-        <v>19</v>
-      </c>
-      <c r="G27" s="8">
-        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
-        <v>1</v>
-      </c>
-      <c r="H27" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>10.3.19.1</v>
-      </c>
       <c r="I27" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D27, " ", "255.255.255.0"," ", H27))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>ip route 172.1.0.0 255.255.255.0 10.3.19.1</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B28" s="12">
+      <c r="B28" s="10">
         <v>2</v>
       </c>
       <c r="C28" s="7">
         <v>6</v>
       </c>
       <c r="D28" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>172.2.6.0</v>
       </c>
       <c r="E28" s="8">
-        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
       <c r="F28" s="8">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>19</v>
       </c>
       <c r="G28" s="8">
-        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H28" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>10.3.19.1</v>
       </c>
       <c r="I28" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D28, " ", "255.255.255.0"," ", H28))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>ip route 172.2.6.0 255.255.255.0 10.3.19.1</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B29" s="12">
+      <c r="B29" s="10">
         <v>2</v>
       </c>
       <c r="C29" s="7">
@@ -12102,192 +13249,192 @@
         <v>5</v>
       </c>
       <c r="D29" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>172.2.5.0</v>
       </c>
       <c r="E29" s="8">
-        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
       <c r="F29" s="8">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>19</v>
       </c>
       <c r="G29" s="8">
-        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H29" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>10.3.19.1</v>
       </c>
       <c r="I29" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D29, " ", "255.255.255.0"," ", H29))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>ip route 172.2.5.0 255.255.255.0 10.3.19.1</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B30" s="12">
+      <c r="B30" s="10">
         <v>2</v>
       </c>
       <c r="C30" s="7">
-        <f t="shared" ref="C30:C34" si="4">C29-1</f>
+        <f t="shared" ref="C30:C34" si="9">C29-1</f>
         <v>4</v>
       </c>
       <c r="D30" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>172.2.4.0</v>
       </c>
       <c r="E30" s="8">
-        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
       <c r="F30" s="8">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>19</v>
       </c>
       <c r="G30" s="8">
-        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H30" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>10.3.19.1</v>
       </c>
       <c r="I30" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D30, " ", "255.255.255.0"," ", H30))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>ip route 172.2.4.0 255.255.255.0 10.3.19.1</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B31" s="12">
+      <c r="B31" s="10">
         <v>2</v>
       </c>
       <c r="C31" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="D31" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>172.2.3.0</v>
       </c>
       <c r="E31" s="8">
-        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
       <c r="F31" s="8">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>19</v>
       </c>
       <c r="G31" s="8">
-        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H31" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>10.3.19.1</v>
       </c>
       <c r="I31" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D31, " ", "255.255.255.0"," ", H31))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>ip route 172.2.3.0 255.255.255.0 10.3.19.1</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B32" s="12">
+      <c r="B32" s="10">
         <v>2</v>
       </c>
       <c r="C32" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="D32" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>172.2.2.0</v>
       </c>
       <c r="E32" s="8">
-        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
       <c r="F32" s="8">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>19</v>
       </c>
       <c r="G32" s="8">
-        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H32" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>10.3.19.1</v>
       </c>
       <c r="I32" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D32, " ", "255.255.255.0"," ", H32))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>ip route 172.2.2.0 255.255.255.0 10.3.19.1</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B33" s="12">
+      <c r="B33" s="10">
         <v>2</v>
       </c>
       <c r="C33" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="D33" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>172.2.1.0</v>
       </c>
       <c r="E33" s="8">
-        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
       <c r="F33" s="8">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>19</v>
       </c>
       <c r="G33" s="8">
-        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H33" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>10.3.19.1</v>
       </c>
       <c r="I33" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D33, " ", "255.255.255.0"," ", H33))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>ip route 172.2.1.0 255.255.255.0 10.3.19.1</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B34" s="12">
+      <c r="B34" s="10">
         <v>2</v>
       </c>
       <c r="C34" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="D34" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>172.2.0.0</v>
       </c>
       <c r="E34" s="8">
-        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
       <c r="F34" s="8">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>19</v>
       </c>
       <c r="G34" s="8">
-        <f>IF(MATCH("*",$A$1:$A$34) &gt; ROW(), 2, 1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H34" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>10.3.19.1</v>
       </c>
       <c r="I34" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ip route", " ", D34, " ", "255.255.255.0"," ", H34))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>ip route 172.2.0.0 255.255.255.0 10.3.19.1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se termina enrutamiento static ipv6
</commit_message>
<xml_diff>
--- a/taller-2/Taller#2.xlsx
+++ b/taller-2/Taller#2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan\Documents\GitHub\Interconexion\taller-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB9156F-3B81-4A8C-9A80-9F1F04256FE4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA24CFB-4126-4541-8BA1-F57408CE2659}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ipv4" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Enrutamiento4E3" sheetId="4" r:id="rId5"/>
     <sheet name="Enrutamiento6E1" sheetId="6" r:id="rId6"/>
     <sheet name="Enrutamiento6E3" sheetId="7" r:id="rId7"/>
+    <sheet name="Enrutamiento6E2" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="40">
   <si>
     <t>#</t>
   </si>
@@ -151,6 +152,12 @@
   </si>
   <si>
     <t>ipv6 unicast-routing</t>
+  </si>
+  <si>
+    <t>2001:F1:1::1</t>
+  </si>
+  <si>
+    <t>2001:F2:1::2</t>
   </si>
 </sst>
 </file>
@@ -13501,7 +13508,7 @@
         <v>2001:A5:1::1</v>
       </c>
       <c r="I1" t="str">
-        <f>IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ipv6 route", " ", D1, "/112"," ", H1))</f>
+        <f t="shared" ref="I1:I34" si="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ipv6 route", " ", D1, "/112"," ", H1))</f>
         <v>#</v>
       </c>
     </row>
@@ -13514,7 +13521,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="8" t="str">
-        <f t="shared" ref="D2:D34" si="1">_xlfn.CONCAT("2001:",B2,":",C2,"::")</f>
+        <f t="shared" ref="D2:D34" si="2">_xlfn.CONCAT("2001:",B2,":",C2,"::")</f>
         <v>2001:1:5::</v>
       </c>
       <c r="E2" s="8">
@@ -13522,19 +13529,19 @@
         <v>1</v>
       </c>
       <c r="F2" s="8" t="str">
-        <f t="shared" ref="F2:F34" ca="1" si="2">_xlfn.CONCAT(_xlfn.SWITCH(E2,1,"A",2,"B",3,"C"), IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1))</f>
+        <f t="shared" ref="F2:F34" ca="1" si="3">_xlfn.CONCAT(_xlfn.SWITCH(E2,1,"A",2,"B",3,"C"), IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1))</f>
         <v>A5</v>
       </c>
       <c r="G2" s="8">
-        <f t="shared" ref="G2:G34" si="3">IF(MATCH("*",$A$1:$A$34) &lt; ROW(), 2, 1)</f>
+        <f t="shared" ref="G2:G34" si="4">IF(MATCH("*",$A$1:$A$34) &lt; ROW(), 2, 1)</f>
         <v>2</v>
       </c>
       <c r="H2" s="8" t="str">
-        <f t="shared" ref="H2:H34" ca="1" si="4">_xlfn.CONCAT("2001:",F2,":1::",G2)</f>
+        <f t="shared" ref="H2:H34" ca="1" si="5">_xlfn.CONCAT("2001:",F2,":1::",G2)</f>
         <v>2001:A5:1::2</v>
       </c>
       <c r="I2" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ipv6 route", " ", D2, "/112"," ", H2))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>ipv6 route 2001:1:5::/112 2001:A5:1::2</v>
       </c>
     </row>
@@ -13543,11 +13550,11 @@
         <v>1</v>
       </c>
       <c r="C3" s="7">
-        <f t="shared" ref="C3:C6" si="5">C2-1</f>
+        <f t="shared" ref="C3:C6" si="6">C2-1</f>
         <v>4</v>
       </c>
       <c r="D3" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2001:1:4::</v>
       </c>
       <c r="E3" s="8">
@@ -13555,19 +13562,19 @@
         <v>1</v>
       </c>
       <c r="F3" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>A5</v>
       </c>
       <c r="G3" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="H3" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2001:A5:1::2</v>
       </c>
       <c r="I3" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ipv6 route", " ", D3, "/112"," ", H3))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>ipv6 route 2001:1:4::/112 2001:A5:1::2</v>
       </c>
     </row>
@@ -13576,11 +13583,11 @@
         <v>1</v>
       </c>
       <c r="C4" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="D4" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2001:1:3::</v>
       </c>
       <c r="E4" s="8">
@@ -13588,19 +13595,19 @@
         <v>1</v>
       </c>
       <c r="F4" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>A5</v>
       </c>
       <c r="G4" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="H4" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2001:A5:1::2</v>
       </c>
       <c r="I4" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ipv6 route", " ", D4, "/112"," ", H4))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>ipv6 route 2001:1:3::/112 2001:A5:1::2</v>
       </c>
     </row>
@@ -13609,11 +13616,11 @@
         <v>1</v>
       </c>
       <c r="C5" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="D5" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2001:1:2::</v>
       </c>
       <c r="E5" s="8">
@@ -13621,19 +13628,19 @@
         <v>1</v>
       </c>
       <c r="F5" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>A5</v>
       </c>
       <c r="G5" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="H5" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2001:A5:1::2</v>
       </c>
       <c r="I5" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ipv6 route", " ", D5, "/112"," ", H5))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>ipv6 route 2001:1:2::/112 2001:A5:1::2</v>
       </c>
     </row>
@@ -13642,11 +13649,11 @@
         <v>1</v>
       </c>
       <c r="C6" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="D6" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2001:1:1::</v>
       </c>
       <c r="E6" s="8">
@@ -13654,19 +13661,19 @@
         <v>1</v>
       </c>
       <c r="F6" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>A5</v>
       </c>
       <c r="G6" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="H6" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2001:A5:1::2</v>
       </c>
       <c r="I6" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ipv6 route", " ", D6, "/112"," ", H6))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>ipv6 route 2001:1:1::/112 2001:A5:1::2</v>
       </c>
     </row>
@@ -13678,7 +13685,7 @@
         <v>7</v>
       </c>
       <c r="D7" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2001:2:7::</v>
       </c>
       <c r="E7" s="8">
@@ -13686,19 +13693,19 @@
         <v>1</v>
       </c>
       <c r="F7" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>A5</v>
       </c>
       <c r="G7" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="H7" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2001:A5:1::2</v>
       </c>
       <c r="I7" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ipv6 route", " ", D7, "/112"," ", H7))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>ipv6 route 2001:2:7::/112 2001:A5:1::2</v>
       </c>
     </row>
@@ -13707,11 +13714,11 @@
         <v>2</v>
       </c>
       <c r="C8" s="7">
-        <f t="shared" ref="C8:C13" si="6">C7-1</f>
+        <f t="shared" ref="C8:C13" si="7">C7-1</f>
         <v>6</v>
       </c>
       <c r="D8" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2001:2:6::</v>
       </c>
       <c r="E8" s="8">
@@ -13719,19 +13726,19 @@
         <v>1</v>
       </c>
       <c r="F8" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>A5</v>
       </c>
       <c r="G8" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="H8" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2001:A5:1::2</v>
       </c>
       <c r="I8" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ipv6 route", " ", D8, "/112"," ", H8))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>ipv6 route 2001:2:6::/112 2001:A5:1::2</v>
       </c>
     </row>
@@ -13740,11 +13747,11 @@
         <v>2</v>
       </c>
       <c r="C9" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="D9" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2001:2:5::</v>
       </c>
       <c r="E9" s="8">
@@ -13752,19 +13759,19 @@
         <v>1</v>
       </c>
       <c r="F9" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>A5</v>
       </c>
       <c r="G9" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="H9" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2001:A5:1::2</v>
       </c>
       <c r="I9" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ipv6 route", " ", D9, "/112"," ", H9))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>ipv6 route 2001:2:5::/112 2001:A5:1::2</v>
       </c>
     </row>
@@ -13773,11 +13780,11 @@
         <v>2</v>
       </c>
       <c r="C10" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D10" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2001:2:4::</v>
       </c>
       <c r="E10" s="8">
@@ -13785,19 +13792,19 @@
         <v>1</v>
       </c>
       <c r="F10" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>A5</v>
       </c>
       <c r="G10" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="H10" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2001:A5:1::2</v>
       </c>
       <c r="I10" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ipv6 route", " ", D10, "/112"," ", H10))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>ipv6 route 2001:2:4::/112 2001:A5:1::2</v>
       </c>
     </row>
@@ -13806,11 +13813,11 @@
         <v>2</v>
       </c>
       <c r="C11" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="D11" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2001:2:3::</v>
       </c>
       <c r="E11" s="8">
@@ -13818,19 +13825,19 @@
         <v>1</v>
       </c>
       <c r="F11" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>A5</v>
       </c>
       <c r="G11" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="H11" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2001:A5:1::2</v>
       </c>
       <c r="I11" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ipv6 route", " ", D11, "/112"," ", H11))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>ipv6 route 2001:2:3::/112 2001:A5:1::2</v>
       </c>
     </row>
@@ -13839,11 +13846,11 @@
         <v>2</v>
       </c>
       <c r="C12" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="D12" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2001:2:2::</v>
       </c>
       <c r="E12" s="8">
@@ -13851,19 +13858,19 @@
         <v>1</v>
       </c>
       <c r="F12" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>A5</v>
       </c>
       <c r="G12" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="H12" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2001:A5:1::2</v>
       </c>
       <c r="I12" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ipv6 route", " ", D12, "/112"," ", H12))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>ipv6 route 2001:2:2::/112 2001:A5:1::2</v>
       </c>
     </row>
@@ -13872,11 +13879,11 @@
         <v>2</v>
       </c>
       <c r="C13" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="D13" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2001:2:1::</v>
       </c>
       <c r="E13" s="8">
@@ -13884,19 +13891,19 @@
         <v>1</v>
       </c>
       <c r="F13" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>A5</v>
       </c>
       <c r="G13" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="H13" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2001:A5:1::2</v>
       </c>
       <c r="I13" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ipv6 route", " ", D13, "/112"," ", H13))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>ipv6 route 2001:2:1::/112 2001:A5:1::2</v>
       </c>
     </row>
@@ -13908,7 +13915,7 @@
         <v>21</v>
       </c>
       <c r="D14" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2001:3:21::</v>
       </c>
       <c r="E14" s="8">
@@ -13916,19 +13923,19 @@
         <v>1</v>
       </c>
       <c r="F14" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>A5</v>
       </c>
       <c r="G14" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="H14" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2001:A5:1::2</v>
       </c>
       <c r="I14" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ipv6 route", " ", D14, "/112"," ", H14))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>ipv6 route 2001:3:21::/112 2001:A5:1::2</v>
       </c>
     </row>
@@ -13941,7 +13948,7 @@
         <v>20</v>
       </c>
       <c r="D15" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2001:3:20::</v>
       </c>
       <c r="E15" s="8">
@@ -13949,19 +13956,19 @@
         <v>1</v>
       </c>
       <c r="F15" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>A5</v>
       </c>
       <c r="G15" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="H15" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2001:A5:1::2</v>
       </c>
       <c r="I15" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ipv6 route", " ", D15, "/112"," ", H15))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>ipv6 route 2001:3:20::/112 2001:A5:1::2</v>
       </c>
     </row>
@@ -13970,11 +13977,11 @@
         <v>3</v>
       </c>
       <c r="C16" s="7">
-        <f t="shared" ref="C16:C34" si="7">C15-1</f>
+        <f t="shared" ref="C16:C34" si="8">C15-1</f>
         <v>19</v>
       </c>
       <c r="D16" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2001:3:19::</v>
       </c>
       <c r="E16" s="8">
@@ -13982,19 +13989,19 @@
         <v>1</v>
       </c>
       <c r="F16" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>A5</v>
       </c>
       <c r="G16" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="H16" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2001:A5:1::2</v>
       </c>
       <c r="I16" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ipv6 route", " ", D16, "/112"," ", H16))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>ipv6 route 2001:3:19::/112 2001:A5:1::2</v>
       </c>
     </row>
@@ -14003,11 +14010,11 @@
         <v>3</v>
       </c>
       <c r="C17" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="D17" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2001:3:18::</v>
       </c>
       <c r="E17" s="8">
@@ -14015,19 +14022,19 @@
         <v>1</v>
       </c>
       <c r="F17" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>A5</v>
       </c>
       <c r="G17" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="H17" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2001:A5:1::2</v>
       </c>
       <c r="I17" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ipv6 route", " ", D17, "/112"," ", H17))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>ipv6 route 2001:3:18::/112 2001:A5:1::2</v>
       </c>
     </row>
@@ -14036,11 +14043,11 @@
         <v>3</v>
       </c>
       <c r="C18" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>17</v>
       </c>
       <c r="D18" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2001:3:17::</v>
       </c>
       <c r="E18" s="8">
@@ -14048,19 +14055,19 @@
         <v>1</v>
       </c>
       <c r="F18" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>A5</v>
       </c>
       <c r="G18" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="H18" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2001:A5:1::2</v>
       </c>
       <c r="I18" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ipv6 route", " ", D18, "/112"," ", H18))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>ipv6 route 2001:3:17::/112 2001:A5:1::2</v>
       </c>
     </row>
@@ -14069,11 +14076,11 @@
         <v>3</v>
       </c>
       <c r="C19" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>16</v>
       </c>
       <c r="D19" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2001:3:16::</v>
       </c>
       <c r="E19" s="8">
@@ -14081,19 +14088,19 @@
         <v>1</v>
       </c>
       <c r="F19" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>A5</v>
       </c>
       <c r="G19" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="H19" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2001:A5:1::2</v>
       </c>
       <c r="I19" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ipv6 route", " ", D19, "/112"," ", H19))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>ipv6 route 2001:3:16::/112 2001:A5:1::2</v>
       </c>
     </row>
@@ -14102,11 +14109,11 @@
         <v>3</v>
       </c>
       <c r="C20" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="D20" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2001:3:15::</v>
       </c>
       <c r="E20" s="8">
@@ -14114,19 +14121,19 @@
         <v>1</v>
       </c>
       <c r="F20" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>A5</v>
       </c>
       <c r="G20" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="H20" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2001:A5:1::2</v>
       </c>
       <c r="I20" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ipv6 route", " ", D20, "/112"," ", H20))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>ipv6 route 2001:3:15::/112 2001:A5:1::2</v>
       </c>
     </row>
@@ -14135,11 +14142,11 @@
         <v>3</v>
       </c>
       <c r="C21" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>14</v>
       </c>
       <c r="D21" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2001:3:14::</v>
       </c>
       <c r="E21" s="8">
@@ -14147,19 +14154,19 @@
         <v>1</v>
       </c>
       <c r="F21" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>A5</v>
       </c>
       <c r="G21" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="H21" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2001:A5:1::2</v>
       </c>
       <c r="I21" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ipv6 route", " ", D21, "/112"," ", H21))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>ipv6 route 2001:3:14::/112 2001:A5:1::2</v>
       </c>
     </row>
@@ -14168,11 +14175,11 @@
         <v>3</v>
       </c>
       <c r="C22" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>13</v>
       </c>
       <c r="D22" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2001:3:13::</v>
       </c>
       <c r="E22" s="8">
@@ -14180,19 +14187,19 @@
         <v>1</v>
       </c>
       <c r="F22" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>A5</v>
       </c>
       <c r="G22" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="H22" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2001:A5:1::2</v>
       </c>
       <c r="I22" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ipv6 route", " ", D22, "/112"," ", H22))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>ipv6 route 2001:3:13::/112 2001:A5:1::2</v>
       </c>
     </row>
@@ -14201,11 +14208,11 @@
         <v>3</v>
       </c>
       <c r="C23" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
       <c r="D23" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2001:3:12::</v>
       </c>
       <c r="E23" s="8">
@@ -14213,19 +14220,19 @@
         <v>1</v>
       </c>
       <c r="F23" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>A5</v>
       </c>
       <c r="G23" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="H23" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2001:A5:1::2</v>
       </c>
       <c r="I23" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ipv6 route", " ", D23, "/112"," ", H23))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>ipv6 route 2001:3:12::/112 2001:A5:1::2</v>
       </c>
     </row>
@@ -14234,11 +14241,11 @@
         <v>3</v>
       </c>
       <c r="C24" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
       <c r="D24" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2001:3:11::</v>
       </c>
       <c r="E24" s="8">
@@ -14246,19 +14253,19 @@
         <v>1</v>
       </c>
       <c r="F24" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>A5</v>
       </c>
       <c r="G24" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="H24" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2001:A5:1::2</v>
       </c>
       <c r="I24" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ipv6 route", " ", D24, "/112"," ", H24))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>ipv6 route 2001:3:11::/112 2001:A5:1::2</v>
       </c>
     </row>
@@ -14271,7 +14278,7 @@
         <v>10</v>
       </c>
       <c r="D25" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2001:3:10::</v>
       </c>
       <c r="E25" s="8">
@@ -14279,19 +14286,19 @@
         <v>1</v>
       </c>
       <c r="F25" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>A5</v>
       </c>
       <c r="G25" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="H25" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2001:A5:1::2</v>
       </c>
       <c r="I25" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ipv6 route", " ", D25, "/112"," ", H25))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>ipv6 route 2001:3:10::/112 2001:A5:1::2</v>
       </c>
     </row>
@@ -14300,11 +14307,11 @@
         <v>3</v>
       </c>
       <c r="C26" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="D26" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2001:3:9::</v>
       </c>
       <c r="E26" s="8">
@@ -14312,19 +14319,19 @@
         <v>1</v>
       </c>
       <c r="F26" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>A5</v>
       </c>
       <c r="G26" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="H26" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2001:A5:1::2</v>
       </c>
       <c r="I26" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ipv6 route", " ", D26, "/112"," ", H26))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>ipv6 route 2001:3:9::/112 2001:A5:1::2</v>
       </c>
     </row>
@@ -14333,11 +14340,11 @@
         <v>3</v>
       </c>
       <c r="C27" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="D27" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2001:3:8::</v>
       </c>
       <c r="E27" s="8">
@@ -14345,19 +14352,19 @@
         <v>1</v>
       </c>
       <c r="F27" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>A5</v>
       </c>
       <c r="G27" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="H27" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2001:A5:1::2</v>
       </c>
       <c r="I27" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ipv6 route", " ", D27, "/112"," ", H27))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>ipv6 route 2001:3:8::/112 2001:A5:1::2</v>
       </c>
     </row>
@@ -14366,11 +14373,11 @@
         <v>3</v>
       </c>
       <c r="C28" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="D28" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2001:3:7::</v>
       </c>
       <c r="E28" s="8">
@@ -14378,19 +14385,19 @@
         <v>1</v>
       </c>
       <c r="F28" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>A5</v>
       </c>
       <c r="G28" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="H28" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2001:A5:1::2</v>
       </c>
       <c r="I28" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ipv6 route", " ", D28, "/112"," ", H28))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>ipv6 route 2001:3:7::/112 2001:A5:1::2</v>
       </c>
     </row>
@@ -14399,11 +14406,11 @@
         <v>3</v>
       </c>
       <c r="C29" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="D29" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2001:3:6::</v>
       </c>
       <c r="E29" s="8">
@@ -14411,19 +14418,19 @@
         <v>1</v>
       </c>
       <c r="F29" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>A5</v>
       </c>
       <c r="G29" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="H29" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2001:A5:1::2</v>
       </c>
       <c r="I29" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ipv6 route", " ", D29, "/112"," ", H29))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>ipv6 route 2001:3:6::/112 2001:A5:1::2</v>
       </c>
     </row>
@@ -14432,11 +14439,11 @@
         <v>3</v>
       </c>
       <c r="C30" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="D30" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2001:3:5::</v>
       </c>
       <c r="E30" s="8">
@@ -14444,19 +14451,19 @@
         <v>1</v>
       </c>
       <c r="F30" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>A5</v>
       </c>
       <c r="G30" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="H30" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2001:A5:1::2</v>
       </c>
       <c r="I30" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ipv6 route", " ", D30, "/112"," ", H30))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>ipv6 route 2001:3:5::/112 2001:A5:1::2</v>
       </c>
     </row>
@@ -14465,11 +14472,11 @@
         <v>3</v>
       </c>
       <c r="C31" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="D31" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2001:3:4::</v>
       </c>
       <c r="E31" s="8">
@@ -14477,19 +14484,19 @@
         <v>1</v>
       </c>
       <c r="F31" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>A5</v>
       </c>
       <c r="G31" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="H31" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2001:A5:1::2</v>
       </c>
       <c r="I31" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ipv6 route", " ", D31, "/112"," ", H31))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>ipv6 route 2001:3:4::/112 2001:A5:1::2</v>
       </c>
     </row>
@@ -14498,11 +14505,11 @@
         <v>3</v>
       </c>
       <c r="C32" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="D32" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2001:3:3::</v>
       </c>
       <c r="E32" s="8">
@@ -14510,19 +14517,19 @@
         <v>1</v>
       </c>
       <c r="F32" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>A5</v>
       </c>
       <c r="G32" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="H32" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2001:A5:1::2</v>
       </c>
       <c r="I32" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ipv6 route", " ", D32, "/112"," ", H32))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>ipv6 route 2001:3:3::/112 2001:A5:1::2</v>
       </c>
     </row>
@@ -14531,11 +14538,11 @@
         <v>3</v>
       </c>
       <c r="C33" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="D33" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2001:3:2::</v>
       </c>
       <c r="E33" s="8">
@@ -14543,19 +14550,19 @@
         <v>1</v>
       </c>
       <c r="F33" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>A5</v>
       </c>
       <c r="G33" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="H33" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2001:A5:1::2</v>
       </c>
       <c r="I33" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ipv6 route", " ", D33, "/112"," ", H33))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>ipv6 route 2001:3:2::/112 2001:A5:1::2</v>
       </c>
     </row>
@@ -14564,11 +14571,11 @@
         <v>3</v>
       </c>
       <c r="C34" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="D34" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2001:3:1::</v>
       </c>
       <c r="E34" s="8">
@@ -14576,19 +14583,19 @@
         <v>1</v>
       </c>
       <c r="F34" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>A5</v>
       </c>
       <c r="G34" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="H34" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2001:A5:1::2</v>
       </c>
       <c r="I34" t="str">
-        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ipv6 route", " ", D34, "/112"," ", H34))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>ipv6 route 2001:3:1::/112 2001:A5:1::2</v>
       </c>
     </row>
@@ -14606,7 +14613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E87B96A-0425-47B5-BF94-4BABDB53A147}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -15753,4 +15760,1148 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E11DFEC-26E0-40F0-A187-62739B4F9FFE}">
+  <dimension ref="A1:I35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <cols>
+    <col min="1" max="1" width="2.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="10">
+        <v>2</v>
+      </c>
+      <c r="C1" s="7">
+        <v>7</v>
+      </c>
+      <c r="D1" s="8" t="str">
+        <f t="shared" ref="D1:D7" si="0">_xlfn.CONCAT("2001:",B1,":",C1,"::")</f>
+        <v>2001:2:7::</v>
+      </c>
+      <c r="E1" s="8">
+        <f ca="1">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>2</v>
+      </c>
+      <c r="F1" s="8" t="str">
+        <f ca="1">_xlfn.CONCAT(_xlfn.SWITCH(E1,1,"A",2,"B",3,"C"), IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1))</f>
+        <v>B1</v>
+      </c>
+      <c r="G1" s="8">
+        <f>IF(MATCH("*",$A$1:$A$34) &lt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H1" s="8" t="str">
+        <f t="shared" ref="H1:H7" ca="1" si="1">_xlfn.CONCAT("2001:",F1,":1::",G1)</f>
+        <v>2001:B1:1::1</v>
+      </c>
+      <c r="I1" t="str">
+        <f ca="1">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ipv6 route", " ", D1, "/112"," ", H1))</f>
+        <v>ipv6 route 2001:2:7::/112 2001:B1:1::1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="10">
+        <v>2</v>
+      </c>
+      <c r="C2" s="7">
+        <f t="shared" ref="C2:C7" si="2">C1-1</f>
+        <v>6</v>
+      </c>
+      <c r="D2" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>2001:2:6::</v>
+      </c>
+      <c r="E2" s="8">
+        <f t="shared" ref="E2:E34" ca="1" si="3">INDIRECT(_xlfn.CONCAT("B",MATCH("*",$A$1:$A$34)))</f>
+        <v>2</v>
+      </c>
+      <c r="F2" s="8" t="str">
+        <f t="shared" ref="F2:F34" ca="1" si="4">_xlfn.CONCAT(_xlfn.SWITCH(E2,1,"A",2,"B",3,"C"), IF(MATCH("*",$A$1:$A$34) &gt; ROW(), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))), INDIRECT(_xlfn.CONCAT("C",MATCH("*",$A$1:$A$34))) - 1))</f>
+        <v>B1</v>
+      </c>
+      <c r="G2" s="8">
+        <f t="shared" ref="G2:G34" si="5">IF(MATCH("*",$A$1:$A$34) &lt; ROW(), 2, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H2" s="8" t="str">
+        <f t="shared" ref="H2:H34" ca="1" si="6">_xlfn.CONCAT("2001:",F2,":1::",G2)</f>
+        <v>2001:B1:1::1</v>
+      </c>
+      <c r="I2" t="str">
+        <f t="shared" ref="I2:I34" ca="1" si="7">IF(MATCH("*",$A$1:$A$34) = ROW(),"#",_xlfn.CONCAT("ipv6 route", " ", D2, "/112"," ", H2))</f>
+        <v>ipv6 route 2001:2:6::/112 2001:B1:1::1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="10">
+        <v>2</v>
+      </c>
+      <c r="C3" s="7">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="D3" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>2001:2:5::</v>
+      </c>
+      <c r="E3" s="8">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F3" s="8" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>B1</v>
+      </c>
+      <c r="G3" s="8">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="H3" s="8" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>2001:B1:1::1</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v>ipv6 route 2001:2:5::/112 2001:B1:1::1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="10">
+        <v>2</v>
+      </c>
+      <c r="C4" s="7">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="D4" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>2001:2:4::</v>
+      </c>
+      <c r="E4" s="8">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F4" s="8" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>B1</v>
+      </c>
+      <c r="G4" s="8">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="H4" s="8" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>2001:B1:1::1</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v>ipv6 route 2001:2:4::/112 2001:B1:1::1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="10">
+        <v>2</v>
+      </c>
+      <c r="C5" s="7">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="D5" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>2001:2:3::</v>
+      </c>
+      <c r="E5" s="8">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F5" s="8" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>B1</v>
+      </c>
+      <c r="G5" s="8">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="H5" s="8" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>2001:B1:1::1</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v>ipv6 route 2001:2:3::/112 2001:B1:1::1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="10">
+        <v>2</v>
+      </c>
+      <c r="C6" s="7">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="D6" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>2001:2:2::</v>
+      </c>
+      <c r="E6" s="8">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F6" s="8" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>B1</v>
+      </c>
+      <c r="G6" s="8">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="H6" s="8" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>2001:B1:1::1</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v>ipv6 route 2001:2:2::/112 2001:B1:1::1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="10">
+        <v>2</v>
+      </c>
+      <c r="C7" s="7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D7" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>2001:2:1::</v>
+      </c>
+      <c r="E7" s="8">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F7" s="8" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>B0</v>
+      </c>
+      <c r="G7" s="8">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="H7" s="8" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>2001:B0:1::1</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="7"/>
+        <v>#</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="B8" s="9">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7">
+        <v>6</v>
+      </c>
+      <c r="D8" s="8" t="str">
+        <f>_xlfn.CONCAT("2001:",B8,":",C8,"::")</f>
+        <v>2001:1:6::</v>
+      </c>
+      <c r="E8" s="8">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F8" s="8" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>B0</v>
+      </c>
+      <c r="G8" s="8">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="7"/>
+        <v>ipv6 route 2001:1:6::/112 2001:F1:1::1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="B9" s="9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="7">
+        <f>C8-1</f>
+        <v>5</v>
+      </c>
+      <c r="D9" s="8" t="str">
+        <f t="shared" ref="D9:D34" si="8">_xlfn.CONCAT("2001:",B9,":",C9,"::")</f>
+        <v>2001:1:5::</v>
+      </c>
+      <c r="E9" s="8">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F9" s="8" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>B0</v>
+      </c>
+      <c r="G9" s="8">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="7"/>
+        <v>ipv6 route 2001:1:5::/112 2001:F1:1::1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="B10" s="9">
+        <v>1</v>
+      </c>
+      <c r="C10" s="7">
+        <f t="shared" ref="C10:C13" si="9">C9-1</f>
+        <v>4</v>
+      </c>
+      <c r="D10" s="8" t="str">
+        <f t="shared" si="8"/>
+        <v>2001:1:4::</v>
+      </c>
+      <c r="E10" s="8">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F10" s="8" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>B0</v>
+      </c>
+      <c r="G10" s="8">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="7"/>
+        <v>ipv6 route 2001:1:4::/112 2001:F1:1::1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="B11" s="9">
+        <v>1</v>
+      </c>
+      <c r="C11" s="7">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="D11" s="8" t="str">
+        <f t="shared" si="8"/>
+        <v>2001:1:3::</v>
+      </c>
+      <c r="E11" s="8">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F11" s="8" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>B0</v>
+      </c>
+      <c r="G11" s="8">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="7"/>
+        <v>ipv6 route 2001:1:3::/112 2001:F1:1::1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="B12" s="9">
+        <v>1</v>
+      </c>
+      <c r="C12" s="7">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="D12" s="8" t="str">
+        <f t="shared" si="8"/>
+        <v>2001:1:2::</v>
+      </c>
+      <c r="E12" s="8">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F12" s="8" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>B0</v>
+      </c>
+      <c r="G12" s="8">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="7"/>
+        <v>ipv6 route 2001:1:2::/112 2001:F1:1::1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="B13" s="9">
+        <v>1</v>
+      </c>
+      <c r="C13" s="7">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="D13" s="8" t="str">
+        <f t="shared" si="8"/>
+        <v>2001:1:1::</v>
+      </c>
+      <c r="E13" s="8">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F13" s="8" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>B0</v>
+      </c>
+      <c r="G13" s="8">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="7"/>
+        <v>ipv6 route 2001:1:1::/112 2001:F1:1::1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="B14" s="11">
+        <v>3</v>
+      </c>
+      <c r="C14" s="7">
+        <v>21</v>
+      </c>
+      <c r="D14" s="8" t="str">
+        <f t="shared" si="8"/>
+        <v>2001:3:21::</v>
+      </c>
+      <c r="E14" s="8">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F14" s="8" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>B0</v>
+      </c>
+      <c r="G14" s="8">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="7"/>
+        <v>ipv6 route 2001:3:21::/112 2001:F2:1::2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="B15" s="11">
+        <v>3</v>
+      </c>
+      <c r="C15" s="7">
+        <f>C14-1</f>
+        <v>20</v>
+      </c>
+      <c r="D15" s="8" t="str">
+        <f t="shared" si="8"/>
+        <v>2001:3:20::</v>
+      </c>
+      <c r="E15" s="8">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F15" s="8" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>B0</v>
+      </c>
+      <c r="G15" s="8">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="7"/>
+        <v>ipv6 route 2001:3:20::/112 2001:F2:1::2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="B16" s="11">
+        <v>3</v>
+      </c>
+      <c r="C16" s="7">
+        <f t="shared" ref="C16:C34" si="10">C15-1</f>
+        <v>19</v>
+      </c>
+      <c r="D16" s="8" t="str">
+        <f t="shared" si="8"/>
+        <v>2001:3:19::</v>
+      </c>
+      <c r="E16" s="8">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F16" s="8" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>B0</v>
+      </c>
+      <c r="G16" s="8">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="7"/>
+        <v>ipv6 route 2001:3:19::/112 2001:F2:1::2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9">
+      <c r="B17" s="11">
+        <v>3</v>
+      </c>
+      <c r="C17" s="7">
+        <f t="shared" si="10"/>
+        <v>18</v>
+      </c>
+      <c r="D17" s="8" t="str">
+        <f t="shared" si="8"/>
+        <v>2001:3:18::</v>
+      </c>
+      <c r="E17" s="8">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F17" s="8" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>B0</v>
+      </c>
+      <c r="G17" s="8">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="7"/>
+        <v>ipv6 route 2001:3:18::/112 2001:F2:1::2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9">
+      <c r="B18" s="11">
+        <v>3</v>
+      </c>
+      <c r="C18" s="7">
+        <f t="shared" si="10"/>
+        <v>17</v>
+      </c>
+      <c r="D18" s="8" t="str">
+        <f t="shared" si="8"/>
+        <v>2001:3:17::</v>
+      </c>
+      <c r="E18" s="8">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F18" s="8" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>B0</v>
+      </c>
+      <c r="G18" s="8">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="7"/>
+        <v>ipv6 route 2001:3:17::/112 2001:F2:1::2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9">
+      <c r="B19" s="11">
+        <v>3</v>
+      </c>
+      <c r="C19" s="7">
+        <f t="shared" si="10"/>
+        <v>16</v>
+      </c>
+      <c r="D19" s="8" t="str">
+        <f t="shared" si="8"/>
+        <v>2001:3:16::</v>
+      </c>
+      <c r="E19" s="8">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F19" s="8" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>B0</v>
+      </c>
+      <c r="G19" s="8">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="7"/>
+        <v>ipv6 route 2001:3:16::/112 2001:F2:1::2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9">
+      <c r="B20" s="11">
+        <v>3</v>
+      </c>
+      <c r="C20" s="7">
+        <f t="shared" si="10"/>
+        <v>15</v>
+      </c>
+      <c r="D20" s="8" t="str">
+        <f t="shared" si="8"/>
+        <v>2001:3:15::</v>
+      </c>
+      <c r="E20" s="8">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F20" s="8" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>B0</v>
+      </c>
+      <c r="G20" s="8">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="7"/>
+        <v>ipv6 route 2001:3:15::/112 2001:F2:1::2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9">
+      <c r="B21" s="11">
+        <v>3</v>
+      </c>
+      <c r="C21" s="7">
+        <f t="shared" si="10"/>
+        <v>14</v>
+      </c>
+      <c r="D21" s="8" t="str">
+        <f t="shared" si="8"/>
+        <v>2001:3:14::</v>
+      </c>
+      <c r="E21" s="8">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F21" s="8" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>B0</v>
+      </c>
+      <c r="G21" s="8">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="7"/>
+        <v>ipv6 route 2001:3:14::/112 2001:F2:1::2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9">
+      <c r="B22" s="11">
+        <v>3</v>
+      </c>
+      <c r="C22" s="7">
+        <f t="shared" si="10"/>
+        <v>13</v>
+      </c>
+      <c r="D22" s="8" t="str">
+        <f t="shared" si="8"/>
+        <v>2001:3:13::</v>
+      </c>
+      <c r="E22" s="8">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F22" s="8" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>B0</v>
+      </c>
+      <c r="G22" s="8">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="7"/>
+        <v>ipv6 route 2001:3:13::/112 2001:F2:1::2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9">
+      <c r="B23" s="11">
+        <v>3</v>
+      </c>
+      <c r="C23" s="7">
+        <f t="shared" si="10"/>
+        <v>12</v>
+      </c>
+      <c r="D23" s="8" t="str">
+        <f t="shared" si="8"/>
+        <v>2001:3:12::</v>
+      </c>
+      <c r="E23" s="8">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F23" s="8" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>B0</v>
+      </c>
+      <c r="G23" s="8">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" si="7"/>
+        <v>ipv6 route 2001:3:12::/112 2001:F2:1::2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9">
+      <c r="B24" s="11">
+        <v>3</v>
+      </c>
+      <c r="C24" s="7">
+        <f t="shared" si="10"/>
+        <v>11</v>
+      </c>
+      <c r="D24" s="8" t="str">
+        <f t="shared" si="8"/>
+        <v>2001:3:11::</v>
+      </c>
+      <c r="E24" s="8">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F24" s="8" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>B0</v>
+      </c>
+      <c r="G24" s="8">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I24" t="str">
+        <f t="shared" si="7"/>
+        <v>ipv6 route 2001:3:11::/112 2001:F2:1::2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9">
+      <c r="B25" s="11">
+        <v>3</v>
+      </c>
+      <c r="C25" s="7">
+        <f>C24-1</f>
+        <v>10</v>
+      </c>
+      <c r="D25" s="8" t="str">
+        <f t="shared" si="8"/>
+        <v>2001:3:10::</v>
+      </c>
+      <c r="E25" s="8">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F25" s="8" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>B0</v>
+      </c>
+      <c r="G25" s="8">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" si="7"/>
+        <v>ipv6 route 2001:3:10::/112 2001:F2:1::2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9">
+      <c r="B26" s="11">
+        <v>3</v>
+      </c>
+      <c r="C26" s="7">
+        <f t="shared" si="10"/>
+        <v>9</v>
+      </c>
+      <c r="D26" s="8" t="str">
+        <f t="shared" si="8"/>
+        <v>2001:3:9::</v>
+      </c>
+      <c r="E26" s="8">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F26" s="8" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>B0</v>
+      </c>
+      <c r="G26" s="8">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I26" t="str">
+        <f t="shared" si="7"/>
+        <v>ipv6 route 2001:3:9::/112 2001:F2:1::2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9">
+      <c r="B27" s="11">
+        <v>3</v>
+      </c>
+      <c r="C27" s="7">
+        <f t="shared" si="10"/>
+        <v>8</v>
+      </c>
+      <c r="D27" s="8" t="str">
+        <f t="shared" si="8"/>
+        <v>2001:3:8::</v>
+      </c>
+      <c r="E27" s="8">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F27" s="8" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>B0</v>
+      </c>
+      <c r="G27" s="8">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="H27" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I27" t="str">
+        <f t="shared" si="7"/>
+        <v>ipv6 route 2001:3:8::/112 2001:F2:1::2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9">
+      <c r="B28" s="11">
+        <v>3</v>
+      </c>
+      <c r="C28" s="7">
+        <f t="shared" si="10"/>
+        <v>7</v>
+      </c>
+      <c r="D28" s="8" t="str">
+        <f t="shared" si="8"/>
+        <v>2001:3:7::</v>
+      </c>
+      <c r="E28" s="8">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F28" s="8" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>B0</v>
+      </c>
+      <c r="G28" s="8">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I28" t="str">
+        <f t="shared" si="7"/>
+        <v>ipv6 route 2001:3:7::/112 2001:F2:1::2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9">
+      <c r="B29" s="11">
+        <v>3</v>
+      </c>
+      <c r="C29" s="7">
+        <f t="shared" si="10"/>
+        <v>6</v>
+      </c>
+      <c r="D29" s="8" t="str">
+        <f t="shared" si="8"/>
+        <v>2001:3:6::</v>
+      </c>
+      <c r="E29" s="8">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F29" s="8" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>B0</v>
+      </c>
+      <c r="G29" s="8">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I29" t="str">
+        <f t="shared" si="7"/>
+        <v>ipv6 route 2001:3:6::/112 2001:F2:1::2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9">
+      <c r="B30" s="11">
+        <v>3</v>
+      </c>
+      <c r="C30" s="7">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="D30" s="8" t="str">
+        <f t="shared" si="8"/>
+        <v>2001:3:5::</v>
+      </c>
+      <c r="E30" s="8">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F30" s="8" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>B0</v>
+      </c>
+      <c r="G30" s="8">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I30" t="str">
+        <f t="shared" si="7"/>
+        <v>ipv6 route 2001:3:5::/112 2001:F2:1::2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9">
+      <c r="B31" s="11">
+        <v>3</v>
+      </c>
+      <c r="C31" s="7">
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="D31" s="8" t="str">
+        <f t="shared" si="8"/>
+        <v>2001:3:4::</v>
+      </c>
+      <c r="E31" s="8">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F31" s="8" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>B0</v>
+      </c>
+      <c r="G31" s="8">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="H31" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I31" t="str">
+        <f t="shared" si="7"/>
+        <v>ipv6 route 2001:3:4::/112 2001:F2:1::2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9">
+      <c r="B32" s="11">
+        <v>3</v>
+      </c>
+      <c r="C32" s="7">
+        <f t="shared" si="10"/>
+        <v>3</v>
+      </c>
+      <c r="D32" s="8" t="str">
+        <f t="shared" si="8"/>
+        <v>2001:3:3::</v>
+      </c>
+      <c r="E32" s="8">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F32" s="8" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>B0</v>
+      </c>
+      <c r="G32" s="8">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="H32" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I32" t="str">
+        <f t="shared" si="7"/>
+        <v>ipv6 route 2001:3:3::/112 2001:F2:1::2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9">
+      <c r="B33" s="11">
+        <v>3</v>
+      </c>
+      <c r="C33" s="7">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="D33" s="8" t="str">
+        <f t="shared" si="8"/>
+        <v>2001:3:2::</v>
+      </c>
+      <c r="E33" s="8">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F33" s="8" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>B0</v>
+      </c>
+      <c r="G33" s="8">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="H33" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I33" t="str">
+        <f t="shared" si="7"/>
+        <v>ipv6 route 2001:3:2::/112 2001:F2:1::2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9">
+      <c r="B34" s="11">
+        <v>3</v>
+      </c>
+      <c r="C34" s="7">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="D34" s="8" t="str">
+        <f t="shared" si="8"/>
+        <v>2001:3:1::</v>
+      </c>
+      <c r="E34" s="8">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F34" s="8" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>B0</v>
+      </c>
+      <c r="G34" s="8">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I34" t="str">
+        <f t="shared" si="7"/>
+        <v>ipv6 route 2001:3:1::/112 2001:F2:1::2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9">
+      <c r="I35" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>